<commit_message>
:congratulations: Complete the tasks of plot batch.
1. Further bug fixes in sngstats. Add help lines and RT removal of less
than 300ms for subject level analysis.
2. Take into consideration of multiple conditions when plotting figures
for each task.
3. Binary file changes are missed. :sob:
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="549">
   <si>
     <t>符号判断</t>
   </si>
@@ -1197,879 +1197,883 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>STIM</t>
+  </si>
+  <si>
+    <t>⊙</t>
+  </si>
+  <si>
+    <t>〒</t>
+  </si>
+  <si>
+    <t>♀</t>
+  </si>
+  <si>
+    <t>※</t>
+  </si>
+  <si>
+    <t>¤</t>
+  </si>
+  <si>
+    <t>§</t>
+  </si>
+  <si>
+    <t>SCat</t>
+  </si>
+  <si>
+    <t>各</t>
+  </si>
+  <si>
+    <t>力</t>
+  </si>
+  <si>
+    <t>四</t>
+  </si>
+  <si>
+    <t>爱</t>
+  </si>
+  <si>
+    <t>众</t>
+  </si>
+  <si>
+    <t>次</t>
+  </si>
+  <si>
+    <t>泪</t>
+  </si>
+  <si>
+    <t>办</t>
+  </si>
+  <si>
+    <t>块</t>
+  </si>
+  <si>
+    <t>互</t>
+  </si>
+  <si>
+    <t>过</t>
+  </si>
+  <si>
+    <t>代</t>
+  </si>
+  <si>
+    <t>去</t>
+  </si>
+  <si>
+    <t>认</t>
+  </si>
+  <si>
+    <t>弄</t>
+  </si>
+  <si>
+    <t>入</t>
+  </si>
+  <si>
+    <t>动</t>
+  </si>
+  <si>
+    <t>燕</t>
+  </si>
+  <si>
+    <t>妙</t>
+  </si>
+  <si>
+    <t>校</t>
+  </si>
+  <si>
+    <t>立</t>
+  </si>
+  <si>
+    <t>变</t>
+  </si>
+  <si>
+    <t>放</t>
+  </si>
+  <si>
+    <t>再</t>
+  </si>
+  <si>
+    <t>到</t>
+  </si>
+  <si>
+    <t>多</t>
+  </si>
+  <si>
+    <t>家</t>
+  </si>
+  <si>
+    <t>巴</t>
+  </si>
+  <si>
+    <t>他</t>
+  </si>
+  <si>
+    <t>光</t>
+  </si>
+  <si>
+    <t>春</t>
+  </si>
+  <si>
+    <t>吃</t>
+  </si>
+  <si>
+    <t>语</t>
+  </si>
+  <si>
+    <t>灰</t>
+  </si>
+  <si>
+    <t>反</t>
+  </si>
+  <si>
+    <t>迷</t>
+  </si>
+  <si>
+    <t>活</t>
+  </si>
+  <si>
+    <t>习</t>
+  </si>
+  <si>
+    <t>牙</t>
+  </si>
+  <si>
+    <t>洋</t>
+  </si>
+  <si>
+    <t>打</t>
+  </si>
+  <si>
+    <t>平</t>
+  </si>
+  <si>
+    <t>门</t>
+  </si>
+  <si>
+    <t>节</t>
+  </si>
+  <si>
+    <t>祖</t>
+  </si>
+  <si>
+    <t>杆</t>
+  </si>
+  <si>
+    <t>早</t>
+  </si>
+  <si>
+    <t>总</t>
+  </si>
+  <si>
+    <t>品</t>
+  </si>
+  <si>
+    <t>百</t>
+  </si>
+  <si>
+    <t>āuh</t>
+  </si>
+  <si>
+    <t>méin</t>
+  </si>
+  <si>
+    <t>bàg</t>
+  </si>
+  <si>
+    <t>lù</t>
+  </si>
+  <si>
+    <t>rànɡ</t>
+  </si>
+  <si>
+    <t>dluī</t>
+  </si>
+  <si>
+    <t>xìnɡ</t>
+  </si>
+  <si>
+    <t>cónɡ</t>
+  </si>
+  <si>
+    <t>huà</t>
+  </si>
+  <si>
+    <t>hsū</t>
+  </si>
+  <si>
+    <t>ɡuānɡ</t>
+  </si>
+  <si>
+    <t>wāin</t>
+  </si>
+  <si>
+    <t>yè</t>
+  </si>
+  <si>
+    <t>bǐg</t>
+  </si>
+  <si>
+    <t>hóu</t>
+  </si>
+  <si>
+    <t>uǎn</t>
+  </si>
+  <si>
+    <t>biǐ</t>
+  </si>
+  <si>
+    <t>zhēn</t>
+  </si>
+  <si>
+    <t>jāin</t>
+  </si>
+  <si>
+    <t>tiān</t>
+  </si>
+  <si>
+    <t>qiū</t>
+  </si>
+  <si>
+    <t>liǎm</t>
+  </si>
+  <si>
+    <t>máio</t>
+  </si>
+  <si>
+    <t>jiān</t>
+  </si>
+  <si>
+    <t>siān</t>
+  </si>
+  <si>
+    <t>māo</t>
+  </si>
+  <si>
+    <t>fiàn</t>
+  </si>
+  <si>
+    <t>niág</t>
+  </si>
+  <si>
+    <t>jīnq</t>
+  </si>
+  <si>
+    <t>wài</t>
+  </si>
+  <si>
+    <t>xǔng</t>
+  </si>
+  <si>
+    <t>tián</t>
+  </si>
+  <si>
+    <t>nàl</t>
+  </si>
+  <si>
+    <t>xiiē</t>
+  </si>
+  <si>
+    <t>wū</t>
+  </si>
+  <si>
+    <t>shēnɡ</t>
+  </si>
+  <si>
+    <t>pāi</t>
+  </si>
+  <si>
+    <t>boì</t>
+  </si>
+  <si>
+    <t>dòu</t>
+  </si>
+  <si>
+    <t>dòn</t>
+  </si>
+  <si>
+    <t>poǎ</t>
+  </si>
+  <si>
+    <t>iàn</t>
+  </si>
+  <si>
+    <t>chī</t>
+  </si>
+  <si>
+    <t>biān</t>
+  </si>
+  <si>
+    <t>lám</t>
+  </si>
+  <si>
+    <t>zhèɡ</t>
+  </si>
+  <si>
+    <t>yǔ</t>
+  </si>
+  <si>
+    <t>xuě</t>
+  </si>
+  <si>
+    <t>shǎo</t>
+  </si>
+  <si>
+    <t>草地</t>
+  </si>
+  <si>
+    <t>跳高</t>
+  </si>
+  <si>
+    <t>菜园</t>
+  </si>
+  <si>
+    <t>这些</t>
+  </si>
+  <si>
+    <t>走过</t>
+  </si>
+  <si>
+    <t>跑步</t>
+  </si>
+  <si>
+    <t>出来</t>
+  </si>
+  <si>
+    <t>远近</t>
+  </si>
+  <si>
+    <t>晚上</t>
+  </si>
+  <si>
+    <t>绿色</t>
+  </si>
+  <si>
+    <t>电视</t>
+  </si>
+  <si>
+    <t>作业</t>
+  </si>
+  <si>
+    <t>田野</t>
+  </si>
+  <si>
+    <t>读书</t>
+  </si>
+  <si>
+    <t>身体</t>
+  </si>
+  <si>
+    <t>漂亮</t>
+  </si>
+  <si>
+    <t>同学</t>
+  </si>
+  <si>
+    <t>长城</t>
+  </si>
+  <si>
+    <t>豆角</t>
+  </si>
+  <si>
+    <t>外面</t>
+  </si>
+  <si>
+    <t>回答</t>
+  </si>
+  <si>
+    <t>现在</t>
+  </si>
+  <si>
+    <t>景色</t>
+  </si>
+  <si>
+    <t>妈妈</t>
+  </si>
+  <si>
+    <t>竹子</t>
+  </si>
+  <si>
+    <t>何花</t>
+  </si>
+  <si>
+    <t>里想</t>
+  </si>
+  <si>
+    <t>平论</t>
+  </si>
+  <si>
+    <t>马蚁</t>
+  </si>
+  <si>
+    <t>心闻</t>
+  </si>
+  <si>
+    <t>站士</t>
+  </si>
+  <si>
+    <t>拉圾</t>
+  </si>
+  <si>
+    <t>石快</t>
+  </si>
+  <si>
+    <t>亭止</t>
+  </si>
+  <si>
+    <t>纺问</t>
+  </si>
+  <si>
+    <t>安净</t>
+  </si>
+  <si>
+    <t>诚功</t>
+  </si>
+  <si>
+    <t>风争</t>
+  </si>
+  <si>
+    <t>蓝子</t>
+  </si>
+  <si>
+    <t>交傲</t>
+  </si>
+  <si>
+    <t>树跟</t>
+  </si>
+  <si>
+    <t>罗卜</t>
+  </si>
+  <si>
+    <t>足求</t>
+  </si>
+  <si>
+    <t>事晴</t>
+  </si>
+  <si>
+    <t>西呱</t>
+  </si>
+  <si>
+    <t>你门</t>
+  </si>
+  <si>
+    <t>可昔</t>
+  </si>
+  <si>
+    <t>海阳</t>
+  </si>
+  <si>
+    <t>旦是</t>
+  </si>
+  <si>
+    <t>店脑</t>
+  </si>
+  <si>
+    <t>公鸡</t>
+  </si>
+  <si>
+    <t>燕子</t>
+  </si>
+  <si>
+    <t>青蛙</t>
+  </si>
+  <si>
+    <t>水牛</t>
+  </si>
+  <si>
+    <t>老鼠</t>
+  </si>
+  <si>
+    <t>山羊</t>
+  </si>
+  <si>
+    <t>黑狗</t>
+  </si>
+  <si>
+    <t>熊猫</t>
+  </si>
+  <si>
+    <t>黄牛</t>
+  </si>
+  <si>
+    <t>松鼠</t>
+  </si>
+  <si>
+    <t>野鸭</t>
+  </si>
+  <si>
+    <t>老虎</t>
+  </si>
+  <si>
+    <t>兔子</t>
+  </si>
+  <si>
+    <t>大象</t>
+  </si>
+  <si>
+    <t>猴子</t>
+  </si>
+  <si>
+    <t>狮子</t>
+  </si>
+  <si>
+    <t>乌龟</t>
+  </si>
+  <si>
+    <t>乌鸦</t>
+  </si>
+  <si>
+    <t>蝌蚪</t>
+  </si>
+  <si>
+    <t>黑熊</t>
+  </si>
+  <si>
+    <t>孔雀</t>
+  </si>
+  <si>
+    <t>大雁</t>
+  </si>
+  <si>
+    <t>海鸥</t>
+  </si>
+  <si>
+    <t>蜘蛛</t>
+  </si>
+  <si>
+    <t>壁虎</t>
+  </si>
+  <si>
+    <t>房屋</t>
+  </si>
+  <si>
+    <t>花朵</t>
+  </si>
+  <si>
+    <t>白云</t>
+  </si>
+  <si>
+    <t>马车</t>
+  </si>
+  <si>
+    <t>飞机</t>
+  </si>
+  <si>
+    <t>高山</t>
+  </si>
+  <si>
+    <t>故乡</t>
+  </si>
+  <si>
+    <t>茶几</t>
+  </si>
+  <si>
+    <t>明月</t>
+  </si>
+  <si>
+    <t>尘土</t>
+  </si>
+  <si>
+    <t>竹排</t>
+  </si>
+  <si>
+    <t>鸟岛</t>
+  </si>
+  <si>
+    <t>皮球</t>
+  </si>
+  <si>
+    <t>商场</t>
+  </si>
+  <si>
+    <t>土地</t>
+  </si>
+  <si>
+    <t>早晨</t>
+  </si>
+  <si>
+    <t>胡子</t>
+  </si>
+  <si>
+    <t>木鱼</t>
+  </si>
+  <si>
+    <t>毛巾</t>
+  </si>
+  <si>
+    <t>贺卡</t>
+  </si>
+  <si>
+    <t>雨伞</t>
+  </si>
+  <si>
+    <t>沙发</t>
+  </si>
+  <si>
+    <t>尾巴</t>
+  </si>
+  <si>
+    <t>雪人</t>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>NSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotalTime NTotalTrl NAccTrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotalTime NTotalTrl NAccTrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpecialVars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语义判断(高级)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>捉虫(高级版)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Congruent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Incongruent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Repeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall Congruent Incongruent CongEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STIM RT ACC Resp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condition SCat ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>Count RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit FA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_hit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MergeCond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>VarsCond</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>STIM</t>
-  </si>
-  <si>
-    <t>⊙</t>
-  </si>
-  <si>
-    <t>〒</t>
-  </si>
-  <si>
-    <t>♀</t>
-  </si>
-  <si>
-    <t>※</t>
-  </si>
-  <si>
-    <t>¤</t>
-  </si>
-  <si>
-    <t>§</t>
-  </si>
-  <si>
-    <t>SCat</t>
-  </si>
-  <si>
-    <t>各</t>
-  </si>
-  <si>
-    <t>力</t>
-  </si>
-  <si>
-    <t>四</t>
-  </si>
-  <si>
-    <t>爱</t>
-  </si>
-  <si>
-    <t>众</t>
-  </si>
-  <si>
-    <t>次</t>
-  </si>
-  <si>
-    <t>泪</t>
-  </si>
-  <si>
-    <t>办</t>
-  </si>
-  <si>
-    <t>块</t>
-  </si>
-  <si>
-    <t>互</t>
-  </si>
-  <si>
-    <t>过</t>
-  </si>
-  <si>
-    <t>代</t>
-  </si>
-  <si>
-    <t>去</t>
-  </si>
-  <si>
-    <t>认</t>
-  </si>
-  <si>
-    <t>弄</t>
-  </si>
-  <si>
-    <t>入</t>
-  </si>
-  <si>
-    <t>动</t>
-  </si>
-  <si>
-    <t>燕</t>
-  </si>
-  <si>
-    <t>妙</t>
-  </si>
-  <si>
-    <t>校</t>
-  </si>
-  <si>
-    <t>立</t>
-  </si>
-  <si>
-    <t>变</t>
-  </si>
-  <si>
-    <t>放</t>
-  </si>
-  <si>
-    <t>再</t>
-  </si>
-  <si>
-    <t>到</t>
-  </si>
-  <si>
-    <t>多</t>
-  </si>
-  <si>
-    <t>家</t>
-  </si>
-  <si>
-    <t>巴</t>
-  </si>
-  <si>
-    <t>他</t>
-  </si>
-  <si>
-    <t>光</t>
-  </si>
-  <si>
-    <t>春</t>
-  </si>
-  <si>
-    <t>吃</t>
-  </si>
-  <si>
-    <t>语</t>
-  </si>
-  <si>
-    <t>灰</t>
-  </si>
-  <si>
-    <t>反</t>
-  </si>
-  <si>
-    <t>迷</t>
-  </si>
-  <si>
-    <t>活</t>
-  </si>
-  <si>
-    <t>习</t>
-  </si>
-  <si>
-    <t>牙</t>
-  </si>
-  <si>
-    <t>洋</t>
-  </si>
-  <si>
-    <t>打</t>
-  </si>
-  <si>
-    <t>平</t>
-  </si>
-  <si>
-    <t>门</t>
-  </si>
-  <si>
-    <t>节</t>
-  </si>
-  <si>
-    <t>祖</t>
-  </si>
-  <si>
-    <t>杆</t>
-  </si>
-  <si>
-    <t>早</t>
-  </si>
-  <si>
-    <t>总</t>
-  </si>
-  <si>
-    <t>品</t>
-  </si>
-  <si>
-    <t>百</t>
-  </si>
-  <si>
-    <t>āuh</t>
-  </si>
-  <si>
-    <t>méin</t>
-  </si>
-  <si>
-    <t>bàg</t>
-  </si>
-  <si>
-    <t>lù</t>
-  </si>
-  <si>
-    <t>rànɡ</t>
-  </si>
-  <si>
-    <t>dluī</t>
-  </si>
-  <si>
-    <t>xìnɡ</t>
-  </si>
-  <si>
-    <t>cónɡ</t>
-  </si>
-  <si>
-    <t>huà</t>
-  </si>
-  <si>
-    <t>hsū</t>
-  </si>
-  <si>
-    <t>ɡuānɡ</t>
-  </si>
-  <si>
-    <t>wāin</t>
-  </si>
-  <si>
-    <t>yè</t>
-  </si>
-  <si>
-    <t>bǐg</t>
-  </si>
-  <si>
-    <t>hóu</t>
-  </si>
-  <si>
-    <t>uǎn</t>
-  </si>
-  <si>
-    <t>biǐ</t>
-  </si>
-  <si>
-    <t>zhēn</t>
-  </si>
-  <si>
-    <t>jāin</t>
-  </si>
-  <si>
-    <t>tiān</t>
-  </si>
-  <si>
-    <t>qiū</t>
-  </si>
-  <si>
-    <t>liǎm</t>
-  </si>
-  <si>
-    <t>máio</t>
-  </si>
-  <si>
-    <t>jiān</t>
-  </si>
-  <si>
-    <t>siān</t>
-  </si>
-  <si>
-    <t>māo</t>
-  </si>
-  <si>
-    <t>fiàn</t>
-  </si>
-  <si>
-    <t>niág</t>
-  </si>
-  <si>
-    <t>jīnq</t>
-  </si>
-  <si>
-    <t>wài</t>
-  </si>
-  <si>
-    <t>xǔng</t>
-  </si>
-  <si>
-    <t>tián</t>
-  </si>
-  <si>
-    <t>nàl</t>
-  </si>
-  <si>
-    <t>xiiē</t>
-  </si>
-  <si>
-    <t>wū</t>
-  </si>
-  <si>
-    <t>shēnɡ</t>
-  </si>
-  <si>
-    <t>pāi</t>
-  </si>
-  <si>
-    <t>boì</t>
-  </si>
-  <si>
-    <t>dòu</t>
-  </si>
-  <si>
-    <t>dòn</t>
-  </si>
-  <si>
-    <t>poǎ</t>
-  </si>
-  <si>
-    <t>iàn</t>
-  </si>
-  <si>
-    <t>chī</t>
-  </si>
-  <si>
-    <t>biān</t>
-  </si>
-  <si>
-    <t>lám</t>
-  </si>
-  <si>
-    <t>zhèɡ</t>
-  </si>
-  <si>
-    <t>yǔ</t>
-  </si>
-  <si>
-    <t>xuě</t>
-  </si>
-  <si>
-    <t>shǎo</t>
-  </si>
-  <si>
-    <t>草地</t>
-  </si>
-  <si>
-    <t>跳高</t>
-  </si>
-  <si>
-    <t>菜园</t>
-  </si>
-  <si>
-    <t>这些</t>
-  </si>
-  <si>
-    <t>走过</t>
-  </si>
-  <si>
-    <t>跑步</t>
-  </si>
-  <si>
-    <t>出来</t>
-  </si>
-  <si>
-    <t>远近</t>
-  </si>
-  <si>
-    <t>晚上</t>
-  </si>
-  <si>
-    <t>绿色</t>
-  </si>
-  <si>
-    <t>电视</t>
-  </si>
-  <si>
-    <t>作业</t>
-  </si>
-  <si>
-    <t>田野</t>
-  </si>
-  <si>
-    <t>读书</t>
-  </si>
-  <si>
-    <t>身体</t>
-  </si>
-  <si>
-    <t>漂亮</t>
-  </si>
-  <si>
-    <t>同学</t>
-  </si>
-  <si>
-    <t>长城</t>
-  </si>
-  <si>
-    <t>豆角</t>
-  </si>
-  <si>
-    <t>外面</t>
-  </si>
-  <si>
-    <t>回答</t>
-  </si>
-  <si>
-    <t>现在</t>
-  </si>
-  <si>
-    <t>景色</t>
-  </si>
-  <si>
-    <t>妈妈</t>
-  </si>
-  <si>
-    <t>竹子</t>
-  </si>
-  <si>
-    <t>何花</t>
-  </si>
-  <si>
-    <t>里想</t>
-  </si>
-  <si>
-    <t>平论</t>
-  </si>
-  <si>
-    <t>马蚁</t>
-  </si>
-  <si>
-    <t>心闻</t>
-  </si>
-  <si>
-    <t>站士</t>
-  </si>
-  <si>
-    <t>拉圾</t>
-  </si>
-  <si>
-    <t>石快</t>
-  </si>
-  <si>
-    <t>亭止</t>
-  </si>
-  <si>
-    <t>纺问</t>
-  </si>
-  <si>
-    <t>安净</t>
-  </si>
-  <si>
-    <t>诚功</t>
-  </si>
-  <si>
-    <t>风争</t>
-  </si>
-  <si>
-    <t>蓝子</t>
-  </si>
-  <si>
-    <t>交傲</t>
-  </si>
-  <si>
-    <t>树跟</t>
-  </si>
-  <si>
-    <t>罗卜</t>
-  </si>
-  <si>
-    <t>足求</t>
-  </si>
-  <si>
-    <t>事晴</t>
-  </si>
-  <si>
-    <t>西呱</t>
-  </si>
-  <si>
-    <t>你门</t>
-  </si>
-  <si>
-    <t>可昔</t>
-  </si>
-  <si>
-    <t>海阳</t>
-  </si>
-  <si>
-    <t>旦是</t>
-  </si>
-  <si>
-    <t>店脑</t>
-  </si>
-  <si>
-    <t>公鸡</t>
-  </si>
-  <si>
-    <t>燕子</t>
-  </si>
-  <si>
-    <t>青蛙</t>
-  </si>
-  <si>
-    <t>水牛</t>
-  </si>
-  <si>
-    <t>老鼠</t>
-  </si>
-  <si>
-    <t>山羊</t>
-  </si>
-  <si>
-    <t>黑狗</t>
-  </si>
-  <si>
-    <t>熊猫</t>
-  </si>
-  <si>
-    <t>黄牛</t>
-  </si>
-  <si>
-    <t>松鼠</t>
-  </si>
-  <si>
-    <t>野鸭</t>
-  </si>
-  <si>
-    <t>老虎</t>
-  </si>
-  <si>
-    <t>兔子</t>
-  </si>
-  <si>
-    <t>大象</t>
-  </si>
-  <si>
-    <t>猴子</t>
-  </si>
-  <si>
-    <t>狮子</t>
-  </si>
-  <si>
-    <t>乌龟</t>
-  </si>
-  <si>
-    <t>乌鸦</t>
-  </si>
-  <si>
-    <t>蝌蚪</t>
-  </si>
-  <si>
-    <t>黑熊</t>
-  </si>
-  <si>
-    <t>孔雀</t>
-  </si>
-  <si>
-    <t>大雁</t>
-  </si>
-  <si>
-    <t>海鸥</t>
-  </si>
-  <si>
-    <t>蜘蛛</t>
-  </si>
-  <si>
-    <t>壁虎</t>
-  </si>
-  <si>
-    <t>房屋</t>
-  </si>
-  <si>
-    <t>花朵</t>
-  </si>
-  <si>
-    <t>白云</t>
-  </si>
-  <si>
-    <t>马车</t>
-  </si>
-  <si>
-    <t>飞机</t>
-  </si>
-  <si>
-    <t>高山</t>
-  </si>
-  <si>
-    <t>故乡</t>
-  </si>
-  <si>
-    <t>茶几</t>
-  </si>
-  <si>
-    <t>明月</t>
-  </si>
-  <si>
-    <t>尘土</t>
-  </si>
-  <si>
-    <t>竹排</t>
-  </si>
-  <si>
-    <t>鸟岛</t>
-  </si>
-  <si>
-    <t>皮球</t>
-  </si>
-  <si>
-    <t>商场</t>
-  </si>
-  <si>
-    <t>土地</t>
-  </si>
-  <si>
-    <t>早晨</t>
-  </si>
-  <si>
-    <t>胡子</t>
-  </si>
-  <si>
-    <t>木鱼</t>
-  </si>
-  <si>
-    <t>毛巾</t>
-  </si>
-  <si>
-    <t>贺卡</t>
-  </si>
-  <si>
-    <t>雨伞</t>
-  </si>
-  <si>
-    <t>沙发</t>
-  </si>
-  <si>
-    <t>尾巴</t>
-  </si>
-  <si>
-    <t>雪人</t>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>NSN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NSN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalTime NTotalTrl NAccTrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalTime NTotalTrl NAccTrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpecialVars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语义判断(高级)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>捉虫(高级版)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NSN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Category</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Congruent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Incongruent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Repeat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Overall Congruent Incongruent CongEffect</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Overall Repeat Switch SwitchCost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NSN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STIM RT ACC Resp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Condition SCat ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>efficiency</t>
-  </si>
-  <si>
-    <t>Count RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit FA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Count_hit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MergeCond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>L R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2485,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2532,7 +2536,7 @@
         <v>264</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>265</v>
+        <v>546</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>186</v>
@@ -2541,10 +2545,10 @@
         <v>212</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
@@ -2580,7 +2584,7 @@
         <v>188</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
@@ -2616,7 +2620,7 @@
         <v>188</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
@@ -2652,7 +2656,7 @@
         <v>188</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
@@ -2688,7 +2692,7 @@
         <v>188</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
@@ -2724,7 +2728,7 @@
         <v>188</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -2733,7 +2737,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -2760,7 +2764,7 @@
         <v>188</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
@@ -2911,7 +2915,7 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -2933,7 +2937,7 @@
         <v>155</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>210</v>
@@ -2967,7 +2971,7 @@
         <v>155</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>210</v>
@@ -3001,7 +3005,7 @@
         <v>155</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>210</v>
@@ -3035,7 +3039,7 @@
         <v>155</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>210</v>
@@ -3426,7 +3430,7 @@
         <v>179</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>116</v>
@@ -3438,16 +3442,16 @@
         <v>239</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="K28" s="2"/>
     </row>
@@ -3469,7 +3473,7 @@
         <v>162</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>210</v>
@@ -3485,7 +3489,7 @@
         <v>188</v>
       </c>
       <c r="M29" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.15">
@@ -3506,7 +3510,7 @@
         <v>162</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>210</v>
@@ -3519,10 +3523,10 @@
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="M30" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.15">
@@ -3761,7 +3765,7 @@
         <v>167</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>210</v>
@@ -3795,7 +3799,7 @@
         <v>167</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>210</v>
@@ -3838,7 +3842,7 @@
         <v>197</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>536</v>
+        <v>547</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -3870,7 +3874,7 @@
         <v>197</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -3902,7 +3906,7 @@
         <v>197</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -3934,7 +3938,7 @@
         <v>197</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -4026,7 +4030,7 @@
         <v>197</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>537</v>
+        <v>548</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -4184,10 +4188,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -4304,10 +4308,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -4387,13 +4391,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -4401,7 +4405,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4412,7 +4416,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -4423,7 +4427,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -4434,7 +4438,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -4462,13 +4466,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -4476,7 +4480,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4487,7 +4491,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -4779,7 +4783,7 @@
         <v>75</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -5027,7 +5031,7 @@
         <v>70</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -5283,15 +5287,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5299,7 +5303,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5307,7 +5311,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5315,7 +5319,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5323,7 +5327,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5331,7 +5335,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5358,15 +5362,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5374,7 +5378,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5382,7 +5386,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5390,7 +5394,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5398,7 +5402,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5406,7 +5410,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5414,7 +5418,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5422,7 +5426,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5430,7 +5434,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5438,7 +5442,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5446,7 +5450,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5454,7 +5458,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5462,7 +5466,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5470,7 +5474,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -5478,7 +5482,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -5486,7 +5490,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -5494,7 +5498,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5502,7 +5506,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -5510,7 +5514,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5518,7 +5522,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -5526,7 +5530,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -5534,7 +5538,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5542,7 +5546,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5550,7 +5554,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -5558,7 +5562,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -5566,7 +5570,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -5574,7 +5578,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -5582,7 +5586,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -5590,7 +5594,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -5598,7 +5602,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -5606,7 +5610,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -5614,7 +5618,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -5622,7 +5626,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -5630,7 +5634,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5638,7 +5642,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5646,7 +5650,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5654,7 +5658,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -5662,7 +5666,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -5670,7 +5674,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -5678,7 +5682,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -5686,7 +5690,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -5694,7 +5698,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -5702,7 +5706,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -5710,7 +5714,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -5718,7 +5722,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -5726,7 +5730,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -5734,7 +5738,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -5742,7 +5746,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -5750,7 +5754,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -5758,7 +5762,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="9" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -5783,15 +5787,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5799,7 +5803,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5807,7 +5811,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5815,7 +5819,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5823,7 +5827,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5831,7 +5835,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5839,7 +5843,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5847,7 +5851,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5855,7 +5859,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5863,7 +5867,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5871,7 +5875,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5879,7 +5883,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5887,7 +5891,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5895,7 +5899,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -5903,7 +5907,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -5911,7 +5915,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -5919,7 +5923,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5927,7 +5931,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -5935,7 +5939,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5943,7 +5947,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -5951,7 +5955,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -5959,7 +5963,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5967,7 +5971,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5975,7 +5979,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -5983,7 +5987,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -5991,7 +5995,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -5999,7 +6003,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -6007,7 +6011,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -6015,7 +6019,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -6023,7 +6027,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -6031,7 +6035,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -6039,7 +6043,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -6047,7 +6051,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -6055,7 +6059,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -6063,7 +6067,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -6071,7 +6075,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -6079,7 +6083,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -6087,7 +6091,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -6095,7 +6099,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -6103,7 +6107,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -6111,7 +6115,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -6119,7 +6123,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -6127,7 +6131,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -6135,7 +6139,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -6143,7 +6147,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -6151,7 +6155,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -6159,7 +6163,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -6167,7 +6171,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -6175,7 +6179,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -6183,7 +6187,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -6209,15 +6213,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6225,7 +6229,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6233,7 +6237,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -6241,7 +6245,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6249,7 +6253,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6257,7 +6261,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -6265,7 +6269,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -6273,7 +6277,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6281,7 +6285,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6289,7 +6293,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6297,7 +6301,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6305,7 +6309,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6313,7 +6317,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6321,7 +6325,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -6329,7 +6333,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -6337,7 +6341,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -6345,7 +6349,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -6353,7 +6357,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -6361,7 +6365,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -6369,7 +6373,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -6377,7 +6381,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -6385,7 +6389,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -6393,7 +6397,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -6401,7 +6405,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -6409,7 +6413,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -6417,7 +6421,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -6425,7 +6429,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -6433,7 +6437,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -6441,7 +6445,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -6449,7 +6453,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -6457,7 +6461,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -6465,7 +6469,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -6473,7 +6477,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -6481,7 +6485,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -6489,7 +6493,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -6497,7 +6501,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -6505,7 +6509,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -6513,7 +6517,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -6521,7 +6525,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -6529,7 +6533,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -6537,7 +6541,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -6545,7 +6549,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -6553,7 +6557,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -6561,7 +6565,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -6569,7 +6573,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -6577,7 +6581,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -6585,7 +6589,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -6593,7 +6597,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -6601,7 +6605,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -6609,7 +6613,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -6636,15 +6640,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6652,7 +6656,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6660,7 +6664,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6668,7 +6672,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6676,7 +6680,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6684,7 +6688,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6692,7 +6696,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -6700,7 +6704,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6708,7 +6712,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6716,7 +6720,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -6724,7 +6728,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6732,7 +6736,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -6740,7 +6744,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6748,7 +6752,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -6756,7 +6760,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -6764,7 +6768,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -6772,7 +6776,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -6780,7 +6784,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -6788,7 +6792,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -6796,7 +6800,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -6804,7 +6808,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -6812,7 +6816,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -6820,7 +6824,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -6828,7 +6832,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -6836,7 +6840,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -6844,7 +6848,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -6852,7 +6856,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -6860,7 +6864,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -6868,7 +6872,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -6876,7 +6880,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -6884,7 +6888,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -6892,7 +6896,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -6900,7 +6904,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -6908,7 +6912,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -6916,7 +6920,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -6924,7 +6928,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -6932,7 +6936,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -6940,7 +6944,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -6948,7 +6952,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -6956,7 +6960,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -6964,7 +6968,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -6972,7 +6976,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -6980,7 +6984,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -6988,7 +6992,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -6996,7 +7000,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -7004,7 +7008,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -7012,7 +7016,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -7020,7 +7024,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -7028,7 +7032,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -7036,7 +7040,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -7063,15 +7067,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7079,7 +7083,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -7087,7 +7091,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -7095,7 +7099,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -7103,7 +7107,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7111,7 +7115,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -7119,7 +7123,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -7127,7 +7131,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -7135,7 +7139,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -7143,7 +7147,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -7151,7 +7155,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -7159,7 +7163,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -7167,7 +7171,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -7175,7 +7179,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -7183,7 +7187,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -7191,7 +7195,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -7199,7 +7203,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -7207,7 +7211,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -7215,7 +7219,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -7223,7 +7227,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -7231,7 +7235,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -7239,7 +7243,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -7247,7 +7251,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -7255,7 +7259,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -7263,7 +7267,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -7271,7 +7275,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -7279,7 +7283,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -7287,7 +7291,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -7295,7 +7299,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -7303,7 +7307,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -7311,7 +7315,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -7319,7 +7323,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -7327,7 +7331,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -7335,7 +7339,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -7343,7 +7347,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -7351,7 +7355,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -7359,7 +7363,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -7367,7 +7371,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -7375,7 +7379,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -7383,7 +7387,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -7391,7 +7395,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -7399,7 +7403,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -7407,7 +7411,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -7415,7 +7419,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -7423,7 +7427,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -7431,7 +7435,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -7439,7 +7443,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -7447,7 +7451,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -7455,7 +7459,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -7463,7 +7467,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B51">
         <v>0</v>

</xml_diff>

<commit_message>
Initiate the slide jobs.
Further jobs needed. Some basic ideas constructed.
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="550">
   <si>
     <t>符号判断</t>
   </si>
@@ -2074,6 +2074,10 @@
   </si>
   <si>
     <t>Overall Repeat Switch SwitchCost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlideSection</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2487,30 +2491,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" customWidth="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
     <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.25" customWidth="1"/>
-    <col min="10" max="10" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.25" customWidth="1"/>
     <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="13.625" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -2550,8 +2555,11 @@
       <c r="M1" s="2" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N1" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <f>ROW() - 1</f>
         <v>1</v>
@@ -2586,10 +2594,13 @@
       <c r="L2" s="2" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <f t="shared" ref="A3:A51" si="0">ROW() - 1</f>
+        <f>ROW() - 1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2622,10 +2633,13 @@
       <c r="L3" s="2" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2658,10 +2672,13 @@
       <c r="L4" s="2" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2694,10 +2711,13 @@
       <c r="L5" s="2" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2730,10 +2750,13 @@
       <c r="L6" s="2" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2766,10 +2789,13 @@
       <c r="L7" s="2" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2790,721 +2816,782 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A10" s="2">
+        <f>ROW() - 1</f>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A11" s="2">
+        <f>ROW() - 1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A12" s="2">
+        <f>ROW() - 1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
+        <f>ROW() - 1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="N13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <f>ROW() - 1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A10" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>529</v>
+        <v>58</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+        <v>189</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="N14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>529</v>
+        <v>58</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+        <v>189</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="N15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>529</v>
+        <v>58</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+        <v>189</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="N16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>189</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+        <v>523</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="N17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>59</v>
+        <v>529</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>221</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+        <v>188</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A20" s="2">
+        <f>ROW() - 1</f>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A21" s="2">
+        <f>ROW() - 1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A22" s="2">
+        <f>ROW() - 1</f>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
+      <c r="I22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A23" s="2">
+        <f>ROW() - 1</f>
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="N23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
+        <f>ROW() - 1</f>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A20" s="2">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="N24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
+        <f>ROW() - 1</f>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
+      <c r="I25" s="2"/>
+      <c r="J25" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="K25" s="2"/>
+      <c r="N25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
+        <f>ROW() - 1</f>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A22" s="2">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A23" s="2">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A25" s="2">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A26" s="2">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="K26" s="2"/>
+      <c r="N26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
+        <f>ROW() - 1</f>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A27" s="2">
-        <f t="shared" si="0"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="N27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
+        <f>ROW() - 1</f>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A28" s="2">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>239</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
+        <f>ROW() - 1</f>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="J29" s="10" t="s">
         <v>539</v>
       </c>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A29" s="2">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="K29" s="2"/>
+      <c r="N29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A30" s="2">
+        <f>ROW() - 1</f>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="M29" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A30" s="2">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>162</v>
@@ -3523,521 +3610,577 @@
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
-        <v>545</v>
+        <v>188</v>
       </c>
       <c r="M30" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>183</v>
+        <v>536</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="I31" s="2"/>
+        <v>210</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K31" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="M31" t="s">
+        <v>544</v>
+      </c>
+      <c r="N31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>183</v>
+        <v>167</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>521</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="I32" s="2"/>
+        <v>210</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K32" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>183</v>
+        <v>167</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>522</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="I33" s="2"/>
+        <v>210</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>208</v>
+      </c>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K33" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>201</v>
+        <v>217</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>547</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>223</v>
+        <v>535</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>224</v>
+        <v>535</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>181</v>
+        <v>49</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>201</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>521</v>
+        <v>207</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>190</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K38" s="2"/>
+      <c r="N38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>522</v>
+        <v>206</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>185</v>
+        <v>218</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>208</v>
+        <v>548</v>
       </c>
       <c r="J39" s="2"/>
-      <c r="K39" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K39" s="2"/>
+      <c r="N39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>206</v>
+        <v>163</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>547</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>206</v>
+        <v>163</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>535</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>206</v>
+        <v>163</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>535</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>535</v>
+        <v>215</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="I44" s="2"/>
+        <v>216</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="I45" s="2"/>
+        <v>216</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>548</v>
+        <v>215</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -4059,9 +4202,9 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -4085,7 +4228,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -4115,7 +4258,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -4139,7 +4282,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -4162,6 +4305,9 @@
       <c r="K51" s="2"/>
     </row>
   </sheetData>
+  <sortState ref="A2:N51">
+    <sortCondition ref="N2:N51"/>
+  </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}" topLeftCell="A11">
       <selection activeCell="J25" sqref="J25"/>

</xml_diff>

<commit_message>
:joy: :joy: Works done in Chongqing excursion.
Add some initial lines to create a pandoc markdown to produce slides to
presenting data analysis results. :v:
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\git\CCDPro\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CCDPro\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
     <sheet name="Flanker" sheetId="16" r:id="rId12"/>
     <sheet name="TaskSwitching" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <customWorkbookViews>
     <customWorkbookView name="psychezl - 个人视图" guid="{EA03B590-7847-4E8E-A1B2-851363113915}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
   </customWorkbookViews>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="557">
   <si>
     <t>符号判断</t>
   </si>
@@ -2078,14 +2078,42 @@
   </si>
   <si>
     <t>SlideSection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SectionSummary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Languange Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Math Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Processing Speed Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attention Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Executive Function &amp; Updating Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Span &amp; Memory Tasks</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2229,7 +2257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2491,13 +2519,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="C24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40:O46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" customWidth="1"/>
@@ -2515,7 +2543,7 @@
     <col min="14" max="14" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -2558,10 +2586,13 @@
       <c r="N1" s="2" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O1" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2597,10 +2628,13 @@
       <c r="N2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2636,10 +2670,13 @@
       <c r="N3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O3" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2675,10 +2712,13 @@
       <c r="N4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O4" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2714,10 +2754,13 @@
       <c r="N5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O5" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2753,10 +2796,13 @@
       <c r="N6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O6" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2792,10 +2838,13 @@
       <c r="N7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O7" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2819,10 +2868,13 @@
       <c r="N8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O8" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2856,10 +2908,13 @@
       <c r="N9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O9" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2893,10 +2948,13 @@
       <c r="N10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O10" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2930,10 +2988,13 @@
       <c r="N11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O11" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2967,10 +3028,13 @@
       <c r="N12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O12" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3002,10 +3066,13 @@
       <c r="N13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O13" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3037,10 +3104,13 @@
       <c r="N14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O14" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3072,10 +3142,13 @@
       <c r="N15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O15" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3107,10 +3180,13 @@
       <c r="N16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O16" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -3142,10 +3218,13 @@
       <c r="N17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O17" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3179,10 +3258,13 @@
       <c r="N18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O18" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3216,10 +3298,13 @@
       <c r="N19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O19" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -3253,10 +3338,13 @@
       <c r="N20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O20" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -3290,10 +3378,13 @@
       <c r="N21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O21" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -3327,10 +3418,13 @@
       <c r="N22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O22" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -3364,10 +3458,13 @@
       <c r="N23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O23" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -3401,10 +3498,13 @@
       <c r="N24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O24" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -3436,10 +3536,13 @@
       <c r="N25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O25" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -3471,10 +3574,13 @@
       <c r="N26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O26" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -3504,10 +3610,13 @@
       <c r="N27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O27" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3541,10 +3650,13 @@
       <c r="N28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O28" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -3578,10 +3690,13 @@
       <c r="N29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O29" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3618,10 +3733,13 @@
       <c r="N30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O30" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -3658,10 +3776,13 @@
       <c r="N31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O31" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3695,10 +3816,13 @@
       <c r="N32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O32" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3732,10 +3856,13 @@
       <c r="N33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O33" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" ref="A34:A51" si="1">ROW() - 1</f>
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -3767,10 +3894,13 @@
       <c r="N34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O34" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -3802,10 +3932,13 @@
       <c r="N35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O35" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3837,10 +3970,13 @@
       <c r="N36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O36" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -3870,10 +4006,13 @@
       <c r="N37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O37" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -3903,10 +4042,13 @@
       <c r="N38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O38" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -3938,10 +4080,13 @@
       <c r="N39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O39" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -3971,10 +4116,13 @@
       <c r="N40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O40" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -4004,10 +4152,13 @@
       <c r="N41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O41" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -4037,10 +4188,13 @@
       <c r="N42">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O42" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -4072,10 +4226,13 @@
       <c r="N43">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O43" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -4107,10 +4264,13 @@
       <c r="N44">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O44" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -4142,10 +4302,13 @@
       <c r="N45">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O45" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -4177,10 +4340,13 @@
       <c r="N46">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O46" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -4202,9 +4368,9 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15">
       <c r="A48" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -4226,9 +4392,9 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:11">
       <c r="A49" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -4256,9 +4422,9 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:11">
       <c r="A50" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -4280,9 +4446,9 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11">
       <c r="A51" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -4330,9 +4496,9 @@
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -4340,7 +4506,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4348,7 +4514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4356,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4364,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4372,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4380,7 +4546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4388,7 +4554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4396,7 +4562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4404,7 +4570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4412,7 +4578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4420,7 +4586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4428,7 +4594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4450,9 +4616,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -4460,7 +4626,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4468,7 +4634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4476,7 +4642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4484,7 +4650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4492,7 +4658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4500,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4508,7 +4674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4530,12 +4696,12 @@
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -4546,7 +4712,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4557,7 +4723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4568,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4579,7 +4745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4605,12 +4771,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -4621,7 +4787,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4632,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4657,7 +4823,7 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.625" bestFit="1" customWidth="1"/>
@@ -4668,7 +4834,7 @@
     <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -4694,7 +4860,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <f>ROW() - 1</f>
         <v>1</v>
@@ -4716,7 +4882,7 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <f>ROW() - 1</f>
         <v>2</v>
@@ -4738,7 +4904,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A27" si="0">ROW() - 1</f>
         <v>3</v>
@@ -4760,7 +4926,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4782,7 +4948,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4804,7 +4970,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4826,7 +4992,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4848,7 +5014,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4870,7 +5036,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4892,7 +5058,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4914,7 +5080,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4936,7 +5102,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4960,7 +5126,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4982,7 +5148,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5006,7 +5172,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5028,7 +5194,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5052,7 +5218,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5074,7 +5240,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5096,7 +5262,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5118,7 +5284,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5140,7 +5306,7 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5162,7 +5328,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5184,7 +5350,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5208,7 +5374,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5230,7 +5396,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5246,7 +5412,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5285,7 +5451,7 @@
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.375" bestFit="1" customWidth="1"/>
@@ -5294,7 +5460,7 @@
     <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>225</v>
       </c>
@@ -5305,7 +5471,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -5317,7 +5483,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="1" customFormat="1">
       <c r="A3">
         <f t="shared" ref="A3:A9" si="0">ROW()-1</f>
         <v>2</v>
@@ -5333,7 +5499,7 @@
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5345,7 +5511,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5357,7 +5523,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5369,7 +5535,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5381,7 +5547,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5393,7 +5559,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5426,12 +5592,12 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -5439,7 +5605,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>266</v>
       </c>
@@ -5447,7 +5613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>267</v>
       </c>
@@ -5455,7 +5621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>268</v>
       </c>
@@ -5463,7 +5629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>269</v>
       </c>
@@ -5471,7 +5637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>270</v>
       </c>
@@ -5479,7 +5645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>271</v>
       </c>
@@ -5501,12 +5667,12 @@
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -5514,7 +5680,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
         <v>471</v>
       </c>
@@ -5522,7 +5688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
         <v>472</v>
       </c>
@@ -5530,7 +5696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
         <v>473</v>
       </c>
@@ -5538,7 +5704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="9" t="s">
         <v>474</v>
       </c>
@@ -5546,7 +5712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" s="9" t="s">
         <v>475</v>
       </c>
@@ -5554,7 +5720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" s="9" t="s">
         <v>476</v>
       </c>
@@ -5562,7 +5728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
         <v>477</v>
       </c>
@@ -5570,7 +5736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
         <v>478</v>
       </c>
@@ -5578,7 +5744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
         <v>479</v>
       </c>
@@ -5586,7 +5752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" s="9" t="s">
         <v>480</v>
       </c>
@@ -5594,7 +5760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" s="9" t="s">
         <v>481</v>
       </c>
@@ -5602,7 +5768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="9" t="s">
         <v>482</v>
       </c>
@@ -5610,7 +5776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" s="9" t="s">
         <v>483</v>
       </c>
@@ -5618,7 +5784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="9" t="s">
         <v>484</v>
       </c>
@@ -5626,7 +5792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" s="9" t="s">
         <v>485</v>
       </c>
@@ -5634,7 +5800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" s="9" t="s">
         <v>486</v>
       </c>
@@ -5642,7 +5808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" s="9" t="s">
         <v>487</v>
       </c>
@@ -5650,7 +5816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" s="9" t="s">
         <v>488</v>
       </c>
@@ -5658,7 +5824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" s="9" t="s">
         <v>489</v>
       </c>
@@ -5666,7 +5832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" s="9" t="s">
         <v>490</v>
       </c>
@@ -5674,7 +5840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22" s="9" t="s">
         <v>491</v>
       </c>
@@ -5682,7 +5848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23" s="9" t="s">
         <v>492</v>
       </c>
@@ -5690,7 +5856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24" s="9" t="s">
         <v>493</v>
       </c>
@@ -5698,7 +5864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25" s="9" t="s">
         <v>494</v>
       </c>
@@ -5706,7 +5872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26" s="9" t="s">
         <v>495</v>
       </c>
@@ -5714,7 +5880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27" s="9" t="s">
         <v>496</v>
       </c>
@@ -5722,7 +5888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28" s="9" t="s">
         <v>497</v>
       </c>
@@ -5730,7 +5896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29" s="9" t="s">
         <v>498</v>
       </c>
@@ -5738,7 +5904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" s="9" t="s">
         <v>499</v>
       </c>
@@ -5746,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" s="9" t="s">
         <v>500</v>
       </c>
@@ -5754,7 +5920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" s="9" t="s">
         <v>501</v>
       </c>
@@ -5762,7 +5928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" s="9" t="s">
         <v>502</v>
       </c>
@@ -5770,7 +5936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" s="9" t="s">
         <v>503</v>
       </c>
@@ -5778,7 +5944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" s="9" t="s">
         <v>504</v>
       </c>
@@ -5786,7 +5952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36" s="9" t="s">
         <v>505</v>
       </c>
@@ -5794,7 +5960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37" s="9" t="s">
         <v>506</v>
       </c>
@@ -5802,7 +5968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38" s="9" t="s">
         <v>507</v>
       </c>
@@ -5810,7 +5976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39" s="9" t="s">
         <v>508</v>
       </c>
@@ -5818,7 +5984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40" s="9" t="s">
         <v>509</v>
       </c>
@@ -5826,7 +5992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41" s="9" t="s">
         <v>510</v>
       </c>
@@ -5834,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42" s="9" t="s">
         <v>511</v>
       </c>
@@ -5842,7 +6008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43" s="9" t="s">
         <v>512</v>
       </c>
@@ -5850,7 +6016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44" s="9" t="s">
         <v>513</v>
       </c>
@@ -5858,7 +6024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45" s="9" t="s">
         <v>514</v>
       </c>
@@ -5866,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46" s="9" t="s">
         <v>515</v>
       </c>
@@ -5874,7 +6040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47" s="9" t="s">
         <v>516</v>
       </c>
@@ -5882,7 +6048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48" s="9" t="s">
         <v>517</v>
       </c>
@@ -5890,7 +6056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49" s="9" t="s">
         <v>518</v>
       </c>
@@ -5898,7 +6064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50" s="9" t="s">
         <v>519</v>
       </c>
@@ -5906,7 +6072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2">
       <c r="A51" s="9" t="s">
         <v>520</v>
       </c>
@@ -5926,12 +6092,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -5939,7 +6105,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -5947,7 +6113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>274</v>
       </c>
@@ -5955,7 +6121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>275</v>
       </c>
@@ -5963,7 +6129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>276</v>
       </c>
@@ -5971,7 +6137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>277</v>
       </c>
@@ -5979,7 +6145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>278</v>
       </c>
@@ -5987,7 +6153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>279</v>
       </c>
@@ -5995,7 +6161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -6003,7 +6169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>281</v>
       </c>
@@ -6011,7 +6177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -6019,7 +6185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>283</v>
       </c>
@@ -6027,7 +6193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>284</v>
       </c>
@@ -6035,7 +6201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>285</v>
       </c>
@@ -6043,7 +6209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>286</v>
       </c>
@@ -6051,7 +6217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>287</v>
       </c>
@@ -6059,7 +6225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>288</v>
       </c>
@@ -6067,7 +6233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>289</v>
       </c>
@@ -6075,7 +6241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>290</v>
       </c>
@@ -6083,7 +6249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>291</v>
       </c>
@@ -6091,7 +6257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>292</v>
       </c>
@@ -6099,7 +6265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>293</v>
       </c>
@@ -6107,7 +6273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>294</v>
       </c>
@@ -6115,7 +6281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>295</v>
       </c>
@@ -6123,7 +6289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>296</v>
       </c>
@@ -6131,7 +6297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>297</v>
       </c>
@@ -6139,7 +6305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>298</v>
       </c>
@@ -6147,7 +6313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>299</v>
       </c>
@@ -6155,7 +6321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>300</v>
       </c>
@@ -6163,7 +6329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>301</v>
       </c>
@@ -6171,7 +6337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>302</v>
       </c>
@@ -6179,7 +6345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>303</v>
       </c>
@@ -6187,7 +6353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -6195,7 +6361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>305</v>
       </c>
@@ -6203,7 +6369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>306</v>
       </c>
@@ -6211,7 +6377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>307</v>
       </c>
@@ -6219,7 +6385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>308</v>
       </c>
@@ -6227,7 +6393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>309</v>
       </c>
@@ -6235,7 +6401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>310</v>
       </c>
@@ -6243,7 +6409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>311</v>
       </c>
@@ -6251,7 +6417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>312</v>
       </c>
@@ -6259,7 +6425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>313</v>
       </c>
@@ -6267,7 +6433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>314</v>
       </c>
@@ -6275,7 +6441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>315</v>
       </c>
@@ -6283,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>316</v>
       </c>
@@ -6291,7 +6457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>317</v>
       </c>
@@ -6299,7 +6465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>318</v>
       </c>
@@ -6307,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>319</v>
       </c>
@@ -6315,7 +6481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>320</v>
       </c>
@@ -6323,7 +6489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>321</v>
       </c>
@@ -6331,7 +6497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>322</v>
       </c>
@@ -6351,13 +6517,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -6365,7 +6531,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>323</v>
       </c>
@@ -6373,7 +6539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -6381,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>325</v>
       </c>
@@ -6389,7 +6555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>326</v>
       </c>
@@ -6397,7 +6563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>327</v>
       </c>
@@ -6405,7 +6571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>328</v>
       </c>
@@ -6413,7 +6579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>329</v>
       </c>
@@ -6421,7 +6587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>330</v>
       </c>
@@ -6429,7 +6595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>331</v>
       </c>
@@ -6437,7 +6603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>332</v>
       </c>
@@ -6445,7 +6611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>333</v>
       </c>
@@ -6453,7 +6619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>334</v>
       </c>
@@ -6461,7 +6627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>335</v>
       </c>
@@ -6469,7 +6635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>336</v>
       </c>
@@ -6477,7 +6643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>337</v>
       </c>
@@ -6485,7 +6651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>338</v>
       </c>
@@ -6493,7 +6659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>339</v>
       </c>
@@ -6501,7 +6667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>329</v>
       </c>
@@ -6509,7 +6675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>340</v>
       </c>
@@ -6517,7 +6683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>341</v>
       </c>
@@ -6525,7 +6691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>342</v>
       </c>
@@ -6533,7 +6699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>343</v>
       </c>
@@ -6541,7 +6707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>344</v>
       </c>
@@ -6549,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>345</v>
       </c>
@@ -6557,7 +6723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>346</v>
       </c>
@@ -6565,7 +6731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>347</v>
       </c>
@@ -6573,7 +6739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>348</v>
       </c>
@@ -6581,7 +6747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>349</v>
       </c>
@@ -6589,7 +6755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>350</v>
       </c>
@@ -6597,7 +6763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>351</v>
       </c>
@@ -6605,7 +6771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>352</v>
       </c>
@@ -6613,7 +6779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>353</v>
       </c>
@@ -6621,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>354</v>
       </c>
@@ -6629,7 +6795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>355</v>
       </c>
@@ -6637,7 +6803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>356</v>
       </c>
@@ -6645,7 +6811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>357</v>
       </c>
@@ -6653,7 +6819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>358</v>
       </c>
@@ -6661,7 +6827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>359</v>
       </c>
@@ -6669,7 +6835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>360</v>
       </c>
@@ -6677,7 +6843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>361</v>
       </c>
@@ -6685,7 +6851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>362</v>
       </c>
@@ -6693,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>363</v>
       </c>
@@ -6701,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>364</v>
       </c>
@@ -6709,7 +6875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>365</v>
       </c>
@@ -6717,7 +6883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>366</v>
       </c>
@@ -6725,7 +6891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>367</v>
       </c>
@@ -6733,7 +6899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>368</v>
       </c>
@@ -6741,7 +6907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>369</v>
       </c>
@@ -6749,7 +6915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>370</v>
       </c>
@@ -6757,7 +6923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>371</v>
       </c>
@@ -6779,12 +6945,12 @@
       <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -6792,7 +6958,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>372</v>
       </c>
@@ -6800,7 +6966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>373</v>
       </c>
@@ -6808,7 +6974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>374</v>
       </c>
@@ -6816,7 +6982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>375</v>
       </c>
@@ -6824,7 +6990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>376</v>
       </c>
@@ -6832,7 +6998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>377</v>
       </c>
@@ -6840,7 +7006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -6848,7 +7014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>379</v>
       </c>
@@ -6856,7 +7022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>380</v>
       </c>
@@ -6864,7 +7030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>381</v>
       </c>
@@ -6872,7 +7038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>382</v>
       </c>
@@ -6880,7 +7046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>383</v>
       </c>
@@ -6888,7 +7054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>384</v>
       </c>
@@ -6896,7 +7062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>385</v>
       </c>
@@ -6904,7 +7070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>386</v>
       </c>
@@ -6912,7 +7078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>387</v>
       </c>
@@ -6920,7 +7086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>388</v>
       </c>
@@ -6928,7 +7094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>389</v>
       </c>
@@ -6936,7 +7102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>390</v>
       </c>
@@ -6944,7 +7110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>391</v>
       </c>
@@ -6952,7 +7118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>392</v>
       </c>
@@ -6960,7 +7126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>393</v>
       </c>
@@ -6968,7 +7134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>394</v>
       </c>
@@ -6976,7 +7142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>395</v>
       </c>
@@ -6984,7 +7150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>396</v>
       </c>
@@ -6992,7 +7158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>397</v>
       </c>
@@ -7000,7 +7166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>398</v>
       </c>
@@ -7008,7 +7174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>399</v>
       </c>
@@ -7016,7 +7182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>400</v>
       </c>
@@ -7024,7 +7190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>401</v>
       </c>
@@ -7032,7 +7198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>402</v>
       </c>
@@ -7040,7 +7206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>403</v>
       </c>
@@ -7048,7 +7214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>404</v>
       </c>
@@ -7056,7 +7222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>405</v>
       </c>
@@ -7064,7 +7230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>406</v>
       </c>
@@ -7072,7 +7238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>407</v>
       </c>
@@ -7080,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>408</v>
       </c>
@@ -7088,7 +7254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>409</v>
       </c>
@@ -7096,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>410</v>
       </c>
@@ -7104,7 +7270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>411</v>
       </c>
@@ -7112,7 +7278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>412</v>
       </c>
@@ -7120,7 +7286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>413</v>
       </c>
@@ -7128,7 +7294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>414</v>
       </c>
@@ -7136,7 +7302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>415</v>
       </c>
@@ -7144,7 +7310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>416</v>
       </c>
@@ -7152,7 +7318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>417</v>
       </c>
@@ -7160,7 +7326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>418</v>
       </c>
@@ -7168,7 +7334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>419</v>
       </c>
@@ -7176,7 +7342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>420</v>
       </c>
@@ -7184,7 +7350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>421</v>
       </c>
@@ -7206,12 +7372,12 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -7219,7 +7385,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>422</v>
       </c>
@@ -7227,7 +7393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>423</v>
       </c>
@@ -7235,7 +7401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>424</v>
       </c>
@@ -7243,7 +7409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>425</v>
       </c>
@@ -7251,7 +7417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>426</v>
       </c>
@@ -7259,7 +7425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>427</v>
       </c>
@@ -7267,7 +7433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>428</v>
       </c>
@@ -7275,7 +7441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>429</v>
       </c>
@@ -7283,7 +7449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>430</v>
       </c>
@@ -7291,7 +7457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>431</v>
       </c>
@@ -7299,7 +7465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>432</v>
       </c>
@@ -7307,7 +7473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>433</v>
       </c>
@@ -7315,7 +7481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>434</v>
       </c>
@@ -7323,7 +7489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>435</v>
       </c>
@@ -7331,7 +7497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>436</v>
       </c>
@@ -7339,7 +7505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>437</v>
       </c>
@@ -7347,7 +7513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>438</v>
       </c>
@@ -7355,7 +7521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>439</v>
       </c>
@@ -7363,7 +7529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>440</v>
       </c>
@@ -7371,7 +7537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>441</v>
       </c>
@@ -7379,7 +7545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>442</v>
       </c>
@@ -7387,7 +7553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>443</v>
       </c>
@@ -7395,7 +7561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>444</v>
       </c>
@@ -7403,7 +7569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>445</v>
       </c>
@@ -7411,7 +7577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>446</v>
       </c>
@@ -7419,7 +7585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>447</v>
       </c>
@@ -7427,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>448</v>
       </c>
@@ -7435,7 +7601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>449</v>
       </c>
@@ -7443,7 +7609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>450</v>
       </c>
@@ -7451,7 +7617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>451</v>
       </c>
@@ -7459,7 +7625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>452</v>
       </c>
@@ -7467,7 +7633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>453</v>
       </c>
@@ -7475,7 +7641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>454</v>
       </c>
@@ -7483,7 +7649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>455</v>
       </c>
@@ -7491,7 +7657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>456</v>
       </c>
@@ -7499,7 +7665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>457</v>
       </c>
@@ -7507,7 +7673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>458</v>
       </c>
@@ -7515,7 +7681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>459</v>
       </c>
@@ -7523,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>460</v>
       </c>
@@ -7531,7 +7697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>461</v>
       </c>
@@ -7539,7 +7705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>377</v>
       </c>
@@ -7547,7 +7713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>462</v>
       </c>
@@ -7555,7 +7721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>463</v>
       </c>
@@ -7563,7 +7729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>464</v>
       </c>
@@ -7571,7 +7737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>465</v>
       </c>
@@ -7579,7 +7745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>466</v>
       </c>
@@ -7587,7 +7753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>467</v>
       </c>
@@ -7595,7 +7761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>468</v>
       </c>
@@ -7603,7 +7769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>469</v>
       </c>
@@ -7611,7 +7777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>470</v>
       </c>

</xml_diff>

<commit_message>
:tada: :see_no_evil: Processing framework done!
More polish works done. The featuring jobs done are
1. the data processing pipeline now formed, and
2. the data processing for reading task is now added. :smile: :v:
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="563">
   <si>
     <t>符号判断</t>
   </si>
@@ -2123,6 +2123,18 @@
   </si>
   <si>
     <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotalTime CountTotalTrl CountAccTrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTotalTrl CountAccTrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountAccTrl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2538,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2828,7 +2840,7 @@
         <v>178</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -2851,12 +2863,17 @@
       <c r="D8" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="2" t="s">
+        <v>562</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
+      <c r="K8" t="s">
+        <v>561</v>
+      </c>
       <c r="M8">
         <v>1</v>
       </c>
@@ -5878,7 +5895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add the SID column in schoolInfo and fmtext worksheet.
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
     <sheet name="para" sheetId="2" r:id="rId2"/>
     <sheet name="schoolinfo" sheetId="3" r:id="rId3"/>
     <sheet name="gradeinfo" sheetId="19" r:id="rId4"/>
-    <sheet name="Symbol" sheetId="4" r:id="rId5"/>
-    <sheet name="Orthograph" sheetId="5" r:id="rId6"/>
-    <sheet name="Tone" sheetId="6" r:id="rId7"/>
-    <sheet name="Pinyin" sheetId="7" r:id="rId8"/>
-    <sheet name="Lexic" sheetId="8" r:id="rId9"/>
-    <sheet name="Semantic" sheetId="9" r:id="rId10"/>
-    <sheet name="GNGLure" sheetId="13" r:id="rId11"/>
-    <sheet name="GNGFruit" sheetId="14" r:id="rId12"/>
-    <sheet name="Flanker" sheetId="16" r:id="rId13"/>
-    <sheet name="TaskSwitching" sheetId="18" r:id="rId14"/>
+    <sheet name="fmtext" sheetId="20" r:id="rId5"/>
+    <sheet name="Symbol" sheetId="4" r:id="rId6"/>
+    <sheet name="Orthograph" sheetId="5" r:id="rId7"/>
+    <sheet name="Tone" sheetId="6" r:id="rId8"/>
+    <sheet name="Pinyin" sheetId="7" r:id="rId9"/>
+    <sheet name="Lexic" sheetId="8" r:id="rId10"/>
+    <sheet name="Semantic" sheetId="9" r:id="rId11"/>
+    <sheet name="GNGLure" sheetId="13" r:id="rId12"/>
+    <sheet name="GNGFruit" sheetId="14" r:id="rId13"/>
+    <sheet name="Flanker" sheetId="16" r:id="rId14"/>
+    <sheet name="TaskSwitching" sheetId="18" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <customWorkbookViews>
@@ -287,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="598">
   <si>
     <t>符号判断</t>
   </si>
@@ -2234,6 +2235,107 @@
   <si>
     <t>Condition STIM ACC RT</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fmt</t>
+  </si>
+  <si>
+    <t>ext</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jpeg</t>
+  </si>
+  <si>
+    <t>.jpg</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>.png</t>
+  </si>
+  <si>
+    <t>tiff</t>
+  </si>
+  <si>
+    <t>.tif</t>
+  </si>
+  <si>
+    <t>tiffn</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>.emf</t>
+  </si>
+  <si>
+    <t>bmpmono</t>
+  </si>
+  <si>
+    <t>.bmp</t>
+  </si>
+  <si>
+    <t>bmp</t>
+  </si>
+  <si>
+    <t>bmp16m</t>
+  </si>
+  <si>
+    <t>bmp256</t>
+  </si>
+  <si>
+    <t>hdf</t>
+  </si>
+  <si>
+    <t>.hdf</t>
+  </si>
+  <si>
+    <t>pbm</t>
+  </si>
+  <si>
+    <t>.pbm</t>
+  </si>
+  <si>
+    <t>pbmraw</t>
+  </si>
+  <si>
+    <t>pcxmono</t>
+  </si>
+  <si>
+    <t>.pcx</t>
+  </si>
+  <si>
+    <t>pcx24b</t>
+  </si>
+  <si>
+    <t>pcx256</t>
+  </si>
+  <si>
+    <t>pcx16</t>
+  </si>
+  <si>
+    <t>pgm</t>
+  </si>
+  <si>
+    <t>.pgm</t>
+  </si>
+  <si>
+    <t>pgmraw</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>.ppm</t>
+  </si>
+  <si>
+    <t>ppmraw</t>
   </si>
 </sst>
 </file>
@@ -2703,7 +2805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -4806,6 +4908,433 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>358</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>359</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>360</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>361</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>363</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>364</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>365</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>366</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>367</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>368</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>369</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>370</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>371</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>372</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>373</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>374</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>375</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>376</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>377</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>378</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>379</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>380</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>381</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>382</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>383</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>384</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>385</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>386</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>387</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>388</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>389</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>390</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>391</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>392</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>393</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>394</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>395</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>396</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>397</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>398</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>399</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B51"/>
+  <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B6" sqref="B1:B1048576"/>
     </sheetView>
@@ -5229,7 +5758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -5349,7 +5878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -5429,7 +5958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -5504,7 +6033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -6189,7 +6718,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6211,6 +6740,9 @@
       <c r="C1" t="s">
         <v>208</v>
       </c>
+      <c r="D1" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
@@ -6223,6 +6755,9 @@
       <c r="C2" t="s">
         <v>218</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3">
@@ -6235,7 +6770,9 @@
       <c r="C3" t="s">
         <v>219</v>
       </c>
-      <c r="D3"/>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3"/>
@@ -6251,6 +6788,9 @@
       <c r="C4" t="s">
         <v>217</v>
       </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
@@ -6263,6 +6803,9 @@
       <c r="C5" t="s">
         <v>213</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
@@ -6275,6 +6818,9 @@
       <c r="C6" t="s">
         <v>215</v>
       </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
@@ -6287,6 +6833,9 @@
       <c r="C7" t="s">
         <v>212</v>
       </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
@@ -6299,6 +6848,9 @@
       <c r="C8" t="s">
         <v>211</v>
       </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
@@ -6310,6 +6862,9 @@
       </c>
       <c r="C9" t="s">
         <v>216</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -6509,6 +7064,191 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>572</v>
+      </c>
+      <c r="B4" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>574</v>
+      </c>
+      <c r="B5" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>575</v>
+      </c>
+      <c r="B6" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>577</v>
+      </c>
+      <c r="B7" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>579</v>
+      </c>
+      <c r="B8" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>580</v>
+      </c>
+      <c r="B9" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>581</v>
+      </c>
+      <c r="B10" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>582</v>
+      </c>
+      <c r="B11" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>584</v>
+      </c>
+      <c r="B12" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>586</v>
+      </c>
+      <c r="B13" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>587</v>
+      </c>
+      <c r="B14" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>589</v>
+      </c>
+      <c r="B15" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>590</v>
+      </c>
+      <c r="B16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>591</v>
+      </c>
+      <c r="B17" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>592</v>
+      </c>
+      <c r="B18" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>594</v>
+      </c>
+      <c r="B19" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>595</v>
+      </c>
+      <c r="B20" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>597</v>
+      </c>
+      <c r="B21" t="s">
+        <v>596</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6574,433 +7314,6 @@
       </c>
       <c r="B7">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
-        <v>450</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="9" t="s">
-        <v>451</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="9" t="s">
-        <v>453</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="9" t="s">
-        <v>455</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="9" t="s">
-        <v>456</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
-        <v>457</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="9" t="s">
-        <v>458</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="9" t="s">
-        <v>459</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="9" t="s">
-        <v>460</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="9" t="s">
-        <v>461</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="9" t="s">
-        <v>462</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="9" t="s">
-        <v>463</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="9" t="s">
-        <v>464</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="9" t="s">
-        <v>465</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="9" t="s">
-        <v>466</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="9" t="s">
-        <v>467</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="9" t="s">
-        <v>468</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="9" t="s">
-        <v>471</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="9" t="s">
-        <v>476</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="9" t="s">
-        <v>477</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="9" t="s">
-        <v>480</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="9" t="s">
-        <v>483</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="9" t="s">
-        <v>484</v>
-      </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="B44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="B45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="9" t="s">
-        <v>493</v>
-      </c>
-      <c r="B46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="B48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="9" t="s">
-        <v>496</v>
-      </c>
-      <c r="B49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="9" t="s">
-        <v>497</v>
-      </c>
-      <c r="B50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="B51">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7031,400 +7344,400 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>251</v>
+      <c r="A2" s="9" t="s">
+        <v>449</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>252</v>
+      <c r="A3" s="9" t="s">
+        <v>450</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>253</v>
+      <c r="A4" s="9" t="s">
+        <v>451</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>254</v>
+      <c r="A5" s="9" t="s">
+        <v>452</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>255</v>
+      <c r="A6" s="9" t="s">
+        <v>453</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>256</v>
+      <c r="A7" s="9" t="s">
+        <v>454</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>257</v>
+      <c r="A8" s="9" t="s">
+        <v>455</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>258</v>
+      <c r="A9" s="9" t="s">
+        <v>456</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>259</v>
+      <c r="A10" s="9" t="s">
+        <v>457</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>260</v>
+      <c r="A11" s="9" t="s">
+        <v>458</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>261</v>
+      <c r="A12" s="9" t="s">
+        <v>459</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>262</v>
+      <c r="A13" s="9" t="s">
+        <v>460</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>263</v>
+      <c r="A14" s="9" t="s">
+        <v>461</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>264</v>
+      <c r="A15" s="9" t="s">
+        <v>462</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>265</v>
+      <c r="A16" s="9" t="s">
+        <v>463</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>266</v>
+      <c r="A17" s="9" t="s">
+        <v>464</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>267</v>
+      <c r="A18" s="9" t="s">
+        <v>465</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>268</v>
+      <c r="A19" s="9" t="s">
+        <v>466</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>269</v>
+      <c r="A20" s="9" t="s">
+        <v>467</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>270</v>
+      <c r="A21" s="9" t="s">
+        <v>468</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>271</v>
+      <c r="A22" s="9" t="s">
+        <v>469</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>272</v>
+      <c r="A23" s="9" t="s">
+        <v>470</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>273</v>
+      <c r="A24" s="9" t="s">
+        <v>471</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>274</v>
+      <c r="A25" s="9" t="s">
+        <v>472</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>275</v>
+      <c r="A26" s="9" t="s">
+        <v>473</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>276</v>
+      <c r="A27" s="9" t="s">
+        <v>474</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>277</v>
+      <c r="A28" s="9" t="s">
+        <v>475</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>278</v>
+      <c r="A29" s="9" t="s">
+        <v>476</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>279</v>
+      <c r="A30" s="9" t="s">
+        <v>477</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>280</v>
+      <c r="A31" s="9" t="s">
+        <v>478</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>281</v>
+      <c r="A32" s="9" t="s">
+        <v>479</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>282</v>
+      <c r="A33" s="9" t="s">
+        <v>480</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>283</v>
+      <c r="A34" s="9" t="s">
+        <v>481</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>284</v>
+      <c r="A35" s="9" t="s">
+        <v>482</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>285</v>
+      <c r="A36" s="9" t="s">
+        <v>483</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>286</v>
+      <c r="A37" s="9" t="s">
+        <v>484</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>287</v>
+      <c r="A38" s="9" t="s">
+        <v>485</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
-        <v>288</v>
+      <c r="A39" s="9" t="s">
+        <v>486</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>289</v>
+      <c r="A40" s="9" t="s">
+        <v>487</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>290</v>
+      <c r="A41" s="9" t="s">
+        <v>488</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
-        <v>291</v>
+      <c r="A42" s="9" t="s">
+        <v>489</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
-        <v>292</v>
+      <c r="A43" s="9" t="s">
+        <v>490</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>293</v>
+      <c r="A44" s="9" t="s">
+        <v>491</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>294</v>
+      <c r="A45" s="9" t="s">
+        <v>492</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
-        <v>295</v>
+      <c r="A46" s="9" t="s">
+        <v>493</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
-        <v>296</v>
+      <c r="A47" s="9" t="s">
+        <v>494</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
-        <v>297</v>
+      <c r="A48" s="9" t="s">
+        <v>495</v>
       </c>
       <c r="B48">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
-        <v>298</v>
+      <c r="A49" s="9" t="s">
+        <v>496</v>
       </c>
       <c r="B49">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
-        <v>299</v>
+      <c r="A50" s="9" t="s">
+        <v>497</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
-        <v>300</v>
+      <c r="A51" s="9" t="s">
+        <v>498</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -7446,8 +7759,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -7460,31 +7772,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>251</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>252</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>254</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -7492,7 +7804,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>255</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7500,15 +7812,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>256</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>257</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -7516,7 +7828,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -7524,7 +7836,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -7532,15 +7844,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>311</v>
+        <v>261</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -7548,15 +7860,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>312</v>
+        <v>262</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>313</v>
+        <v>263</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -7564,15 +7876,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -7580,23 +7892,23 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>307</v>
+        <v>268</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -7604,7 +7916,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>318</v>
+        <v>269</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -7612,15 +7924,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>319</v>
+        <v>270</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>320</v>
+        <v>271</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -7628,7 +7940,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>321</v>
+        <v>272</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -7636,23 +7948,23 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>322</v>
+        <v>273</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>323</v>
+        <v>274</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>324</v>
+        <v>275</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -7660,7 +7972,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>325</v>
+        <v>276</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -7668,15 +7980,15 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>326</v>
+        <v>277</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>327</v>
+        <v>278</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -7684,7 +7996,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>328</v>
+        <v>279</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -7692,7 +8004,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>329</v>
+        <v>280</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -7700,15 +8012,15 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>281</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>331</v>
+        <v>282</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -7716,15 +8028,15 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>332</v>
+        <v>283</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>333</v>
+        <v>284</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -7732,7 +8044,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>334</v>
+        <v>285</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -7740,31 +8052,31 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>335</v>
+        <v>286</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>336</v>
+        <v>287</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>337</v>
+        <v>288</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>338</v>
+        <v>289</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -7772,15 +8084,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>339</v>
+        <v>290</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>340</v>
+        <v>291</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -7788,7 +8100,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>341</v>
+        <v>292</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -7796,7 +8108,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -7804,23 +8116,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>344</v>
+        <v>295</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>345</v>
+        <v>296</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -7828,7 +8140,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>346</v>
+        <v>297</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -7836,26 +8148,26 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>347</v>
+        <v>298</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>348</v>
+        <v>299</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>349</v>
+        <v>300</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7874,7 +8186,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -7887,31 +8200,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>350</v>
+        <v>301</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>351</v>
+        <v>302</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>352</v>
+        <v>303</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>353</v>
+        <v>304</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -7919,7 +8232,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>354</v>
+        <v>305</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7927,15 +8240,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>355</v>
+        <v>306</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>307</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -7943,7 +8256,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>357</v>
+        <v>308</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -7951,7 +8264,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>309</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -7959,15 +8272,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>359</v>
+        <v>310</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>360</v>
+        <v>311</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -7975,15 +8288,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>361</v>
+        <v>312</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>362</v>
+        <v>313</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -7991,15 +8304,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>363</v>
+        <v>314</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>364</v>
+        <v>315</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -8007,23 +8320,23 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>365</v>
+        <v>316</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>366</v>
+        <v>317</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>367</v>
+        <v>307</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -8031,7 +8344,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>368</v>
+        <v>318</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -8039,15 +8352,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>369</v>
+        <v>319</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>370</v>
+        <v>320</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -8055,7 +8368,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -8063,23 +8376,23 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -8087,7 +8400,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>375</v>
+        <v>325</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -8095,15 +8408,15 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>376</v>
+        <v>326</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -8111,7 +8424,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>378</v>
+        <v>328</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -8119,7 +8432,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8127,15 +8440,15 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -8143,15 +8456,15 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>382</v>
+        <v>332</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>383</v>
+        <v>333</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -8159,7 +8472,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>384</v>
+        <v>334</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -8167,31 +8480,31 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>385</v>
+        <v>335</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>386</v>
+        <v>336</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>387</v>
+        <v>337</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>388</v>
+        <v>338</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -8199,15 +8512,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>389</v>
+        <v>339</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -8215,7 +8528,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>391</v>
+        <v>341</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -8223,7 +8536,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>392</v>
+        <v>342</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -8231,23 +8544,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>393</v>
+        <v>343</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>395</v>
+        <v>345</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -8255,7 +8568,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -8263,26 +8576,26 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>397</v>
+        <v>347</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>398</v>
+        <v>348</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>399</v>
+        <v>349</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix in taskSettings.
Nback variables should be MRT.
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="599">
   <si>
     <t>符号判断</t>
   </si>
@@ -988,48 +988,44 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>MNHit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall R1 R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall R1 R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REP Food Face Resp ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Span</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memrep</t>
+  </si>
+  <si>
+    <t>Memsep</t>
+  </si>
+  <si>
+    <t>Conflict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall hit FA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ACC RT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MNHit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall R1 R2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall R1 R2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REP Food Face Resp ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Span</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memrep</t>
-  </si>
-  <si>
-    <t>Memsep</t>
-  </si>
-  <si>
-    <t>Conflict</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall hit FA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Rate_Overall</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2336,6 +2332,14 @@
   </si>
   <si>
     <t>ppmraw</t>
+  </si>
+  <si>
+    <t>ACC MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2805,8 +2809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2841,40 +2845,40 @@
         <v>160</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>171</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>172</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>523</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.15">
@@ -2893,10 +2897,10 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>170</v>
@@ -2909,16 +2913,16 @@
         <v>173</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
@@ -2937,10 +2941,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>170</v>
@@ -2953,16 +2957,16 @@
         <v>173</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
@@ -2981,10 +2985,10 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>170</v>
@@ -2997,16 +3001,16 @@
         <v>173</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
@@ -3025,10 +3029,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>170</v>
@@ -3041,16 +3045,16 @@
         <v>173</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
@@ -3069,10 +3073,10 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>170</v>
@@ -3085,16 +3089,16 @@
         <v>173</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
@@ -3103,7 +3107,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>96</v>
@@ -3113,10 +3117,10 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>170</v>
@@ -3129,16 +3133,16 @@
         <v>173</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O7">
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
@@ -3147,34 +3151,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" t="s">
+        <v>546</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>548</v>
-      </c>
       <c r="O8">
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
@@ -3195,32 +3199,32 @@
         <v>3000</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>178</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L9" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O9">
         <v>2</v>
       </c>
       <c r="P9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
@@ -3241,32 +3245,32 @@
         <v>3000</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>178</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O10">
         <v>2</v>
       </c>
       <c r="P10" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
@@ -3287,29 +3291,29 @@
         <v>2000</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>178</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O11">
         <v>2</v>
       </c>
       <c r="P11" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
@@ -3321,7 +3325,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>144</v>
@@ -3330,29 +3334,29 @@
         <v>3000</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>178</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O12">
         <v>2</v>
       </c>
       <c r="P12" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
@@ -3373,27 +3377,27 @@
         <v>2000</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>182</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="N13" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O13">
         <v>2</v>
       </c>
       <c r="P13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
@@ -3417,7 +3421,7 @@
         <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>174</v>
@@ -3428,13 +3432,13 @@
       </c>
       <c r="K14" s="2"/>
       <c r="N14" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O14">
         <v>3</v>
       </c>
       <c r="P14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
@@ -3458,7 +3462,7 @@
         <v>48</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>174</v>
@@ -3469,13 +3473,13 @@
       </c>
       <c r="K15" s="2"/>
       <c r="N15" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O15">
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
@@ -3499,7 +3503,7 @@
         <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>174</v>
@@ -3510,13 +3514,13 @@
       </c>
       <c r="K16" s="2"/>
       <c r="N16" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O16">
         <v>3</v>
       </c>
       <c r="P16" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
@@ -3540,24 +3544,24 @@
         <v>48</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>174</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K17" s="2"/>
       <c r="N17" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O17">
         <v>3</v>
       </c>
       <c r="P17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
@@ -3578,10 +3582,10 @@
         <v>3000</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>170</v>
@@ -3594,13 +3598,13 @@
         <v>173</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O18">
         <v>3</v>
       </c>
       <c r="P18" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
@@ -3621,10 +3625,10 @@
         <v>3000</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>170</v>
@@ -3637,13 +3641,13 @@
         <v>173</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O19">
         <v>3</v>
       </c>
       <c r="P19" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
@@ -3664,10 +3668,10 @@
         <v>3000</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>170</v>
@@ -3680,13 +3684,13 @@
         <v>173</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O20">
         <v>3</v>
       </c>
       <c r="P20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
@@ -3707,10 +3711,10 @@
         <v>3000</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>170</v>
@@ -3723,13 +3727,13 @@
         <v>173</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O21">
         <v>3</v>
       </c>
       <c r="P21" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
@@ -3750,29 +3754,29 @@
         <v>3000</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>174</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O22">
         <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
@@ -3793,29 +3797,29 @@
         <v>3000</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>174</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O23">
         <v>3</v>
       </c>
       <c r="P23" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
@@ -3836,29 +3840,29 @@
         <v>3000</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>174</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O24">
         <v>3</v>
       </c>
       <c r="P24" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
@@ -3882,7 +3886,7 @@
         <v>48</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>174</v>
@@ -3893,13 +3897,13 @@
       </c>
       <c r="K25" s="2"/>
       <c r="N25" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O25">
         <v>3</v>
       </c>
       <c r="P25" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
@@ -3923,7 +3927,7 @@
         <v>48</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>174</v>
@@ -3934,13 +3938,13 @@
       </c>
       <c r="K26" s="2"/>
       <c r="N26" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O26">
         <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
@@ -3959,10 +3963,10 @@
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>179</v>
@@ -3971,13 +3975,13 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="N27" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O27">
         <v>4</v>
       </c>
       <c r="P27" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
@@ -3992,16 +3996,16 @@
         <v>102</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E28" s="5">
         <v>1000</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>170</v>
@@ -4014,13 +4018,13 @@
         <v>173</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O28">
         <v>4</v>
       </c>
       <c r="P28" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
@@ -4041,29 +4045,29 @@
         <v>500</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H29" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>515</v>
-      </c>
       <c r="J29" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K29" s="2"/>
       <c r="N29" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="O29">
         <v>4</v>
       </c>
       <c r="P29" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
@@ -4084,10 +4088,10 @@
         <v>1000</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>170</v>
@@ -4100,16 +4104,16 @@
         <v>173</v>
       </c>
       <c r="M30" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O30">
         <v>4</v>
       </c>
       <c r="P30" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
@@ -4130,10 +4134,10 @@
         <v>1000</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>170</v>
@@ -4143,19 +4147,19 @@
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="M31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O31">
         <v>4</v>
       </c>
       <c r="P31" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
@@ -4176,10 +4180,10 @@
         <v>2000</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>170</v>
@@ -4192,13 +4196,13 @@
         <v>173</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O32">
         <v>5</v>
       </c>
       <c r="P32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
@@ -4219,29 +4223,29 @@
         <v>0</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>170</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2" t="s">
         <v>173</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O33">
         <v>5</v>
       </c>
       <c r="P33" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.15">
@@ -4262,27 +4266,27 @@
         <v>3000</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>182</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="N34" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O34">
         <v>5</v>
       </c>
       <c r="P34" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.15">
@@ -4303,27 +4307,27 @@
         <v>3000</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>182</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="N35" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O35">
         <v>5</v>
       </c>
       <c r="P35" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.15">
@@ -4342,27 +4346,27 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>182</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="N36" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O36">
         <v>5</v>
       </c>
       <c r="P36" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.15">
@@ -4383,27 +4387,27 @@
         <v>3000</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>182</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="N37" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O37">
         <v>5</v>
       </c>
       <c r="P37" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.15">
@@ -4424,25 +4428,25 @@
         <v>2000</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>183</v>
+        <v>597</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="N38" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O38">
         <v>5</v>
       </c>
       <c r="P38" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.15">
@@ -4463,25 +4467,25 @@
         <v>2000</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>183</v>
+        <v>598</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="N39" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O39">
         <v>5</v>
       </c>
       <c r="P39" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.15">
@@ -4503,7 +4507,7 @@
         <v>168</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>179</v>
@@ -4512,13 +4516,13 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="N40" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O40">
         <v>6</v>
       </c>
       <c r="P40" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.15">
@@ -4540,7 +4544,7 @@
         <v>168</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>179</v>
@@ -4549,13 +4553,13 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="N41" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O41">
         <v>6</v>
       </c>
       <c r="P41" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.15">
@@ -4577,7 +4581,7 @@
         <v>168</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>179</v>
@@ -4586,13 +4590,13 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="N42" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O42">
         <v>6</v>
       </c>
       <c r="P42" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.15">
@@ -4613,27 +4617,27 @@
         <v>2000</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="N43" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O43">
         <v>6</v>
       </c>
       <c r="P43" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.15">
@@ -4654,27 +4658,27 @@
         <v>2000</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>180</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="N44" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="O44">
         <v>6</v>
       </c>
       <c r="P44" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.15">
@@ -4695,27 +4699,27 @@
         <v>2000</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="N45" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="O45">
         <v>6</v>
       </c>
       <c r="P45" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.15">
@@ -4736,27 +4740,27 @@
         <v>2000</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>181</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="N46" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O46">
         <v>6</v>
       </c>
       <c r="P46" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.15">
@@ -4776,7 +4780,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -4801,7 +4805,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -4828,16 +4832,16 @@
         <v>49</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="N49" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.15">
@@ -4919,15 +4923,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4935,7 +4939,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4943,7 +4947,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4951,7 +4955,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4959,7 +4963,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4967,7 +4971,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4975,7 +4979,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4983,7 +4987,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4991,7 +4995,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4999,7 +5003,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5007,7 +5011,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5015,7 +5019,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5023,7 +5027,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5031,7 +5035,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -5039,7 +5043,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -5047,7 +5051,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -5055,7 +5059,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5063,7 +5067,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -5071,7 +5075,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5079,7 +5083,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -5087,7 +5091,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -5095,7 +5099,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5103,7 +5107,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5111,7 +5115,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -5119,7 +5123,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -5127,7 +5131,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -5135,7 +5139,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -5143,7 +5147,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -5151,7 +5155,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -5159,7 +5163,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -5167,7 +5171,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -5175,7 +5179,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -5183,7 +5187,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -5191,7 +5195,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -5199,7 +5203,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5207,7 +5211,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -5215,7 +5219,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -5223,7 +5227,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -5231,7 +5235,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -5239,7 +5243,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -5247,7 +5251,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -5255,7 +5259,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -5263,7 +5267,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -5271,7 +5275,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -5279,7 +5283,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -5287,7 +5291,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -5295,7 +5299,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -5303,7 +5307,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -5311,7 +5315,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -5319,7 +5323,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -5346,15 +5350,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5362,7 +5366,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5370,7 +5374,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5378,7 +5382,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5386,7 +5390,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5394,7 +5398,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5402,7 +5406,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5410,7 +5414,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5418,7 +5422,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5426,7 +5430,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5434,7 +5438,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5442,7 +5446,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5450,7 +5454,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5458,7 +5462,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -5466,7 +5470,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -5474,7 +5478,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -5482,7 +5486,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5490,7 +5494,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -5498,7 +5502,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5506,7 +5510,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -5514,7 +5518,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -5522,7 +5526,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5530,7 +5534,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5538,7 +5542,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -5546,7 +5550,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -5554,7 +5558,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -5562,7 +5566,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -5570,7 +5574,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -5578,7 +5582,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -5586,7 +5590,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -5594,7 +5598,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -5602,7 +5606,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -5610,7 +5614,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -5618,7 +5622,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -5626,7 +5630,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5634,7 +5638,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -5642,7 +5646,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -5650,7 +5654,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -5658,7 +5662,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -5666,7 +5670,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -5674,7 +5678,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -5682,7 +5686,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -5690,7 +5694,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -5698,7 +5702,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -5706,7 +5710,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -5714,7 +5718,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -5722,7 +5726,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -5730,7 +5734,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -5738,7 +5742,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -5746,7 +5750,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -5770,10 +5774,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -5890,10 +5894,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -5973,13 +5977,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -5987,7 +5991,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5998,7 +6002,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -6009,7 +6013,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6020,7 +6024,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -6048,13 +6052,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -6062,7 +6066,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -6073,7 +6077,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -6106,7 +6110,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>50</v>
@@ -6124,10 +6128,10 @@
         <v>52</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -6145,7 +6149,7 @@
         <v>55</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -6158,16 +6162,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>240</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -6233,7 +6237,7 @@
         <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -6334,16 +6338,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>222</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
@@ -6356,16 +6360,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -6387,13 +6391,13 @@
         <v>128</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -6411,10 +6415,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -6433,7 +6437,7 @@
         <v>72</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
@@ -6485,7 +6489,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
@@ -6503,7 +6507,7 @@
         <v>55</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
@@ -6525,7 +6529,7 @@
         <v>63</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -6613,7 +6617,7 @@
         <v>58</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -6732,16 +6736,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" t="s">
         <v>206</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>207</v>
       </c>
-      <c r="C1" t="s">
-        <v>208</v>
-      </c>
       <c r="D1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -6750,10 +6754,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -6765,10 +6769,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -6783,10 +6787,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -6798,10 +6802,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -6813,10 +6817,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -6828,10 +6832,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -6843,10 +6847,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -6858,10 +6862,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -6892,87 +6896,87 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B1" t="s">
         <v>542</v>
-      </c>
-      <c r="B1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B2" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
@@ -6981,7 +6985,7 @@
         <v>一年级</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
@@ -6990,7 +6994,7 @@
         <v>二年级</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
@@ -6999,7 +7003,7 @@
         <v>三年级</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
@@ -7008,7 +7012,7 @@
         <v>四年级</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
@@ -7017,7 +7021,7 @@
         <v>五年级</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
@@ -7026,7 +7030,7 @@
         <v>六年级</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
@@ -7035,7 +7039,7 @@
         <v>七年级</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
@@ -7044,7 +7048,7 @@
         <v>八年级</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
@@ -7053,7 +7057,7 @@
         <v>九年级</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -7066,7 +7070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -7074,170 +7078,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B1" t="s">
         <v>566</v>
-      </c>
-      <c r="B1" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B2" t="s">
         <v>568</v>
-      </c>
-      <c r="B2" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B3" t="s">
         <v>570</v>
-      </c>
-      <c r="B3" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>571</v>
+      </c>
+      <c r="B4" t="s">
         <v>572</v>
-      </c>
-      <c r="B4" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>574</v>
+      </c>
+      <c r="B6" t="s">
         <v>575</v>
-      </c>
-      <c r="B6" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>576</v>
+      </c>
+      <c r="B7" t="s">
         <v>577</v>
-      </c>
-      <c r="B7" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B9" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B10" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>581</v>
+      </c>
+      <c r="B11" t="s">
         <v>582</v>
-      </c>
-      <c r="B11" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>583</v>
+      </c>
+      <c r="B12" t="s">
         <v>584</v>
-      </c>
-      <c r="B12" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B13" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
+        <v>586</v>
+      </c>
+      <c r="B14" t="s">
         <v>587</v>
-      </c>
-      <c r="B14" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B15" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
+        <v>591</v>
+      </c>
+      <c r="B18" t="s">
         <v>592</v>
-      </c>
-      <c r="B18" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B19" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>594</v>
+      </c>
+      <c r="B20" t="s">
         <v>595</v>
-      </c>
-      <c r="B20" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B21" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -7262,15 +7266,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -7278,7 +7282,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7286,7 +7290,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -7294,7 +7298,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -7302,7 +7306,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -7310,7 +7314,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -7337,15 +7341,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7353,7 +7357,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -7361,7 +7365,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -7369,7 +7373,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -7377,7 +7381,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7385,7 +7389,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -7393,7 +7397,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -7401,7 +7405,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -7409,7 +7413,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -7417,7 +7421,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -7425,7 +7429,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -7433,7 +7437,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -7441,7 +7445,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -7449,7 +7453,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -7457,7 +7461,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -7465,7 +7469,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -7473,7 +7477,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -7481,7 +7485,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -7489,7 +7493,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -7497,7 +7501,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -7505,7 +7509,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -7513,7 +7517,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -7521,7 +7525,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -7529,7 +7533,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -7537,7 +7541,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -7545,7 +7549,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -7553,7 +7557,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -7561,7 +7565,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -7569,7 +7573,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -7577,7 +7581,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -7585,7 +7589,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -7593,7 +7597,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -7601,7 +7605,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -7609,7 +7613,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -7617,7 +7621,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -7625,7 +7629,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -7633,7 +7637,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -7641,7 +7645,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -7649,7 +7653,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -7657,7 +7661,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -7665,7 +7669,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -7673,7 +7677,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -7681,7 +7685,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -7689,7 +7693,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -7697,7 +7701,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -7705,7 +7709,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -7713,7 +7717,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -7721,7 +7725,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -7729,7 +7733,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -7737,7 +7741,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -7764,15 +7768,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7780,7 +7784,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -7788,7 +7792,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -7796,7 +7800,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -7804,7 +7808,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7812,7 +7816,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -7820,7 +7824,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -7828,7 +7832,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -7836,7 +7840,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -7844,7 +7848,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -7852,7 +7856,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -7860,7 +7864,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -7868,7 +7872,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -7876,7 +7880,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -7884,7 +7888,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -7892,7 +7896,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -7900,7 +7904,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -7908,7 +7912,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -7916,7 +7920,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -7924,7 +7928,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -7932,7 +7936,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -7940,7 +7944,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -7948,7 +7952,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -7956,7 +7960,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -7964,7 +7968,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -7972,7 +7976,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -7980,7 +7984,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -7988,7 +7992,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -7996,7 +8000,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -8004,7 +8008,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8012,7 +8016,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -8020,7 +8024,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -8028,7 +8032,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -8036,7 +8040,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -8044,7 +8048,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -8052,7 +8056,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -8060,7 +8064,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -8068,7 +8072,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -8076,7 +8080,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -8084,7 +8088,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -8092,7 +8096,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -8100,7 +8104,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -8108,7 +8112,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -8116,7 +8120,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -8124,7 +8128,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -8132,7 +8136,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -8140,7 +8144,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -8148,7 +8152,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -8156,7 +8160,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -8164,7 +8168,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -8192,15 +8196,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -8208,7 +8212,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8216,7 +8220,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -8224,7 +8228,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -8232,7 +8236,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8240,7 +8244,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -8248,7 +8252,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -8256,7 +8260,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -8264,7 +8268,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -8272,7 +8276,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -8280,7 +8284,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -8288,7 +8292,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -8296,7 +8300,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -8304,7 +8308,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -8312,7 +8316,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -8320,7 +8324,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -8328,7 +8332,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -8336,7 +8340,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -8344,7 +8348,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -8352,7 +8356,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -8360,7 +8364,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -8368,7 +8372,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -8376,7 +8380,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -8384,7 +8388,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -8392,7 +8396,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -8400,7 +8404,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -8408,7 +8412,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -8416,7 +8420,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -8424,7 +8428,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -8432,7 +8436,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8440,7 +8444,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -8448,7 +8452,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -8456,7 +8460,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -8464,7 +8468,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -8472,7 +8476,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -8480,7 +8484,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -8488,7 +8492,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -8496,7 +8500,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -8504,7 +8508,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -8512,7 +8516,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -8520,7 +8524,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -8528,7 +8532,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -8536,7 +8540,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -8544,7 +8548,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -8552,7 +8556,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -8560,7 +8564,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -8568,7 +8572,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -8576,7 +8580,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -8584,7 +8588,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -8592,7 +8596,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B51">
         <v>1</v>

</xml_diff>

<commit_message>
Bug fixes and add the analysis of math tasks.
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="604">
   <si>
     <t>符号判断</t>
   </si>
@@ -2156,10 +2156,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CountTotalTrl CountAccTrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CountAccTrl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2342,6 +2338,30 @@
   </si>
   <si>
     <t>RUN S1 S2 CResp NL NR Resp ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTotalTrl CountAccTrl TotalScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mentcompare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>distances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4 D5 D6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4 D5 D6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2812,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A11:XFD12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2848,13 +2868,13 @@
         <v>157</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>238</v>
@@ -2903,7 +2923,7 @@
         <v>216</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>167</v>
@@ -2916,7 +2936,7 @@
         <v>170</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>190</v>
@@ -2947,7 +2967,7 @@
         <v>216</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>167</v>
@@ -2960,7 +2980,7 @@
         <v>170</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>190</v>
@@ -2991,7 +3011,7 @@
         <v>216</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>167</v>
@@ -3004,7 +3024,7 @@
         <v>170</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>190</v>
@@ -3035,7 +3055,7 @@
         <v>216</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>167</v>
@@ -3048,7 +3068,7 @@
         <v>170</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>190</v>
@@ -3079,7 +3099,7 @@
         <v>216</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>167</v>
@@ -3092,7 +3112,7 @@
         <v>170</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>190</v>
@@ -3123,7 +3143,7 @@
         <v>216</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>167</v>
@@ -3136,7 +3156,7 @@
         <v>170</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>190</v>
@@ -3165,17 +3185,17 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" t="s">
+        <v>598</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>543</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>544</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -3202,23 +3222,23 @@
         <v>3000</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>175</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>198</v>
       </c>
       <c r="L9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>193</v>
@@ -3248,23 +3268,23 @@
         <v>3000</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>175</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>198</v>
       </c>
       <c r="L10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>193</v>
@@ -3294,20 +3314,25 @@
         <v>2000</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>558</v>
+        <v>599</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="I11" s="8"/>
+        <v>603</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>601</v>
+      </c>
       <c r="J11" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>198</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>600</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>193</v>
@@ -3328,7 +3353,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>141</v>
@@ -3337,17 +3362,19 @@
         <v>3000</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>558</v>
+        <v>599</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="8" t="s">
+        <v>602</v>
+      </c>
       <c r="J12" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>198</v>
@@ -3383,7 +3410,7 @@
         <v>187</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>179</v>
@@ -3424,7 +3451,7 @@
         <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>171</v>
@@ -3465,7 +3492,7 @@
         <v>48</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>171</v>
@@ -3506,7 +3533,7 @@
         <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>171</v>
@@ -3547,7 +3574,7 @@
         <v>48</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>171</v>
@@ -3588,7 +3615,7 @@
         <v>500</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>167</v>
@@ -3631,7 +3658,7 @@
         <v>500</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>167</v>
@@ -3674,7 +3701,7 @@
         <v>500</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>167</v>
@@ -3717,7 +3744,7 @@
         <v>500</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>167</v>
@@ -3757,10 +3784,10 @@
         <v>3000</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>171</v>
@@ -3800,10 +3827,10 @@
         <v>3000</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>171</v>
@@ -3843,10 +3870,10 @@
         <v>3000</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>171</v>
@@ -3889,7 +3916,7 @@
         <v>48</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>171</v>
@@ -3930,7 +3957,7 @@
         <v>48</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>171</v>
@@ -3969,7 +3996,7 @@
         <v>184</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>176</v>
@@ -4008,7 +4035,7 @@
         <v>216</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>167</v>
@@ -4051,7 +4078,7 @@
         <v>216</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>510</v>
@@ -4094,7 +4121,7 @@
         <v>507</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>167</v>
@@ -4140,7 +4167,7 @@
         <v>507</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>167</v>
@@ -4186,7 +4213,7 @@
         <v>495</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>167</v>
@@ -4229,7 +4256,7 @@
         <v>496</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>167</v>
@@ -4272,7 +4299,7 @@
         <v>187</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>179</v>
@@ -4313,7 +4340,7 @@
         <v>187</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>179</v>
@@ -4352,7 +4379,7 @@
         <v>187</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>179</v>
@@ -4393,7 +4420,7 @@
         <v>187</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>179</v>
@@ -4431,13 +4458,13 @@
         <v>2000</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -4470,13 +4497,13 @@
         <v>2000</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -4510,7 +4537,7 @@
         <v>165</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>176</v>
@@ -4547,7 +4574,7 @@
         <v>165</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>176</v>
@@ -4584,7 +4611,7 @@
         <v>165</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>176</v>
@@ -4623,7 +4650,7 @@
         <v>185</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>189</v>
@@ -4664,7 +4691,7 @@
         <v>186</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>177</v>
@@ -4705,7 +4732,7 @@
         <v>186</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>181</v>
@@ -4746,7 +4773,7 @@
         <v>185</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>178</v>
@@ -4783,7 +4810,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -4808,7 +4835,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -4835,7 +4862,7 @@
         <v>49</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>180</v>
@@ -6096,7 +6123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -6113,7 +6140,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>50</v>
@@ -6240,7 +6267,7 @@
         <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -6262,7 +6289,7 @@
         <v>63</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -6284,7 +6311,7 @@
         <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -6306,7 +6333,7 @@
         <v>61</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -6400,7 +6427,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -6492,7 +6519,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
@@ -6532,7 +6559,7 @@
         <v>63</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -6620,7 +6647,7 @@
         <v>58</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -6748,7 +6775,7 @@
         <v>204</v>
       </c>
       <c r="D1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -7081,170 +7108,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B1" t="s">
         <v>562</v>
-      </c>
-      <c r="B1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B2" t="s">
         <v>564</v>
-      </c>
-      <c r="B2" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>565</v>
+      </c>
+      <c r="B3" t="s">
         <v>566</v>
-      </c>
-      <c r="B3" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>567</v>
+      </c>
+      <c r="B4" t="s">
         <v>568</v>
-      </c>
-      <c r="B4" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>570</v>
+      </c>
+      <c r="B6" t="s">
         <v>571</v>
-      </c>
-      <c r="B6" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>572</v>
+      </c>
+      <c r="B7" t="s">
         <v>573</v>
-      </c>
-      <c r="B7" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B9" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B10" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>577</v>
+      </c>
+      <c r="B11" t="s">
         <v>578</v>
-      </c>
-      <c r="B11" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>579</v>
+      </c>
+      <c r="B12" t="s">
         <v>580</v>
-      </c>
-      <c r="B12" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B13" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
+        <v>582</v>
+      </c>
+      <c r="B14" t="s">
         <v>583</v>
-      </c>
-      <c r="B14" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B15" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B16" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
+        <v>587</v>
+      </c>
+      <c r="B18" t="s">
         <v>588</v>
-      </c>
-      <c r="B18" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>590</v>
+      </c>
+      <c r="B20" t="s">
         <v>591</v>
-      </c>
-      <c r="B20" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B21" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move analysis files to utilis folder.
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="620">
   <si>
     <t>符号判断</t>
   </si>
@@ -2341,18 +2341,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CountTotalTrl CountAccTrl TotalScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mentcompare</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>distances</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>D1 D2 D3 D4 D5 D6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2362,6 +2354,78 @@
   </si>
   <si>
     <t>RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UltimateIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTotalTrl CountAccTrl TotalScore MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CongEffectUnion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SwitchCostUnion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CongEffectUnion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scoring</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2369,7 +2433,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2478,6 +2542,30 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2501,7 +2589,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2548,6 +2636,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2830,10 +2930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2851,10 +2951,11 @@
     <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.75" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.5" customWidth="1"/>
+    <col min="16" max="17" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2895,16 +2996,22 @@
         <v>513</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -2938,17 +3045,20 @@
       <c r="L2" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" t="s">
+        <v>603</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2982,17 +3092,20 @@
       <c r="L3" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" t="s">
+        <v>603</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3026,17 +3139,20 @@
       <c r="L4" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" t="s">
+        <v>603</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3070,17 +3186,20 @@
       <c r="L5" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" t="s">
+        <v>603</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3114,17 +3233,20 @@
       <c r="L6" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" t="s">
+        <v>603</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3158,17 +3280,20 @@
       <c r="L7" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" t="s">
+        <v>603</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3192,19 +3317,22 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" t="s">
-        <v>598</v>
-      </c>
-      <c r="N8" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="N8" t="s">
+        <v>603</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3240,17 +3368,20 @@
       <c r="L9" t="s">
         <v>544</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="N9" t="s">
+        <v>603</v>
+      </c>
+      <c r="P9" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="O9">
-        <v>2</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3286,17 +3417,20 @@
       <c r="L10" t="s">
         <v>544</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" t="s">
+        <v>610</v>
+      </c>
+      <c r="P10" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="O10">
-        <v>2</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="R10" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3314,16 +3448,16 @@
         <v>2000</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>550</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>546</v>
@@ -3331,20 +3465,18 @@
       <c r="K11" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>600</v>
-      </c>
-      <c r="N11" s="8" t="s">
+      <c r="L11" s="8"/>
+      <c r="P11" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="O11">
-        <v>2</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3362,7 +3494,7 @@
         <v>3000</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>550</v>
@@ -3371,7 +3503,7 @@
         <v>175</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>546</v>
@@ -3379,17 +3511,17 @@
       <c r="K12" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="P12" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="O12">
-        <v>2</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3420,17 +3552,20 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="N13" s="2" t="s">
+      <c r="L13" s="18" t="s">
+        <v>618</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="O13">
-        <v>2</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3461,17 +3596,21 @@
         <v>173</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="N14" s="2" t="s">
+      <c r="L14" s="19"/>
+      <c r="N14" t="s">
+        <v>606</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>3</v>
       </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3502,17 +3641,21 @@
         <v>173</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="N15" s="2" t="s">
+      <c r="L15" s="19"/>
+      <c r="N15" t="s">
+        <v>606</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>3</v>
       </c>
-      <c r="P15" t="s">
+      <c r="R15" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3543,17 +3686,21 @@
         <v>173</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="N16" s="2" t="s">
+      <c r="L16" s="19"/>
+      <c r="N16" t="s">
+        <v>606</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>3</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3584,17 +3731,21 @@
         <v>497</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="N17" s="2" t="s">
+      <c r="L17" s="19"/>
+      <c r="N17" t="s">
+        <v>606</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>3</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3627,17 +3778,21 @@
       <c r="K18" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="L18" s="19"/>
+      <c r="N18" t="s">
+        <v>607</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>3</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3670,17 +3825,21 @@
       <c r="K19" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="L19" s="19"/>
+      <c r="N19" t="s">
+        <v>607</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>3</v>
       </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3713,17 +3872,21 @@
       <c r="K20" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="L20" s="19"/>
+      <c r="N20" t="s">
+        <v>607</v>
+      </c>
+      <c r="P20" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>3</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3756,17 +3919,21 @@
       <c r="K21" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="L21" s="19"/>
+      <c r="N21" t="s">
+        <v>607</v>
+      </c>
+      <c r="P21" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>3</v>
       </c>
-      <c r="P21" t="s">
+      <c r="R21" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3799,17 +3966,18 @@
       <c r="K22" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="L22" s="19"/>
+      <c r="P22" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>3</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3842,17 +4010,18 @@
       <c r="K23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="L23" s="19"/>
+      <c r="P23" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="O23">
+      <c r="Q23">
         <v>3</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3885,17 +4054,18 @@
       <c r="K24" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="L24" s="19"/>
+      <c r="P24" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <v>3</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3926,17 +4096,21 @@
         <v>173</v>
       </c>
       <c r="K25" s="2"/>
-      <c r="N25" s="2" t="s">
+      <c r="L25" s="19"/>
+      <c r="N25" t="s">
+        <v>606</v>
+      </c>
+      <c r="P25" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="O25">
+      <c r="Q25">
         <v>3</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3967,17 +4141,21 @@
         <v>173</v>
       </c>
       <c r="K26" s="2"/>
-      <c r="N26" s="2" t="s">
+      <c r="L26" s="19"/>
+      <c r="N26" t="s">
+        <v>606</v>
+      </c>
+      <c r="P26" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="O26">
+      <c r="Q26">
         <v>3</v>
       </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4004,17 +4182,21 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="N27" s="2" t="s">
+      <c r="L27" s="19"/>
+      <c r="N27" t="s">
+        <v>608</v>
+      </c>
+      <c r="P27" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="O27">
+      <c r="Q27">
         <v>4</v>
       </c>
-      <c r="P27" t="s">
+      <c r="R27" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4047,22 +4229,26 @@
       <c r="K28" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="L28" s="19"/>
+      <c r="N28" t="s">
+        <v>607</v>
+      </c>
+      <c r="P28" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <v>4</v>
       </c>
-      <c r="P28" t="s">
+      <c r="R28" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="16" t="s">
         <v>161</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -4089,18 +4275,25 @@
       <c r="J29" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="K29" s="2"/>
-      <c r="N29" s="2" t="s">
+      <c r="K29" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="L29" s="19"/>
+      <c r="N29" s="19" t="s">
+        <v>609</v>
+      </c>
+      <c r="O29" s="19"/>
+      <c r="P29" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <v>4</v>
       </c>
-      <c r="P29" t="s">
+      <c r="R29" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4133,20 +4326,25 @@
       <c r="K30" s="2" t="s">
         <v>170</v>
       </c>
+      <c r="L30" s="19"/>
       <c r="M30" t="s">
         <v>514</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="N30" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="O30" s="17"/>
+      <c r="P30" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O30">
+      <c r="Q30">
         <v>4</v>
       </c>
-      <c r="P30" t="s">
+      <c r="R30" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4179,20 +4377,25 @@
       <c r="K31" s="2" t="s">
         <v>515</v>
       </c>
+      <c r="L31" s="19"/>
       <c r="M31" t="s">
         <v>514</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="N31" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="O31" s="17"/>
+      <c r="P31" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O31">
+      <c r="Q31">
         <v>4</v>
       </c>
-      <c r="P31" t="s">
+      <c r="R31" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4225,17 +4428,22 @@
       <c r="K32" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N32" s="2" t="s">
+      <c r="L32" s="19"/>
+      <c r="N32" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="O32" s="17"/>
+      <c r="P32" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>5</v>
       </c>
-      <c r="P32" t="s">
+      <c r="R32" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4268,17 +4476,22 @@
       <c r="K33" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N33" s="2" t="s">
+      <c r="L33" s="19"/>
+      <c r="N33" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="O33" s="17"/>
+      <c r="P33" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O33">
+      <c r="Q33">
         <v>5</v>
       </c>
-      <c r="P33" t="s">
+      <c r="R33" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <f t="shared" ref="A34:A51" si="1">ROW() - 1</f>
         <v>33</v>
@@ -4309,17 +4522,20 @@
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="N34" s="2" t="s">
+      <c r="L34" s="18" t="s">
+        <v>605</v>
+      </c>
+      <c r="P34" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="O34">
+      <c r="Q34">
         <v>5</v>
       </c>
-      <c r="P34" t="s">
+      <c r="R34" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -4350,17 +4566,20 @@
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="N35" s="2" t="s">
+      <c r="L35" s="18" t="s">
+        <v>605</v>
+      </c>
+      <c r="P35" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="O35">
+      <c r="Q35">
         <v>5</v>
       </c>
-      <c r="P35" t="s">
+      <c r="R35" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -4389,22 +4608,25 @@
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="N36" s="2" t="s">
+      <c r="L36" s="18" t="s">
+        <v>605</v>
+      </c>
+      <c r="P36" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="O36">
+      <c r="Q36">
         <v>5</v>
       </c>
-      <c r="P36" t="s">
+      <c r="R36" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C37" s="13" t="s">
@@ -4430,17 +4652,20 @@
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="N37" s="2" t="s">
+      <c r="L37" s="18" t="s">
+        <v>617</v>
+      </c>
+      <c r="P37" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="O37">
+      <c r="Q37">
         <v>5</v>
       </c>
-      <c r="P37" t="s">
+      <c r="R37" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -4469,17 +4694,20 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="N38" s="2" t="s">
+      <c r="N38" t="s">
+        <v>611</v>
+      </c>
+      <c r="P38" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O38">
+      <c r="Q38">
         <v>5</v>
       </c>
-      <c r="P38" t="s">
+      <c r="R38" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -4508,17 +4736,20 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="N39" s="2" t="s">
+      <c r="N39" t="s">
+        <v>612</v>
+      </c>
+      <c r="P39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O39">
+      <c r="Q39">
         <v>5</v>
       </c>
-      <c r="P39" t="s">
+      <c r="R39" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -4545,17 +4776,20 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="N40" s="2" t="s">
+      <c r="N40" t="s">
+        <v>613</v>
+      </c>
+      <c r="P40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="O40">
+      <c r="Q40">
         <v>6</v>
       </c>
-      <c r="P40" t="s">
+      <c r="R40" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -4582,17 +4816,20 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="N41" s="2" t="s">
+      <c r="N41" t="s">
+        <v>614</v>
+      </c>
+      <c r="P41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="O41">
+      <c r="Q41">
         <v>6</v>
       </c>
-      <c r="P41" t="s">
+      <c r="R41" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -4619,17 +4856,20 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="N42" s="2" t="s">
+      <c r="N42" t="s">
+        <v>615</v>
+      </c>
+      <c r="P42" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="O42">
+      <c r="Q42">
         <v>6</v>
       </c>
-      <c r="P42" t="s">
+      <c r="R42" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -4660,17 +4900,20 @@
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="N43" s="2" t="s">
+      <c r="N43" t="s">
+        <v>616</v>
+      </c>
+      <c r="P43" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="O43">
+      <c r="Q43">
         <v>6</v>
       </c>
-      <c r="P43" t="s">
+      <c r="R43" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -4701,17 +4944,17 @@
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="N44" s="2" t="s">
+      <c r="P44" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="O44">
+      <c r="Q44">
         <v>6</v>
       </c>
-      <c r="P44" t="s">
+      <c r="R44" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -4742,17 +4985,17 @@
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="N45" s="2" t="s">
+      <c r="P45" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="O45">
+      <c r="Q45">
         <v>6</v>
       </c>
-      <c r="P45" t="s">
+      <c r="R45" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -4783,17 +5026,17 @@
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="N46" s="2" t="s">
+      <c r="P46" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="O46">
+      <c r="Q46">
         <v>6</v>
       </c>
-      <c r="P46" t="s">
+      <c r="R46" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -4816,9 +5059,9 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="N47" s="2"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P47" s="2"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -4841,14 +5084,14 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="N48" s="2"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -4870,11 +5113,11 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="N49" s="2" t="s">
+      <c r="P49" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -4895,9 +5138,9 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="N50" s="2"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="P50" s="2"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -4918,11 +5161,11 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="N51" s="2"/>
+      <c r="P51" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:R51">
-    <sortCondition ref="O2:O51"/>
+  <sortState ref="A2:T51">
+    <sortCondition ref="Q2:Q51"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}" topLeftCell="A11">

</xml_diff>

<commit_message>
Initially completed the task.
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="662">
   <si>
     <t>符号判断</t>
   </si>
@@ -2167,10 +2167,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VRT Ter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Subitizing</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2345,11 +2341,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D1 D2 D3 D4 D5 D6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D1 D2 D3 D4 D5 D6</t>
+    <t>UltimateIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTotalTrl CountAccTrl TotalScore MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lang</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2357,75 +2401,198 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UltimateIndex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CountTotalTrl CountAccTrl TotalScore MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CongEffectUnion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SwitchCostUnion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CongEffectUnion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scoring</t>
+    <t>Conflict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Span</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GNG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GNG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GNG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Span</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScoringPara</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3001 3000 3000</t>
+  </si>
+  <si>
+    <t>ScoringVars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotalTime TotalScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall D1 D2 D3 D4 D5 D6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_Overall ACC_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_Overall ACC_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall D1 D2 D3 D4 D5 D8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_Overall ACC_Overall RT_CongEffect ACC_CongEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2500 2000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2800 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3200 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit Rate_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit Rate_hit Count_FA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScoringFun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit Rate_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500 1500 1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500 1500 1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_Overall ACC_Overall RT_SwitchCost ACC_SwitchCost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLACC MLNextACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ML MLACC MLNextACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC_R1 ACC_R2 RT_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>150 100 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1_hitRate R2_hitRate MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 40 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 35 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 35 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ConflictUnion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ConflictUnion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprimeTM dprimeFM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprimeTM dprimeFM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprimeFM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2575,10 +2742,30 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -2589,7 +2776,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2648,6 +2835,48 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2930,10 +3159,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2943,19 +3176,22 @@
     <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.75" customWidth="1"/>
-    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.75" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.25" customWidth="1"/>
     <col min="10" max="10" width="14.75" customWidth="1"/>
     <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.75" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.5" customWidth="1"/>
-    <col min="16" max="17" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="21" customWidth="1"/>
+    <col min="16" max="16" width="57.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2969,15 +3205,15 @@
         <v>157</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="20" t="s">
         <v>238</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -2995,23 +3231,29 @@
       <c r="M1" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>619</v>
+      <c r="N1" s="23" t="s">
+        <v>598</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>642</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -3026,13 +3268,13 @@
         <v>143</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="20" t="s">
         <v>216</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H2" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -3045,20 +3287,26 @@
       <c r="L2" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N2" t="s">
-        <v>603</v>
-      </c>
-      <c r="P2" s="2" t="s">
+      <c r="N2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>611</v>
+      </c>
+      <c r="P2" t="s">
+        <v>627</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3073,13 +3321,13 @@
         <v>143</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="20" t="s">
         <v>216</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H3" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -3092,20 +3340,26 @@
       <c r="L3" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N3" t="s">
-        <v>603</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="N3" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>611</v>
+      </c>
+      <c r="P3" t="s">
+        <v>627</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3120,13 +3374,13 @@
         <v>143</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="20" t="s">
         <v>216</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H4" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -3139,20 +3393,26 @@
       <c r="L4" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N4" t="s">
-        <v>603</v>
-      </c>
-      <c r="P4" s="2" t="s">
+      <c r="N4" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>611</v>
+      </c>
+      <c r="P4" t="s">
+        <v>627</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3167,13 +3427,13 @@
         <v>143</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="20" t="s">
         <v>216</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H5" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -3186,20 +3446,26 @@
       <c r="L5" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N5" t="s">
-        <v>603</v>
-      </c>
-      <c r="P5" s="2" t="s">
+      <c r="N5" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>611</v>
+      </c>
+      <c r="P5" t="s">
+        <v>627</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3214,13 +3480,13 @@
         <v>143</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="20" t="s">
         <v>216</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H6" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -3233,20 +3499,26 @@
       <c r="L6" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N6" t="s">
-        <v>603</v>
-      </c>
-      <c r="P6" s="2" t="s">
+      <c r="N6" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>611</v>
+      </c>
+      <c r="P6" t="s">
+        <v>627</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3261,13 +3533,13 @@
         <v>143</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="20" t="s">
         <v>216</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H7" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -3280,20 +3552,26 @@
       <c r="L7" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N7" t="s">
-        <v>603</v>
-      </c>
-      <c r="P7" s="2" t="s">
+      <c r="N7" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>611</v>
+      </c>
+      <c r="P7" t="s">
+        <v>627</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3308,31 +3586,31 @@
         <v>237</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>549</v>
+      </c>
+      <c r="H8" s="20"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" t="s">
-        <v>604</v>
-      </c>
-      <c r="N8" t="s">
-        <v>603</v>
-      </c>
-      <c r="P8" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3349,39 +3627,44 @@
       <c r="E9" s="7">
         <v>3000</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>557</v>
+      <c r="F9" s="29" t="s">
+        <v>556</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H9" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="H9" s="27" t="s">
         <v>175</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="J9" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>198</v>
-      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
       <c r="L9" t="s">
         <v>544</v>
       </c>
-      <c r="N9" t="s">
-        <v>603</v>
-      </c>
-      <c r="P9" s="8" t="s">
+      <c r="N9" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="P9" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>624</v>
+      </c>
+      <c r="R9" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="Q9">
-        <v>2</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3398,39 +3681,44 @@
       <c r="E10" s="7">
         <v>3000</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>557</v>
+      <c r="F10" s="27" t="s">
+        <v>556</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H10" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>175</v>
       </c>
       <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>198</v>
-      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
       <c r="L10" t="s">
         <v>544</v>
       </c>
-      <c r="N10" t="s">
-        <v>610</v>
-      </c>
-      <c r="P10" s="8" t="s">
+      <c r="N10" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="P10" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>624</v>
+      </c>
+      <c r="R10" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="Q10">
-        <v>2</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3447,36 +3735,41 @@
       <c r="E11" s="8">
         <v>2000</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>598</v>
+      <c r="F11" s="27" t="s">
+        <v>597</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>601</v>
+        <v>549</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>630</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>599</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>198</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="P11" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q11">
-        <v>2</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="O11" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="P11" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>624</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3485,7 +3778,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>141</v>
@@ -3493,35 +3786,40 @@
       <c r="E12" s="8">
         <v>3000</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>598</v>
+      <c r="F12" s="27" t="s">
+        <v>597</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>175</v>
+        <v>549</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>178</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>600</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q12">
-        <v>2</v>
-      </c>
-      <c r="R12" t="s">
+        <v>633</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="O12" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="P12" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>625</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3538,13 +3836,13 @@
       <c r="E13" s="10">
         <v>2000</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="20" t="s">
         <v>187</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H13" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H13" s="28" t="s">
         <v>179</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -3552,20 +3850,30 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="18" t="s">
-        <v>618</v>
-      </c>
-      <c r="P13" s="2" t="s">
+      <c r="L13" s="18"/>
+      <c r="N13" s="31" t="s">
+        <v>656</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>613</v>
+      </c>
+      <c r="P13" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q13">
+        <v>3000</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="Q13">
-        <v>2</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="S13">
+        <v>2</v>
+      </c>
+      <c r="T13" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3582,13 +3890,13 @@
       <c r="E14" s="2">
         <v>3000</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="20" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H14" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I14" s="2"/>
@@ -3597,20 +3905,29 @@
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="19"/>
-      <c r="N14" t="s">
-        <v>606</v>
-      </c>
-      <c r="P14" s="2" t="s">
+      <c r="N14" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P14" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>636</v>
+      </c>
+      <c r="R14" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>3</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3627,13 +3944,13 @@
       <c r="E15" s="2">
         <v>3000</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="20" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H15" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I15" s="2"/>
@@ -3642,20 +3959,29 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="19"/>
-      <c r="N15" t="s">
-        <v>606</v>
-      </c>
-      <c r="P15" s="2" t="s">
+      <c r="N15" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="O15" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P15" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>636</v>
+      </c>
+      <c r="R15" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>3</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3672,13 +3998,13 @@
       <c r="E16" s="2">
         <v>3000</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="20" t="s">
         <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H16" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I16" s="2"/>
@@ -3687,20 +4013,29 @@
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="19"/>
-      <c r="N16" t="s">
-        <v>606</v>
-      </c>
-      <c r="P16" s="2" t="s">
+      <c r="N16" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P16" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>636</v>
+      </c>
+      <c r="R16" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>3</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3717,13 +4052,13 @@
       <c r="E17" s="2">
         <v>3000</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="20" t="s">
         <v>48</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H17" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I17" s="2"/>
@@ -3732,20 +4067,29 @@
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="19"/>
-      <c r="N17" t="s">
-        <v>606</v>
-      </c>
-      <c r="P17" s="2" t="s">
+      <c r="N17" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="O17" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P17" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>636</v>
+      </c>
+      <c r="R17" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>3</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3762,13 +4106,13 @@
       <c r="E18" s="2">
         <v>3000</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="20" t="s">
         <v>500</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H18" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H18" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I18" s="2" t="s">
@@ -3779,20 +4123,29 @@
         <v>170</v>
       </c>
       <c r="L18" s="19"/>
-      <c r="N18" t="s">
-        <v>607</v>
-      </c>
-      <c r="P18" s="2" t="s">
+      <c r="N18" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="O18" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P18" s="32" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q18" s="33" t="s">
+        <v>637</v>
+      </c>
+      <c r="R18" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>3</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3809,13 +4162,13 @@
       <c r="E19" s="2">
         <v>3000</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="20" t="s">
         <v>500</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H19" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H19" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -3826,20 +4179,29 @@
         <v>170</v>
       </c>
       <c r="L19" s="19"/>
-      <c r="N19" t="s">
-        <v>607</v>
-      </c>
-      <c r="P19" s="2" t="s">
+      <c r="N19" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="O19" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P19" s="32" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q19" s="33" t="s">
+        <v>637</v>
+      </c>
+      <c r="R19" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>3</v>
       </c>
-      <c r="R19" t="s">
+      <c r="T19" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3856,13 +4218,13 @@
       <c r="E20" s="2">
         <v>3000</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="20" t="s">
         <v>500</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H20" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H20" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I20" s="2" t="s">
@@ -3873,20 +4235,29 @@
         <v>170</v>
       </c>
       <c r="L20" s="19"/>
-      <c r="N20" t="s">
-        <v>607</v>
-      </c>
-      <c r="P20" s="2" t="s">
+      <c r="N20" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="O20" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P20" s="32" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q20" s="33" t="s">
+        <v>637</v>
+      </c>
+      <c r="R20" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <v>3</v>
       </c>
-      <c r="R20" t="s">
+      <c r="T20" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3903,13 +4274,13 @@
       <c r="E21" s="2">
         <v>3000</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="20" t="s">
         <v>500</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H21" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H21" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -3920,20 +4291,29 @@
         <v>170</v>
       </c>
       <c r="L21" s="19"/>
-      <c r="N21" t="s">
-        <v>607</v>
-      </c>
-      <c r="P21" s="2" t="s">
+      <c r="N21" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="O21" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P21" s="32" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q21" s="33" t="s">
+        <v>637</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>3</v>
       </c>
-      <c r="R21" t="s">
+      <c r="T21" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3950,13 +4330,13 @@
       <c r="E22" s="2">
         <v>3000</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>557</v>
+      <c r="F22" s="20" t="s">
+        <v>556</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H22" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H22" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I22" s="2"/>
@@ -3967,17 +4347,26 @@
         <v>198</v>
       </c>
       <c r="L22" s="19"/>
-      <c r="P22" s="2" t="s">
+      <c r="O22" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P22" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>638</v>
+      </c>
+      <c r="R22" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>3</v>
       </c>
-      <c r="R22" t="s">
+      <c r="T22" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3994,13 +4383,13 @@
       <c r="E23" s="2">
         <v>3000</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>557</v>
+      <c r="F23" s="20" t="s">
+        <v>556</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H23" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H23" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I23" s="2"/>
@@ -4011,17 +4400,26 @@
         <v>198</v>
       </c>
       <c r="L23" s="19"/>
-      <c r="P23" s="2" t="s">
+      <c r="O23" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P23" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>638</v>
+      </c>
+      <c r="R23" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <v>3</v>
       </c>
-      <c r="R23" t="s">
+      <c r="T23" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4038,13 +4436,13 @@
       <c r="E24" s="2">
         <v>3000</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>557</v>
+      <c r="F24" s="20" t="s">
+        <v>556</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H24" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H24" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I24" s="2"/>
@@ -4055,17 +4453,26 @@
         <v>198</v>
       </c>
       <c r="L24" s="19"/>
-      <c r="P24" s="2" t="s">
+      <c r="O24" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P24" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>638</v>
+      </c>
+      <c r="R24" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="Q24">
+      <c r="S24">
         <v>3</v>
       </c>
-      <c r="R24" t="s">
+      <c r="T24" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4082,13 +4489,13 @@
       <c r="E25" s="2">
         <v>3000</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="20" t="s">
         <v>48</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H25" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H25" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I25" s="2"/>
@@ -4097,20 +4504,29 @@
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="19"/>
-      <c r="N25" t="s">
-        <v>606</v>
-      </c>
-      <c r="P25" s="2" t="s">
+      <c r="N25" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="O25" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P25" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>639</v>
+      </c>
+      <c r="R25" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <v>3</v>
       </c>
-      <c r="R25" t="s">
+      <c r="T25" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4127,13 +4543,13 @@
       <c r="E26" s="2">
         <v>1000</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="20" t="s">
         <v>48</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H26" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H26" s="20" t="s">
         <v>171</v>
       </c>
       <c r="I26" s="2"/>
@@ -4142,20 +4558,29 @@
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="19"/>
-      <c r="N26" t="s">
-        <v>606</v>
-      </c>
-      <c r="P26" s="2" t="s">
+      <c r="N26" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="O26" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="P26" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>624</v>
+      </c>
+      <c r="R26" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="Q26">
+      <c r="S26">
         <v>3</v>
       </c>
-      <c r="R26" t="s">
+      <c r="T26" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4170,33 +4595,44 @@
         <v>142</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="20" t="s">
         <v>184</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H27" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H27" s="28" t="s">
         <v>176</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="K27" s="5" t="s">
+        <v>648</v>
+      </c>
       <c r="L27" s="19"/>
-      <c r="N27" t="s">
-        <v>608</v>
-      </c>
-      <c r="P27" s="2" t="s">
+      <c r="N27" s="24" t="s">
+        <v>603</v>
+      </c>
+      <c r="O27" s="21" t="s">
+        <v>615</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="Q27">
+        <v>600</v>
+      </c>
+      <c r="R27" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="Q27">
+      <c r="S27">
         <v>4</v>
       </c>
-      <c r="R27" t="s">
+      <c r="T27" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4213,13 +4649,13 @@
       <c r="E28" s="5">
         <v>1000</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="20" t="s">
         <v>216</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H28" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H28" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I28" s="2" t="s">
@@ -4230,20 +4666,26 @@
         <v>170</v>
       </c>
       <c r="L28" s="19"/>
-      <c r="N28" t="s">
-        <v>607</v>
-      </c>
-      <c r="P28" s="2" t="s">
+      <c r="N28" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="O28" s="21" t="s">
+        <v>616</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="R28" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q28">
+      <c r="S28">
         <v>4</v>
       </c>
-      <c r="R28" t="s">
+      <c r="T28" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4260,13 +4702,13 @@
       <c r="E29" s="5">
         <v>500</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="20" t="s">
         <v>216</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H29" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H29" s="20" t="s">
         <v>510</v>
       </c>
       <c r="I29" s="2" t="s">
@@ -4279,21 +4721,26 @@
         <v>170</v>
       </c>
       <c r="L29" s="19"/>
-      <c r="N29" s="19" t="s">
-        <v>609</v>
-      </c>
-      <c r="O29" s="19"/>
-      <c r="P29" s="2" t="s">
+      <c r="N29" s="25" t="s">
+        <v>604</v>
+      </c>
+      <c r="O29" s="21" t="s">
+        <v>616</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="R29" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="Q29">
+      <c r="S29">
         <v>4</v>
       </c>
-      <c r="R29" t="s">
+      <c r="T29" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4310,13 +4757,13 @@
       <c r="E30" s="5">
         <v>1000</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="20" t="s">
         <v>507</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="H30" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="H30" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I30" s="2" t="s">
@@ -4330,21 +4777,29 @@
       <c r="M30" t="s">
         <v>514</v>
       </c>
-      <c r="N30" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="O30" s="17"/>
-      <c r="P30" s="2" t="s">
+      <c r="N30" s="26" t="s">
+        <v>604</v>
+      </c>
+      <c r="O30" s="22" t="s">
+        <v>617</v>
+      </c>
+      <c r="P30" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="Q30" s="17" t="s">
+        <v>644</v>
+      </c>
+      <c r="R30" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q30">
+      <c r="S30">
         <v>4</v>
       </c>
-      <c r="R30" t="s">
+      <c r="T30" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4361,13 +4816,13 @@
       <c r="E31" s="5">
         <v>1000</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="20" t="s">
         <v>507</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="H31" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="H31" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I31" s="2" t="s">
@@ -4381,21 +4836,29 @@
       <c r="M31" t="s">
         <v>514</v>
       </c>
-      <c r="N31" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="O31" s="17"/>
-      <c r="P31" s="2" t="s">
+      <c r="N31" s="26" t="s">
+        <v>604</v>
+      </c>
+      <c r="O31" s="22" t="s">
+        <v>617</v>
+      </c>
+      <c r="P31" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="Q31" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="R31" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q31">
+      <c r="S31">
         <v>4</v>
       </c>
-      <c r="R31" t="s">
+      <c r="T31" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4412,13 +4875,13 @@
       <c r="E32" s="2">
         <v>2000</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="20" t="s">
         <v>495</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H32" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H32" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -4429,21 +4892,27 @@
         <v>170</v>
       </c>
       <c r="L32" s="19"/>
-      <c r="N32" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="O32" s="17"/>
-      <c r="P32" s="2" t="s">
+      <c r="N32" s="26" t="s">
+        <v>604</v>
+      </c>
+      <c r="O32" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q32">
+      <c r="S32">
         <v>5</v>
       </c>
-      <c r="R32" t="s">
+      <c r="T32" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4460,13 +4929,13 @@
       <c r="E33" s="2">
         <v>0</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="20" t="s">
         <v>496</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H33" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>167</v>
       </c>
       <c r="I33" s="2" t="s">
@@ -4477,21 +4946,27 @@
         <v>170</v>
       </c>
       <c r="L33" s="19"/>
-      <c r="N33" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="O33" s="17"/>
-      <c r="P33" s="2" t="s">
+      <c r="N33" s="26" t="s">
+        <v>604</v>
+      </c>
+      <c r="O33" s="22" t="s">
+        <v>619</v>
+      </c>
+      <c r="P33" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q33">
+      <c r="S33">
         <v>5</v>
       </c>
-      <c r="R33" t="s">
+      <c r="T33" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <f t="shared" ref="A34:A51" si="1">ROW() - 1</f>
         <v>33</v>
@@ -4508,13 +4983,13 @@
       <c r="E34" s="2">
         <v>3000</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="20" t="s">
         <v>187</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H34" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H34" s="28" t="s">
         <v>179</v>
       </c>
       <c r="I34" s="2" t="s">
@@ -4522,20 +4997,30 @@
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="18" t="s">
-        <v>605</v>
-      </c>
-      <c r="P34" s="2" t="s">
+      <c r="L34" s="18"/>
+      <c r="N34" s="24" t="s">
+        <v>657</v>
+      </c>
+      <c r="O34" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="P34" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q34" s="17">
+        <v>2000</v>
+      </c>
+      <c r="R34" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="Q34">
+      <c r="S34">
         <v>5</v>
       </c>
-      <c r="R34" t="s">
+      <c r="T34" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -4552,13 +5037,13 @@
       <c r="E35" s="2">
         <v>3000</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="20" t="s">
         <v>187</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H35" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H35" s="28" t="s">
         <v>179</v>
       </c>
       <c r="I35" s="2" t="s">
@@ -4566,20 +5051,30 @@
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="L35" s="18" t="s">
-        <v>605</v>
-      </c>
-      <c r="P35" s="2" t="s">
+      <c r="L35" s="18"/>
+      <c r="N35" s="24" t="s">
+        <v>657</v>
+      </c>
+      <c r="O35" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="P35" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q35" s="17">
+        <v>3000</v>
+      </c>
+      <c r="R35" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="Q35">
+      <c r="S35">
         <v>5</v>
       </c>
-      <c r="R35" t="s">
+      <c r="T35" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -4594,13 +5089,13 @@
         <v>151</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="20" t="s">
         <v>187</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H36" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H36" s="28" t="s">
         <v>179</v>
       </c>
       <c r="I36" s="2" t="s">
@@ -4608,20 +5103,30 @@
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="18" t="s">
-        <v>605</v>
-      </c>
-      <c r="P36" s="2" t="s">
+      <c r="L36" s="18"/>
+      <c r="N36" s="24" t="s">
+        <v>657</v>
+      </c>
+      <c r="O36" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="P36" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q36" s="17">
+        <v>3000</v>
+      </c>
+      <c r="R36" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="Q36">
+      <c r="S36">
         <v>5</v>
       </c>
-      <c r="R36" t="s">
+      <c r="T36" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -4638,13 +5143,13 @@
       <c r="E37" s="2">
         <v>3000</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="20" t="s">
         <v>187</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H37" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H37" s="28" t="s">
         <v>179</v>
       </c>
       <c r="I37" s="2" t="s">
@@ -4652,20 +5157,30 @@
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="18" t="s">
-        <v>617</v>
-      </c>
-      <c r="P37" s="2" t="s">
+      <c r="L37" s="18"/>
+      <c r="N37" s="24" t="s">
+        <v>657</v>
+      </c>
+      <c r="O37" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="P37" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q37" s="17">
+        <v>3000</v>
+      </c>
+      <c r="R37" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="Q37">
+      <c r="S37">
         <v>5</v>
       </c>
-      <c r="R37" t="s">
+      <c r="T37" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -4682,32 +5197,41 @@
       <c r="E38" s="2">
         <v>2000</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>557</v>
+      <c r="F38" s="28" t="s">
+        <v>556</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>593</v>
+        <v>549</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>592</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="N38" t="s">
-        <v>611</v>
-      </c>
-      <c r="P38" s="2" t="s">
+      <c r="N38" s="24" t="s">
+        <v>606</v>
+      </c>
+      <c r="O38" s="22" t="s">
+        <v>617</v>
+      </c>
+      <c r="P38" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>647</v>
+      </c>
+      <c r="R38" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="Q38">
+      <c r="S38">
         <v>5</v>
       </c>
-      <c r="R38" t="s">
+      <c r="T38" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -4724,32 +5248,41 @@
       <c r="E39" s="2">
         <v>2000</v>
       </c>
-      <c r="F39" s="10" t="s">
-        <v>557</v>
+      <c r="F39" s="30" t="s">
+        <v>556</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>594</v>
+        <v>549</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>593</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="N39" t="s">
-        <v>612</v>
-      </c>
-      <c r="P39" s="2" t="s">
+      <c r="N39" s="24" t="s">
+        <v>607</v>
+      </c>
+      <c r="O39" s="22" t="s">
+        <v>620</v>
+      </c>
+      <c r="P39" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>647</v>
+      </c>
+      <c r="R39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="Q39">
+      <c r="S39">
         <v>5</v>
       </c>
-      <c r="R39" t="s">
+      <c r="T39" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -4764,32 +5297,41 @@
         <v>145</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="20" t="s">
         <v>165</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H40" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H40" s="28" t="s">
         <v>176</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="N40" t="s">
-        <v>613</v>
-      </c>
-      <c r="P40" s="2" t="s">
+      <c r="N40" s="24" t="s">
+        <v>608</v>
+      </c>
+      <c r="O40" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="Q40" s="17">
+        <v>400</v>
+      </c>
+      <c r="R40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="Q40">
+      <c r="S40">
         <v>6</v>
       </c>
-      <c r="R40" t="s">
+      <c r="T40" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -4804,32 +5346,41 @@
         <v>145</v>
       </c>
       <c r="E41" s="5"/>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="20" t="s">
         <v>165</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H41" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H41" s="28" t="s">
         <v>176</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="N41" t="s">
-        <v>614</v>
-      </c>
-      <c r="P41" s="2" t="s">
+      <c r="N41" s="24" t="s">
+        <v>609</v>
+      </c>
+      <c r="O41" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="P41" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="Q41" s="17">
+        <v>500</v>
+      </c>
+      <c r="R41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="Q41">
+      <c r="S41">
         <v>6</v>
       </c>
-      <c r="R41" t="s">
+      <c r="T41" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -4844,32 +5395,41 @@
         <v>145</v>
       </c>
       <c r="E42" s="5"/>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="20" t="s">
         <v>165</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H42" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H42" s="28" t="s">
         <v>176</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="N42" t="s">
-        <v>615</v>
-      </c>
-      <c r="P42" s="2" t="s">
+      <c r="N42" s="24" t="s">
+        <v>610</v>
+      </c>
+      <c r="O42" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="Q42" s="17">
+        <v>600</v>
+      </c>
+      <c r="R42" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="Q42">
+      <c r="S42">
         <v>6</v>
       </c>
-      <c r="R42" t="s">
+      <c r="T42" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -4886,13 +5446,13 @@
       <c r="E43" s="2">
         <v>2000</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="20" t="s">
         <v>185</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H43" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H43" s="20" t="s">
         <v>189</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -4900,20 +5460,29 @@
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="N43" t="s">
-        <v>616</v>
-      </c>
-      <c r="P43" s="2" t="s">
+      <c r="N43" s="24" t="s">
+        <v>660</v>
+      </c>
+      <c r="O43" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="P43" s="17" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q43" s="17" t="s">
+        <v>651</v>
+      </c>
+      <c r="R43" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="Q43">
+      <c r="S43">
         <v>6</v>
       </c>
-      <c r="R43" t="s">
+      <c r="T43" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -4930,31 +5499,45 @@
       <c r="E44" s="2">
         <v>2000</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="20" t="s">
         <v>186</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H44" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H44" s="28" t="s">
         <v>177</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>527</v>
       </c>
       <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="P44" s="2" t="s">
+      <c r="K44" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="N44" s="24" t="s">
+        <v>661</v>
+      </c>
+      <c r="O44" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="P44" s="17" t="s">
+        <v>652</v>
+      </c>
+      <c r="Q44" s="17" t="s">
+        <v>653</v>
+      </c>
+      <c r="R44" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="Q44">
+      <c r="S44">
         <v>6</v>
       </c>
-      <c r="R44" t="s">
+      <c r="T44" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -4971,31 +5554,45 @@
       <c r="E45" s="2">
         <v>2000</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="20" t="s">
         <v>186</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H45" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H45" s="28" t="s">
         <v>181</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>528</v>
       </c>
       <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="P45" s="2" t="s">
+      <c r="K45" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="N45" s="24" t="s">
+        <v>661</v>
+      </c>
+      <c r="O45" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="P45" s="17" t="s">
+        <v>652</v>
+      </c>
+      <c r="Q45" s="17" t="s">
+        <v>654</v>
+      </c>
+      <c r="R45" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="Q45">
+      <c r="S45">
         <v>6</v>
       </c>
-      <c r="R45" t="s">
+      <c r="T45" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -5012,13 +5609,13 @@
       <c r="E46" s="2">
         <v>2000</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="20" t="s">
         <v>185</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="H46" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H46" s="20" t="s">
         <v>178</v>
       </c>
       <c r="I46" s="3" t="s">
@@ -5026,17 +5623,29 @@
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="P46" s="2" t="s">
+      <c r="N46" s="24" t="s">
+        <v>660</v>
+      </c>
+      <c r="O46" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="P46" s="17" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q46" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="R46" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="Q46">
+      <c r="S46">
         <v>6</v>
       </c>
-      <c r="R46" t="s">
+      <c r="T46" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -5051,17 +5660,17 @@
         <v>155</v>
       </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="F47" s="20"/>
       <c r="G47" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H47" s="2"/>
+        <v>549</v>
+      </c>
+      <c r="H47" s="20"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="P47" s="2"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R47" s="2"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -5076,17 +5685,17 @@
         <v>155</v>
       </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+      <c r="F48" s="20"/>
       <c r="G48" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H48" s="2"/>
+        <v>549</v>
+      </c>
+      <c r="H48" s="20"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="P48" s="2"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -5101,23 +5710,23 @@
         <v>156</v>
       </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="20" t="s">
         <v>49</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H49" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H49" s="20" t="s">
         <v>180</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="P49" s="2" t="s">
+      <c r="R49" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -5132,15 +5741,15 @@
         <v>158</v>
       </c>
       <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
+      <c r="F50" s="20"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="H50" s="20"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="P50" s="2"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="R50" s="2"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -5155,17 +5764,17 @@
         <v>159</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
+      <c r="F51" s="20"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
+      <c r="H51" s="20"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="P51" s="2"/>
+      <c r="R51" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:T51">
-    <sortCondition ref="Q2:Q51"/>
+  <sortState ref="A2:V51">
+    <sortCondition ref="S2:S51"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}" topLeftCell="A11">
@@ -6383,7 +6992,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>50</v>
@@ -6510,7 +7119,7 @@
         <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -6532,7 +7141,7 @@
         <v>63</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -6554,7 +7163,7 @@
         <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -6576,7 +7185,7 @@
         <v>61</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -6670,7 +7279,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -6762,7 +7371,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
@@ -6802,7 +7411,7 @@
         <v>63</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -6890,7 +7499,7 @@
         <v>58</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -7018,7 +7627,7 @@
         <v>204</v>
       </c>
       <c r="D1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -7351,170 +7960,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B1" t="s">
         <v>561</v>
-      </c>
-      <c r="B1" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>562</v>
+      </c>
+      <c r="B2" t="s">
         <v>563</v>
-      </c>
-      <c r="B2" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>564</v>
+      </c>
+      <c r="B3" t="s">
         <v>565</v>
-      </c>
-      <c r="B3" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B4" t="s">
         <v>567</v>
-      </c>
-      <c r="B4" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>569</v>
+      </c>
+      <c r="B6" t="s">
         <v>570</v>
-      </c>
-      <c r="B6" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>571</v>
+      </c>
+      <c r="B7" t="s">
         <v>572</v>
-      </c>
-      <c r="B7" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B10" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>576</v>
+      </c>
+      <c r="B11" t="s">
         <v>577</v>
-      </c>
-      <c r="B11" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>578</v>
+      </c>
+      <c r="B12" t="s">
         <v>579</v>
-      </c>
-      <c r="B12" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B13" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
+        <v>581</v>
+      </c>
+      <c r="B14" t="s">
         <v>582</v>
-      </c>
-      <c r="B14" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B15" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B16" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B17" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
+        <v>586</v>
+      </c>
+      <c r="B18" t="s">
         <v>587</v>
-      </c>
-      <c r="B18" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B19" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>589</v>
+      </c>
+      <c r="B20" t="s">
         <v>590</v>
-      </c>
-      <c r="B20" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B21" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completion of scoring! :tada:
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="665">
   <si>
     <t>符号判断</t>
   </si>
@@ -2576,23 +2576,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>dprimeTM dprimeFM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprimeTM dprimeFM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprimeFM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ConflictUnion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dprimeTM dprimeFM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeTM dprimeFM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeFM</t>
+    <t>dprimeUnion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3162,11 +3174,11 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
+      <selection pane="bottomRight" activeCell="N30" sqref="N30:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3852,7 +3864,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="18"/>
       <c r="N13" s="31" t="s">
-        <v>656</v>
+        <v>663</v>
       </c>
       <c r="O13" s="21" t="s">
         <v>613</v>
@@ -4347,6 +4359,9 @@
         <v>198</v>
       </c>
       <c r="L22" s="19"/>
+      <c r="N22" s="24" t="s">
+        <v>661</v>
+      </c>
       <c r="O22" s="21" t="s">
         <v>614</v>
       </c>
@@ -4400,6 +4415,9 @@
         <v>198</v>
       </c>
       <c r="L23" s="19"/>
+      <c r="N23" s="24" t="s">
+        <v>662</v>
+      </c>
       <c r="O23" s="21" t="s">
         <v>614</v>
       </c>
@@ -4453,6 +4471,9 @@
         <v>198</v>
       </c>
       <c r="L24" s="19"/>
+      <c r="N24" s="24" t="s">
+        <v>662</v>
+      </c>
       <c r="O24" s="21" t="s">
         <v>614</v>
       </c>
@@ -4778,7 +4799,7 @@
         <v>514</v>
       </c>
       <c r="N30" s="26" t="s">
-        <v>604</v>
+        <v>664</v>
       </c>
       <c r="O30" s="22" t="s">
         <v>617</v>
@@ -4837,7 +4858,7 @@
         <v>514</v>
       </c>
       <c r="N31" s="26" t="s">
-        <v>604</v>
+        <v>664</v>
       </c>
       <c r="O31" s="22" t="s">
         <v>617</v>
@@ -4999,7 +5020,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="18"/>
       <c r="N34" s="24" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="O34" s="22" t="s">
         <v>613</v>
@@ -5053,7 +5074,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="18"/>
       <c r="N35" s="24" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="O35" s="22" t="s">
         <v>613</v>
@@ -5105,7 +5126,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="18"/>
       <c r="N36" s="24" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="O36" s="22" t="s">
         <v>613</v>
@@ -5159,7 +5180,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="18"/>
       <c r="N37" s="24" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="O37" s="22" t="s">
         <v>613</v>
@@ -5461,7 +5482,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="N43" s="24" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O43" s="22" t="s">
         <v>622</v>
@@ -5513,10 +5534,10 @@
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="5" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="N44" s="24" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O44" s="22" t="s">
         <v>622</v>
@@ -5568,10 +5589,10 @@
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="5" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="N45" s="24" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O45" s="22" t="s">
         <v>622</v>
@@ -5624,7 +5645,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="N46" s="24" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O46" s="22" t="s">
         <v>622</v>

</xml_diff>

<commit_message>
Revert "Completed scoring and index calculation."
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="604">
   <si>
     <t>符号判断</t>
   </si>
@@ -2167,6 +2167,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>VRT Ter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Subitizing</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2337,274 +2341,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CountTotalTrl CountAccTrl TotalScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Mentcompare</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UltimateIndex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CountTotalTrl CountAccTrl TotalScore MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lang</t>
+    <t>distances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4 D5 D6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4 D5 D6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Conflict</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Span</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GNG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GNG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GNG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Span</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScoringPara</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3000 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3001 3000 3000</t>
-  </si>
-  <si>
-    <t>ScoringVars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalTime TotalScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall D1 D2 D3 D4 D5 D6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_Overall ACC_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_Overall ACC_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall D1 D2 D3 D4 D5 D8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_Overall ACC_Overall RT_CongEffect ACC_CongEffect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2500 2000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2800 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3200 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3000 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit Rate_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit Rate_hit Count_FA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScoringFun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit Rate_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1500 1500 1500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1500 1500 1500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_Overall ACC_Overall RT_SwitchCost ACC_SwitchCost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3000 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MLACC MLNextACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ML MLACC MLNextACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC_R1 ACC_R2 RT_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>150 100 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1_hitRate R2_hitRate MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>60 40 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50 35 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50 35 20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ConflictUnion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeTM dprimeFM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeTM dprimeFM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeFM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ConflictUnion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeUnion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2612,7 +2369,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2721,30 +2478,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2754,30 +2487,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -2788,7 +2501,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2835,60 +2548,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3171,14 +2830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="N30" sqref="N30:N31"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3188,22 +2843,18 @@
     <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.75" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.75" customWidth="1"/>
-    <col min="8" max="8" width="15" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.25" customWidth="1"/>
     <col min="10" max="10" width="14.75" customWidth="1"/>
     <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.75" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5" style="21" customWidth="1"/>
-    <col min="16" max="16" width="57.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3217,15 +2868,15 @@
         <v>157</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="F1" s="20" t="s">
+        <v>548</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="H1" s="20" t="s">
+        <v>549</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>238</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -3243,29 +2894,17 @@
       <c r="M1" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="N1" s="23" t="s">
-        <v>598</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>642</v>
+      <c r="N1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>519</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="T1" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -3280,13 +2919,13 @@
         <v>143</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H2" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -3299,26 +2938,17 @@
       <c r="L2" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N2" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>611</v>
+      <c r="N2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>627</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3333,13 +2963,13 @@
         <v>143</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H3" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -3352,26 +2982,17 @@
       <c r="L3" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N3" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>611</v>
+      <c r="N3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>627</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3386,13 +3007,13 @@
         <v>143</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H4" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -3405,26 +3026,17 @@
       <c r="L4" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N4" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>611</v>
+      <c r="N4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>627</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3439,13 +3051,13 @@
         <v>143</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H5" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -3458,26 +3070,17 @@
       <c r="L5" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N5" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="O5" s="21" t="s">
-        <v>611</v>
+      <c r="N5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>627</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3492,13 +3095,13 @@
         <v>143</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H6" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -3511,26 +3114,17 @@
       <c r="L6" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N6" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="O6" s="21" t="s">
-        <v>611</v>
+      <c r="N6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>627</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3545,13 +3139,13 @@
         <v>143</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H7" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -3564,26 +3158,17 @@
       <c r="L7" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N7" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="O7" s="21" t="s">
-        <v>611</v>
+      <c r="N7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>627</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3598,31 +3183,28 @@
         <v>237</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="20"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H8" s="20"/>
+        <v>550</v>
+      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" t="s">
-        <v>600</v>
-      </c>
-      <c r="N8" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="R8" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3639,44 +3221,36 @@
       <c r="E9" s="7">
         <v>3000</v>
       </c>
-      <c r="F9" s="29" t="s">
-        <v>556</v>
+      <c r="F9" s="7" t="s">
+        <v>557</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H9" s="27" t="s">
+        <v>550</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>175</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="J9" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>198</v>
+      </c>
       <c r="L9" t="s">
         <v>544</v>
       </c>
-      <c r="N9" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="O9" s="21" t="s">
-        <v>612</v>
+      <c r="N9" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
       </c>
       <c r="P9" t="s">
-        <v>628</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>624</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="S9">
-        <v>2</v>
-      </c>
-      <c r="T9" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3693,44 +3267,36 @@
       <c r="E10" s="7">
         <v>3000</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>556</v>
+      <c r="F10" s="8" t="s">
+        <v>557</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H10" s="27" t="s">
+        <v>550</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>175</v>
       </c>
       <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="J10" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>198</v>
+      </c>
       <c r="L10" t="s">
         <v>544</v>
       </c>
-      <c r="N10" s="24" t="s">
-        <v>605</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>612</v>
+      <c r="N10" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
       </c>
       <c r="P10" t="s">
-        <v>628</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>624</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="S10">
-        <v>2</v>
-      </c>
-      <c r="T10" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3747,41 +3313,38 @@
       <c r="E11" s="8">
         <v>2000</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>597</v>
+      <c r="F11" s="8" t="s">
+        <v>599</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>630</v>
+        <v>550</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>603</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>629</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="O11" s="21" t="s">
-        <v>612</v>
+        <v>601</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
       </c>
       <c r="P11" t="s">
-        <v>631</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>624</v>
-      </c>
-      <c r="R11" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="S11">
-        <v>2</v>
-      </c>
-      <c r="T11" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3790,7 +3353,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>141</v>
@@ -3798,40 +3361,35 @@
       <c r="E12" s="8">
         <v>3000</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>597</v>
+      <c r="F12" s="8" t="s">
+        <v>599</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>178</v>
+        <v>550</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>633</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="O12" s="21" t="s">
-        <v>612</v>
+        <v>602</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
       </c>
       <c r="P12" t="s">
-        <v>632</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>625</v>
-      </c>
-      <c r="R12" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="S12">
-        <v>2</v>
-      </c>
-      <c r="T12" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3848,13 +3406,13 @@
       <c r="E13" s="10">
         <v>2000</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H13" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>179</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -3862,30 +3420,17 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="18"/>
-      <c r="N13" s="31" t="s">
-        <v>663</v>
-      </c>
-      <c r="O13" s="21" t="s">
-        <v>613</v>
+      <c r="N13" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
       </c>
       <c r="P13" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q13">
-        <v>3000</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="S13">
-        <v>2</v>
-      </c>
-      <c r="T13" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3902,13 +3447,13 @@
       <c r="E14" s="2">
         <v>3000</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H14" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I14" s="2"/>
@@ -3916,30 +3461,17 @@
         <v>173</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="19"/>
-      <c r="N14" s="24" t="s">
-        <v>601</v>
-      </c>
-      <c r="O14" s="21" t="s">
-        <v>614</v>
+      <c r="N14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
       </c>
       <c r="P14" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>636</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="S14">
-        <v>3</v>
-      </c>
-      <c r="T14" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3956,13 +3488,13 @@
       <c r="E15" s="2">
         <v>3000</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H15" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I15" s="2"/>
@@ -3970,30 +3502,17 @@
         <v>173</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="19"/>
-      <c r="N15" s="24" t="s">
-        <v>601</v>
-      </c>
-      <c r="O15" s="21" t="s">
-        <v>614</v>
+      <c r="N15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O15">
+        <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>636</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="S15">
-        <v>3</v>
-      </c>
-      <c r="T15" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4010,13 +3529,13 @@
       <c r="E16" s="2">
         <v>3000</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H16" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I16" s="2"/>
@@ -4024,30 +3543,17 @@
         <v>173</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="19"/>
-      <c r="N16" s="24" t="s">
-        <v>601</v>
-      </c>
-      <c r="O16" s="21" t="s">
-        <v>614</v>
+      <c r="N16" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
       </c>
       <c r="P16" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>636</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="S16">
-        <v>3</v>
-      </c>
-      <c r="T16" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4064,13 +3570,13 @@
       <c r="E17" s="2">
         <v>3000</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H17" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I17" s="2"/>
@@ -4078,30 +3584,17 @@
         <v>497</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="L17" s="19"/>
-      <c r="N17" s="24" t="s">
-        <v>601</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>614</v>
+      <c r="N17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O17">
+        <v>3</v>
       </c>
       <c r="P17" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>636</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="S17">
-        <v>3</v>
-      </c>
-      <c r="T17" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4118,13 +3611,13 @@
       <c r="E18" s="2">
         <v>3000</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="2" t="s">
         <v>500</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H18" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I18" s="2" t="s">
@@ -4134,30 +3627,17 @@
       <c r="K18" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="N18" s="24" t="s">
-        <v>602</v>
-      </c>
-      <c r="O18" s="21" t="s">
-        <v>614</v>
-      </c>
-      <c r="P18" s="32" t="s">
-        <v>640</v>
-      </c>
-      <c r="Q18" s="33" t="s">
-        <v>637</v>
-      </c>
-      <c r="R18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S18">
+      <c r="O18">
         <v>3</v>
       </c>
-      <c r="T18" t="s">
+      <c r="P18" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4174,13 +3654,13 @@
       <c r="E19" s="2">
         <v>3000</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="2" t="s">
         <v>500</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H19" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -4190,30 +3670,17 @@
       <c r="K19" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L19" s="19"/>
-      <c r="N19" s="24" t="s">
-        <v>602</v>
-      </c>
-      <c r="O19" s="21" t="s">
-        <v>614</v>
-      </c>
-      <c r="P19" s="32" t="s">
-        <v>640</v>
-      </c>
-      <c r="Q19" s="33" t="s">
-        <v>637</v>
-      </c>
-      <c r="R19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S19">
+      <c r="O19">
         <v>3</v>
       </c>
-      <c r="T19" t="s">
+      <c r="P19" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4230,13 +3697,13 @@
       <c r="E20" s="2">
         <v>3000</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="2" t="s">
         <v>500</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H20" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I20" s="2" t="s">
@@ -4246,30 +3713,17 @@
       <c r="K20" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="N20" s="24" t="s">
-        <v>602</v>
-      </c>
-      <c r="O20" s="21" t="s">
-        <v>614</v>
-      </c>
-      <c r="P20" s="32" t="s">
-        <v>640</v>
-      </c>
-      <c r="Q20" s="33" t="s">
-        <v>637</v>
-      </c>
-      <c r="R20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S20">
+      <c r="O20">
         <v>3</v>
       </c>
-      <c r="T20" t="s">
+      <c r="P20" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4286,13 +3740,13 @@
       <c r="E21" s="2">
         <v>3000</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="2" t="s">
         <v>500</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H21" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -4302,30 +3756,17 @@
       <c r="K21" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="N21" s="24" t="s">
-        <v>602</v>
-      </c>
-      <c r="O21" s="21" t="s">
-        <v>614</v>
-      </c>
-      <c r="P21" s="32" t="s">
-        <v>640</v>
-      </c>
-      <c r="Q21" s="33" t="s">
-        <v>637</v>
-      </c>
-      <c r="R21" s="2" t="s">
+      <c r="N21" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S21">
+      <c r="O21">
         <v>3</v>
       </c>
-      <c r="T21" t="s">
+      <c r="P21" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4342,13 +3783,13 @@
       <c r="E22" s="2">
         <v>3000</v>
       </c>
-      <c r="F22" s="20" t="s">
-        <v>556</v>
+      <c r="F22" s="2" t="s">
+        <v>557</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H22" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I22" s="2"/>
@@ -4358,30 +3799,17 @@
       <c r="K22" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L22" s="19"/>
-      <c r="N22" s="24" t="s">
-        <v>661</v>
-      </c>
-      <c r="O22" s="21" t="s">
-        <v>614</v>
+      <c r="N22" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O22">
+        <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>638</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="S22">
-        <v>3</v>
-      </c>
-      <c r="T22" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4398,13 +3826,13 @@
       <c r="E23" s="2">
         <v>3000</v>
       </c>
-      <c r="F23" s="20" t="s">
-        <v>556</v>
+      <c r="F23" s="2" t="s">
+        <v>557</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H23" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I23" s="2"/>
@@ -4414,30 +3842,17 @@
       <c r="K23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L23" s="19"/>
-      <c r="N23" s="24" t="s">
-        <v>662</v>
-      </c>
-      <c r="O23" s="21" t="s">
-        <v>614</v>
+      <c r="N23" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
       </c>
       <c r="P23" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>638</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="S23">
-        <v>3</v>
-      </c>
-      <c r="T23" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4454,13 +3869,13 @@
       <c r="E24" s="2">
         <v>3000</v>
       </c>
-      <c r="F24" s="20" t="s">
-        <v>556</v>
+      <c r="F24" s="2" t="s">
+        <v>557</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H24" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I24" s="2"/>
@@ -4470,30 +3885,17 @@
       <c r="K24" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L24" s="19"/>
-      <c r="N24" s="24" t="s">
-        <v>662</v>
-      </c>
-      <c r="O24" s="21" t="s">
-        <v>614</v>
+      <c r="N24" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O24">
+        <v>3</v>
       </c>
       <c r="P24" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>638</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="S24">
-        <v>3</v>
-      </c>
-      <c r="T24" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4510,13 +3912,13 @@
       <c r="E25" s="2">
         <v>3000</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H25" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I25" s="2"/>
@@ -4524,30 +3926,17 @@
         <v>173</v>
       </c>
       <c r="K25" s="2"/>
-      <c r="L25" s="19"/>
-      <c r="N25" s="24" t="s">
-        <v>601</v>
-      </c>
-      <c r="O25" s="21" t="s">
-        <v>614</v>
+      <c r="N25" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O25">
+        <v>3</v>
       </c>
       <c r="P25" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>639</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="S25">
-        <v>3</v>
-      </c>
-      <c r="T25" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4564,13 +3953,13 @@
       <c r="E26" s="2">
         <v>1000</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H26" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I26" s="2"/>
@@ -4578,30 +3967,17 @@
         <v>173</v>
       </c>
       <c r="K26" s="2"/>
-      <c r="L26" s="19"/>
-      <c r="N26" s="24" t="s">
-        <v>601</v>
-      </c>
-      <c r="O26" s="21" t="s">
-        <v>614</v>
+      <c r="N26" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O26">
+        <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>624</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="S26">
-        <v>3</v>
-      </c>
-      <c r="T26" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4616,44 +3992,29 @@
         <v>142</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="5" t="s">
         <v>184</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H27" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>176</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="5" t="s">
-        <v>648</v>
-      </c>
-      <c r="L27" s="19"/>
-      <c r="N27" s="24" t="s">
-        <v>603</v>
-      </c>
-      <c r="O27" s="21" t="s">
-        <v>615</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="Q27">
-        <v>600</v>
-      </c>
-      <c r="R27" s="2" t="s">
+      <c r="K27" s="2"/>
+      <c r="N27" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S27">
+      <c r="O27">
         <v>4</v>
       </c>
-      <c r="T27" t="s">
+      <c r="P27" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4670,13 +4031,13 @@
       <c r="E28" s="5">
         <v>1000</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H28" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I28" s="2" t="s">
@@ -4686,32 +4047,22 @@
       <c r="K28" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L28" s="19"/>
-      <c r="N28" s="24" t="s">
-        <v>602</v>
-      </c>
-      <c r="O28" s="21" t="s">
-        <v>616</v>
-      </c>
-      <c r="P28" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="R28" s="2" t="s">
+      <c r="N28" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S28">
+      <c r="O28">
         <v>4</v>
       </c>
-      <c r="T28" t="s">
+      <c r="P28" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -4723,13 +4074,13 @@
       <c r="E29" s="5">
         <v>500</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H29" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>510</v>
       </c>
       <c r="I29" s="2" t="s">
@@ -4738,30 +4089,18 @@
       <c r="J29" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="K29" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="L29" s="19"/>
-      <c r="N29" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="O29" s="21" t="s">
-        <v>616</v>
-      </c>
-      <c r="P29" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="R29" s="2" t="s">
+      <c r="K29" s="2"/>
+      <c r="N29" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="S29">
+      <c r="O29">
         <v>4</v>
       </c>
-      <c r="T29" t="s">
+      <c r="P29" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4778,13 +4117,13 @@
       <c r="E30" s="5">
         <v>1000</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" s="5" t="s">
         <v>507</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="H30" s="20" t="s">
+        <v>552</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I30" s="2" t="s">
@@ -4794,33 +4133,20 @@
       <c r="K30" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L30" s="19"/>
       <c r="M30" t="s">
         <v>514</v>
       </c>
-      <c r="N30" s="26" t="s">
-        <v>664</v>
-      </c>
-      <c r="O30" s="22" t="s">
-        <v>617</v>
-      </c>
-      <c r="P30" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="Q30" s="17" t="s">
-        <v>644</v>
-      </c>
-      <c r="R30" s="2" t="s">
+      <c r="N30" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S30">
+      <c r="O30">
         <v>4</v>
       </c>
-      <c r="T30" t="s">
+      <c r="P30" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4837,13 +4163,13 @@
       <c r="E31" s="5">
         <v>1000</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="5" t="s">
         <v>507</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="H31" s="20" t="s">
+        <v>552</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I31" s="2" t="s">
@@ -4853,33 +4179,20 @@
       <c r="K31" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="L31" s="19"/>
       <c r="M31" t="s">
         <v>514</v>
       </c>
-      <c r="N31" s="26" t="s">
-        <v>664</v>
-      </c>
-      <c r="O31" s="22" t="s">
-        <v>617</v>
-      </c>
-      <c r="P31" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="Q31" s="17" t="s">
-        <v>645</v>
-      </c>
-      <c r="R31" s="2" t="s">
+      <c r="N31" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S31">
+      <c r="O31">
         <v>4</v>
       </c>
-      <c r="T31" t="s">
+      <c r="P31" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4896,13 +4209,13 @@
       <c r="E32" s="2">
         <v>2000</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="2" t="s">
         <v>495</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H32" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -4912,28 +4225,17 @@
       <c r="K32" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L32" s="19"/>
-      <c r="N32" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="O32" s="22" t="s">
-        <v>618</v>
-      </c>
-      <c r="P32" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S32">
+      <c r="O32">
         <v>5</v>
       </c>
-      <c r="T32" t="s">
+      <c r="P32" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4950,13 +4252,13 @@
       <c r="E33" s="2">
         <v>0</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="2" t="s">
         <v>496</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H33" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>167</v>
       </c>
       <c r="I33" s="2" t="s">
@@ -4966,28 +4268,17 @@
       <c r="K33" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L33" s="19"/>
-      <c r="N33" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="O33" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="P33" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S33">
+      <c r="O33">
         <v>5</v>
       </c>
-      <c r="T33" t="s">
+      <c r="P33" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <f t="shared" ref="A34:A51" si="1">ROW() - 1</f>
         <v>33</v>
@@ -5004,13 +4295,13 @@
       <c r="E34" s="2">
         <v>3000</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H34" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>179</v>
       </c>
       <c r="I34" s="2" t="s">
@@ -5018,30 +4309,17 @@
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="18"/>
-      <c r="N34" s="24" t="s">
-        <v>656</v>
-      </c>
-      <c r="O34" s="22" t="s">
-        <v>613</v>
+      <c r="N34" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="O34">
+        <v>5</v>
       </c>
       <c r="P34" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q34" s="17">
-        <v>2000</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="S34">
-        <v>5</v>
-      </c>
-      <c r="T34" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -5058,13 +4336,13 @@
       <c r="E35" s="2">
         <v>3000</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H35" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>179</v>
       </c>
       <c r="I35" s="2" t="s">
@@ -5072,30 +4350,17 @@
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="L35" s="18"/>
-      <c r="N35" s="24" t="s">
-        <v>656</v>
-      </c>
-      <c r="O35" s="22" t="s">
-        <v>613</v>
+      <c r="N35" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="O35">
+        <v>5</v>
       </c>
       <c r="P35" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q35" s="17">
-        <v>3000</v>
-      </c>
-      <c r="R35" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="S35">
-        <v>5</v>
-      </c>
-      <c r="T35" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -5110,13 +4375,13 @@
         <v>151</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H36" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>179</v>
       </c>
       <c r="I36" s="2" t="s">
@@ -5124,35 +4389,22 @@
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="18"/>
-      <c r="N36" s="24" t="s">
-        <v>656</v>
-      </c>
-      <c r="O36" s="22" t="s">
-        <v>613</v>
+      <c r="N36" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="O36">
+        <v>5</v>
       </c>
       <c r="P36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q36" s="17">
-        <v>3000</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="S36">
-        <v>5</v>
-      </c>
-      <c r="T36" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C37" s="13" t="s">
@@ -5164,13 +4416,13 @@
       <c r="E37" s="2">
         <v>3000</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H37" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>179</v>
       </c>
       <c r="I37" s="2" t="s">
@@ -5178,30 +4430,17 @@
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="18"/>
-      <c r="N37" s="24" t="s">
-        <v>656</v>
-      </c>
-      <c r="O37" s="22" t="s">
-        <v>613</v>
+      <c r="N37" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="O37">
+        <v>5</v>
       </c>
       <c r="P37" t="s">
-        <v>646</v>
-      </c>
-      <c r="Q37" s="17">
-        <v>3000</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="S37">
-        <v>5</v>
-      </c>
-      <c r="T37" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -5218,41 +4457,29 @@
       <c r="E38" s="2">
         <v>2000</v>
       </c>
-      <c r="F38" s="28" t="s">
-        <v>556</v>
+      <c r="F38" s="3" t="s">
+        <v>557</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>592</v>
+        <v>550</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>593</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="N38" s="24" t="s">
-        <v>606</v>
-      </c>
-      <c r="O38" s="22" t="s">
-        <v>617</v>
+      <c r="N38" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O38">
+        <v>5</v>
       </c>
       <c r="P38" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>647</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="S38">
-        <v>5</v>
-      </c>
-      <c r="T38" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -5269,41 +4496,29 @@
       <c r="E39" s="2">
         <v>2000</v>
       </c>
-      <c r="F39" s="30" t="s">
-        <v>556</v>
+      <c r="F39" s="10" t="s">
+        <v>557</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>593</v>
+        <v>550</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>594</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="N39" s="24" t="s">
-        <v>607</v>
-      </c>
-      <c r="O39" s="22" t="s">
-        <v>620</v>
+      <c r="N39" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O39">
+        <v>5</v>
       </c>
       <c r="P39" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>647</v>
-      </c>
-      <c r="R39" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="S39">
-        <v>5</v>
-      </c>
-      <c r="T39" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -5318,41 +4533,29 @@
         <v>145</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="5" t="s">
         <v>165</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H40" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>176</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="N40" s="24" t="s">
-        <v>608</v>
-      </c>
-      <c r="O40" s="22" t="s">
-        <v>621</v>
-      </c>
-      <c r="P40" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="Q40" s="17">
-        <v>400</v>
-      </c>
-      <c r="R40" s="2" t="s">
+      <c r="N40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S40">
+      <c r="O40">
         <v>6</v>
       </c>
-      <c r="T40" t="s">
+      <c r="P40" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -5367,41 +4570,29 @@
         <v>145</v>
       </c>
       <c r="E41" s="5"/>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="5" t="s">
         <v>165</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H41" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>176</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="N41" s="24" t="s">
-        <v>609</v>
-      </c>
-      <c r="O41" s="22" t="s">
-        <v>621</v>
-      </c>
-      <c r="P41" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="Q41" s="17">
-        <v>500</v>
-      </c>
-      <c r="R41" s="2" t="s">
+      <c r="N41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S41">
+      <c r="O41">
         <v>6</v>
       </c>
-      <c r="T41" t="s">
+      <c r="P41" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -5416,41 +4607,29 @@
         <v>145</v>
       </c>
       <c r="E42" s="5"/>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="5" t="s">
         <v>165</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H42" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>176</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="N42" s="24" t="s">
-        <v>610</v>
-      </c>
-      <c r="O42" s="22" t="s">
-        <v>621</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="Q42" s="17">
-        <v>600</v>
-      </c>
-      <c r="R42" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S42">
+      <c r="O42">
         <v>6</v>
       </c>
-      <c r="T42" t="s">
+      <c r="P42" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -5467,13 +4646,13 @@
       <c r="E43" s="2">
         <v>2000</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="2" t="s">
         <v>185</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H43" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>189</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -5481,29 +4660,17 @@
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="N43" s="24" t="s">
-        <v>659</v>
-      </c>
-      <c r="O43" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="P43" s="17" t="s">
-        <v>650</v>
-      </c>
-      <c r="Q43" s="17" t="s">
-        <v>651</v>
-      </c>
-      <c r="R43" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="S43">
+      <c r="O43">
         <v>6</v>
       </c>
-      <c r="T43" t="s">
+      <c r="P43" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -5520,45 +4687,31 @@
       <c r="E44" s="2">
         <v>2000</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H44" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H44" s="3" t="s">
         <v>177</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>527</v>
       </c>
       <c r="J44" s="2"/>
-      <c r="K44" s="5" t="s">
-        <v>657</v>
-      </c>
-      <c r="N44" s="24" t="s">
-        <v>660</v>
-      </c>
-      <c r="O44" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="P44" s="17" t="s">
-        <v>652</v>
-      </c>
-      <c r="Q44" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="R44" s="2" t="s">
+      <c r="K44" s="2"/>
+      <c r="N44" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="S44">
+      <c r="O44">
         <v>6</v>
       </c>
-      <c r="T44" t="s">
+      <c r="P44" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -5575,45 +4728,31 @@
       <c r="E45" s="2">
         <v>2000</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="F45" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H45" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>181</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>528</v>
       </c>
       <c r="J45" s="2"/>
-      <c r="K45" s="5" t="s">
-        <v>658</v>
-      </c>
-      <c r="N45" s="24" t="s">
-        <v>660</v>
-      </c>
-      <c r="O45" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="P45" s="17" t="s">
-        <v>652</v>
-      </c>
-      <c r="Q45" s="17" t="s">
-        <v>654</v>
-      </c>
-      <c r="R45" s="2" t="s">
+      <c r="K45" s="2"/>
+      <c r="N45" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="S45">
+      <c r="O45">
         <v>6</v>
       </c>
-      <c r="T45" t="s">
+      <c r="P45" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -5630,13 +4769,13 @@
       <c r="E46" s="2">
         <v>2000</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="2" t="s">
         <v>185</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="H46" s="20" t="s">
+        <v>554</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>178</v>
       </c>
       <c r="I46" s="3" t="s">
@@ -5644,29 +4783,17 @@
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="N46" s="24" t="s">
-        <v>659</v>
-      </c>
-      <c r="O46" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="P46" s="17" t="s">
-        <v>650</v>
-      </c>
-      <c r="Q46" s="17" t="s">
-        <v>655</v>
-      </c>
-      <c r="R46" s="2" t="s">
+      <c r="N46" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="S46">
+      <c r="O46">
         <v>6</v>
       </c>
-      <c r="T46" t="s">
+      <c r="P46" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -5681,17 +4808,17 @@
         <v>155</v>
       </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="20"/>
+      <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H47" s="20"/>
+        <v>550</v>
+      </c>
+      <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="R47" s="2"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -5706,22 +4833,22 @@
         <v>155</v>
       </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="20"/>
+      <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H48" s="20"/>
+        <v>550</v>
+      </c>
+      <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="R48" s="2"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -5731,23 +4858,23 @@
         <v>156</v>
       </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="20" t="s">
+      <c r="F49" s="2" t="s">
         <v>49</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H49" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>180</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="R49" s="2" t="s">
+      <c r="N49" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -5762,15 +4889,15 @@
         <v>158</v>
       </c>
       <c r="E50" s="2"/>
-      <c r="F50" s="20"/>
+      <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="20"/>
+      <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="R50" s="2"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -5785,17 +4912,17 @@
         <v>159</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="20"/>
+      <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="20"/>
+      <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="R51" s="2"/>
+      <c r="N51" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:V51">
-    <sortCondition ref="S2:S51"/>
+  <sortState ref="A2:R51">
+    <sortCondition ref="O2:O51"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}" topLeftCell="A11">
@@ -7013,7 +6140,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>50</v>
@@ -7140,7 +6267,7 @@
         <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -7162,7 +6289,7 @@
         <v>63</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -7184,7 +6311,7 @@
         <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -7206,7 +6333,7 @@
         <v>61</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -7300,7 +6427,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -7392,7 +6519,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
@@ -7432,7 +6559,7 @@
         <v>63</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -7520,7 +6647,7 @@
         <v>58</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -7648,7 +6775,7 @@
         <v>204</v>
       </c>
       <c r="D1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -7981,170 +7108,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B3" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B4" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>569</v>
+      </c>
+      <c r="B5" t="s">
         <v>568</v>
-      </c>
-      <c r="B5" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B6" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B7" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>574</v>
+      </c>
+      <c r="B8" t="s">
         <v>573</v>
-      </c>
-      <c r="B8" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B9" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B10" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B11" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B12" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
+        <v>581</v>
+      </c>
+      <c r="B13" t="s">
         <v>580</v>
-      </c>
-      <c r="B13" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B14" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>584</v>
+      </c>
+      <c r="B15" t="s">
         <v>583</v>
-      </c>
-      <c r="B15" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B16" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B17" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B18" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
+        <v>589</v>
+      </c>
+      <c r="B19" t="s">
         <v>588</v>
-      </c>
-      <c r="B19" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B20" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
+        <v>592</v>
+      </c>
+      <c r="B21" t="s">
         <v>591</v>
-      </c>
-      <c r="B21" t="s">
-        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the ACC chance level checking.
</commit_message>
<xml_diff>
--- a/scripts/taskSettings.xlsx
+++ b/scripts/taskSettings.xlsx
@@ -138,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="666">
   <si>
     <t>符号判断</t>
   </si>
@@ -2605,6 +2605,10 @@
   </si>
   <si>
     <t>dprimeUnion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChanceACC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3171,14 +3175,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="N30" sqref="N30:N31"/>
+      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3187,23 +3191,23 @@
     <col min="2" max="2" width="12.25" customWidth="1"/>
     <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.75" customWidth="1"/>
-    <col min="8" max="8" width="15" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.25" customWidth="1"/>
-    <col min="10" max="10" width="14.75" customWidth="1"/>
-    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.75" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5" style="21" customWidth="1"/>
-    <col min="16" max="16" width="57.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.75" customWidth="1"/>
+    <col min="7" max="7" width="12.75" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="9" max="9" width="15" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.25" customWidth="1"/>
+    <col min="11" max="11" width="14.75" customWidth="1"/>
+    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.75" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" style="21" customWidth="1"/>
+    <col min="17" max="17" width="57.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3219,53 +3223,56 @@
       <c r="E1" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="O1" s="23" t="s">
         <v>598</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>642</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -3280,45 +3287,48 @@
         <v>143</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="O2" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="P2" s="21" t="s">
         <v>611</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>627</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3333,45 +3343,48 @@
         <v>143</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="I3" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="O3" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="P3" s="21" t="s">
         <v>611</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>627</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3386,45 +3399,48 @@
         <v>143</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="I4" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="O4" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="P4" s="21" t="s">
         <v>611</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>627</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3439,45 +3455,48 @@
         <v>143</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="I5" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="O5" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="P5" s="21" t="s">
         <v>611</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>627</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3492,45 +3511,48 @@
         <v>143</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="I6" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="O6" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="P6" s="21" t="s">
         <v>611</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>627</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3545,45 +3567,48 @@
         <v>143</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="I7" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="N7" s="24" t="s">
+      <c r="O7" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="P7" s="21" t="s">
         <v>611</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>627</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3598,31 +3623,32 @@
         <v>237</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="2"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" t="s">
+      <c r="L8" s="2"/>
+      <c r="M8" t="s">
         <v>600</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="O8" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3639,44 +3665,47 @@
       <c r="E9" s="7">
         <v>3000</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="29" t="s">
         <v>556</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="I9" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" t="s">
+      <c r="L9" s="8"/>
+      <c r="M9" t="s">
         <v>544</v>
       </c>
-      <c r="N9" s="24" t="s">
+      <c r="O9" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="P9" s="21" t="s">
         <v>612</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>628</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>624</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="S9" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="S9">
-        <v>2</v>
-      </c>
-      <c r="T9" t="s">
+      <c r="T9">
+        <v>2</v>
+      </c>
+      <c r="U9" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3693,44 +3722,47 @@
       <c r="E10" s="7">
         <v>3000</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="27" t="s">
         <v>556</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="I10" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" t="s">
+      <c r="L10" s="8"/>
+      <c r="M10" t="s">
         <v>544</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="O10" s="24" t="s">
         <v>605</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="P10" s="21" t="s">
         <v>612</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>628</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>624</v>
       </c>
-      <c r="R10" s="8" t="s">
+      <c r="S10" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="S10">
-        <v>2</v>
-      </c>
-      <c r="T10" t="s">
+      <c r="T10">
+        <v>2</v>
+      </c>
+      <c r="U10" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3747,41 +3779,44 @@
       <c r="E11" s="8">
         <v>2000</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="27" t="s">
         <v>597</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="I11" s="27" t="s">
         <v>630</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>629</v>
       </c>
-      <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="O11" s="21" t="s">
+      <c r="M11" s="8"/>
+      <c r="P11" s="21" t="s">
         <v>612</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>631</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>624</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="S11" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="S11">
-        <v>2</v>
-      </c>
-      <c r="T11" t="s">
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3798,40 +3833,43 @@
       <c r="E12" s="8">
         <v>3000</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>597</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="I12" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>633</v>
       </c>
-      <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="O12" s="21" t="s">
+      <c r="L12" s="8"/>
+      <c r="P12" s="21" t="s">
         <v>612</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>632</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>625</v>
       </c>
-      <c r="R12" s="8" t="s">
+      <c r="S12" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="S12">
-        <v>2</v>
-      </c>
-      <c r="T12" t="s">
+      <c r="T12">
+        <v>2</v>
+      </c>
+      <c r="U12" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3848,44 +3886,47 @@
       <c r="E13" s="10">
         <v>2000</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="I13" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="18"/>
-      <c r="N13" s="31" t="s">
+      <c r="L13" s="2"/>
+      <c r="M13" s="18"/>
+      <c r="O13" s="31" t="s">
         <v>663</v>
       </c>
-      <c r="O13" s="21" t="s">
+      <c r="P13" s="21" t="s">
         <v>613</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>634</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>3000</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="S13" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="S13">
-        <v>2</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="T13">
+        <v>2</v>
+      </c>
+      <c r="U13" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3902,44 +3943,45 @@
       <c r="E14" s="2">
         <v>3000</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="19"/>
-      <c r="N14" s="24" t="s">
+      <c r="L14" s="2"/>
+      <c r="M14" s="19"/>
+      <c r="O14" s="24" t="s">
         <v>601</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="P14" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>635</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>636</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="S14" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>3</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3956,44 +3998,45 @@
       <c r="E15" s="2">
         <v>3000</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="2"/>
+      <c r="G15" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="I15" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="19"/>
-      <c r="N15" s="24" t="s">
+      <c r="L15" s="2"/>
+      <c r="M15" s="19"/>
+      <c r="O15" s="24" t="s">
         <v>601</v>
       </c>
-      <c r="O15" s="21" t="s">
+      <c r="P15" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>635</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>636</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="S15" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>3</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4010,44 +4053,45 @@
       <c r="E16" s="2">
         <v>3000</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="I16" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="19"/>
-      <c r="N16" s="24" t="s">
+      <c r="L16" s="2"/>
+      <c r="M16" s="19"/>
+      <c r="O16" s="24" t="s">
         <v>601</v>
       </c>
-      <c r="O16" s="21" t="s">
+      <c r="P16" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>635</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>636</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="S16" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>3</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4064,44 +4108,45 @@
       <c r="E17" s="2">
         <v>3000</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="2"/>
+      <c r="G17" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="I17" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="19"/>
-      <c r="N17" s="24" t="s">
+      <c r="L17" s="2"/>
+      <c r="M17" s="19"/>
+      <c r="O17" s="24" t="s">
         <v>601</v>
       </c>
-      <c r="O17" s="21" t="s">
+      <c r="P17" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>635</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>636</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="S17" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>3</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4118,46 +4163,49 @@
       <c r="E18" s="2">
         <v>3000</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="I18" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="N18" s="24" t="s">
+      <c r="M18" s="19"/>
+      <c r="O18" s="24" t="s">
         <v>602</v>
       </c>
-      <c r="O18" s="21" t="s">
+      <c r="P18" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P18" s="32" t="s">
+      <c r="Q18" s="32" t="s">
         <v>640</v>
       </c>
-      <c r="Q18" s="33" t="s">
+      <c r="R18" s="33" t="s">
         <v>637</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="S18" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>3</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4174,46 +4222,49 @@
       <c r="E19" s="2">
         <v>3000</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="I19" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L19" s="19"/>
-      <c r="N19" s="24" t="s">
+      <c r="M19" s="19"/>
+      <c r="O19" s="24" t="s">
         <v>602</v>
       </c>
-      <c r="O19" s="21" t="s">
+      <c r="P19" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P19" s="32" t="s">
+      <c r="Q19" s="32" t="s">
         <v>640</v>
       </c>
-      <c r="Q19" s="33" t="s">
+      <c r="R19" s="33" t="s">
         <v>637</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="S19" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>3</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4230,46 +4281,49 @@
       <c r="E20" s="2">
         <v>3000</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="I20" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="N20" s="24" t="s">
+      <c r="M20" s="19"/>
+      <c r="O20" s="24" t="s">
         <v>602</v>
       </c>
-      <c r="O20" s="21" t="s">
+      <c r="P20" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P20" s="32" t="s">
+      <c r="Q20" s="32" t="s">
         <v>640</v>
       </c>
-      <c r="Q20" s="33" t="s">
+      <c r="R20" s="33" t="s">
         <v>637</v>
       </c>
-      <c r="R20" s="2" t="s">
+      <c r="S20" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>3</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4286,46 +4340,49 @@
       <c r="E21" s="2">
         <v>3000</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="I21" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="N21" s="24" t="s">
+      <c r="M21" s="19"/>
+      <c r="O21" s="24" t="s">
         <v>602</v>
       </c>
-      <c r="O21" s="21" t="s">
+      <c r="P21" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P21" s="32" t="s">
+      <c r="Q21" s="32" t="s">
         <v>640</v>
       </c>
-      <c r="Q21" s="33" t="s">
+      <c r="R21" s="33" t="s">
         <v>637</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="S21" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>3</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4342,46 +4399,49 @@
       <c r="E22" s="2">
         <v>3000</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="20" t="s">
         <v>556</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="I22" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="2"/>
+      <c r="K22" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L22" s="19"/>
-      <c r="N22" s="24" t="s">
+      <c r="M22" s="19"/>
+      <c r="O22" s="24" t="s">
         <v>661</v>
       </c>
-      <c r="O22" s="21" t="s">
+      <c r="P22" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>635</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>638</v>
       </c>
-      <c r="R22" s="2" t="s">
+      <c r="S22" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>3</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4398,46 +4458,49 @@
       <c r="E23" s="2">
         <v>3000</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="20" t="s">
         <v>556</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="I23" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L23" s="19"/>
-      <c r="N23" s="24" t="s">
+      <c r="M23" s="19"/>
+      <c r="O23" s="24" t="s">
         <v>662</v>
       </c>
-      <c r="O23" s="21" t="s">
+      <c r="P23" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>635</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>638</v>
       </c>
-      <c r="R23" s="2" t="s">
+      <c r="S23" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <v>3</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4454,46 +4517,49 @@
       <c r="E24" s="2">
         <v>3000</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="20" t="s">
         <v>556</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="I24" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="L24" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L24" s="19"/>
-      <c r="N24" s="24" t="s">
+      <c r="M24" s="19"/>
+      <c r="O24" s="24" t="s">
         <v>662</v>
       </c>
-      <c r="O24" s="21" t="s">
+      <c r="P24" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>635</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>638</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="S24" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <v>3</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4510,44 +4576,45 @@
       <c r="E25" s="2">
         <v>3000</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="2"/>
+      <c r="G25" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="I25" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="19"/>
-      <c r="N25" s="24" t="s">
+      <c r="L25" s="2"/>
+      <c r="M25" s="19"/>
+      <c r="O25" s="24" t="s">
         <v>601</v>
       </c>
-      <c r="O25" s="21" t="s">
+      <c r="P25" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>635</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>639</v>
       </c>
-      <c r="R25" s="2" t="s">
+      <c r="S25" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="S25">
+      <c r="T25">
         <v>3</v>
       </c>
-      <c r="T25" t="s">
+      <c r="U25" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4564,44 +4631,45 @@
       <c r="E26" s="2">
         <v>1000</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="2"/>
+      <c r="G26" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="I26" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K26" s="2"/>
-      <c r="L26" s="19"/>
-      <c r="N26" s="24" t="s">
+      <c r="L26" s="2"/>
+      <c r="M26" s="19"/>
+      <c r="O26" s="24" t="s">
         <v>601</v>
       </c>
-      <c r="O26" s="21" t="s">
+      <c r="P26" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>635</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>624</v>
       </c>
-      <c r="R26" s="2" t="s">
+      <c r="S26" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="S26">
+      <c r="T26">
         <v>3</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4616,44 +4684,45 @@
         <v>142</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="5"/>
+      <c r="G27" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H27" s="28" t="s">
+      <c r="I27" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="2"/>
+      <c r="L27" s="5" t="s">
         <v>648</v>
       </c>
-      <c r="L27" s="19"/>
-      <c r="N27" s="24" t="s">
+      <c r="M27" s="19"/>
+      <c r="O27" s="24" t="s">
         <v>603</v>
       </c>
-      <c r="O27" s="21" t="s">
+      <c r="P27" s="21" t="s">
         <v>615</v>
       </c>
-      <c r="P27" s="5" t="s">
+      <c r="Q27" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>600</v>
       </c>
-      <c r="R27" s="2" t="s">
+      <c r="S27" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <v>4</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4670,43 +4739,44 @@
       <c r="E28" s="5">
         <v>1000</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="5"/>
+      <c r="G28" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="I28" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="2"/>
+      <c r="L28" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L28" s="19"/>
-      <c r="N28" s="24" t="s">
+      <c r="M28" s="19"/>
+      <c r="O28" s="24" t="s">
         <v>602</v>
       </c>
-      <c r="O28" s="21" t="s">
+      <c r="P28" s="21" t="s">
         <v>616</v>
       </c>
-      <c r="P28" s="5" t="s">
+      <c r="Q28" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="R28" s="2" t="s">
+      <c r="S28" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <v>4</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4723,45 +4793,46 @@
       <c r="E29" s="5">
         <v>500</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="5"/>
+      <c r="G29" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="I29" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="J29" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="K29" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="K29" s="18" t="s">
+      <c r="L29" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="L29" s="19"/>
-      <c r="N29" s="25" t="s">
+      <c r="M29" s="19"/>
+      <c r="O29" s="25" t="s">
         <v>604</v>
       </c>
-      <c r="O29" s="21" t="s">
+      <c r="P29" s="21" t="s">
         <v>616</v>
       </c>
-      <c r="P29" s="5" t="s">
+      <c r="Q29" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="S29" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <v>4</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4778,49 +4849,52 @@
       <c r="E30" s="5">
         <v>1000</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="20" t="s">
         <v>507</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="I30" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="2"/>
+      <c r="L30" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L30" s="19"/>
-      <c r="M30" t="s">
+      <c r="M30" s="19"/>
+      <c r="N30" t="s">
         <v>514</v>
       </c>
-      <c r="N30" s="26" t="s">
+      <c r="O30" s="26" t="s">
         <v>664</v>
       </c>
-      <c r="O30" s="22" t="s">
+      <c r="P30" s="22" t="s">
         <v>617</v>
       </c>
-      <c r="P30" s="17" t="s">
+      <c r="Q30" s="17" t="s">
         <v>643</v>
       </c>
-      <c r="Q30" s="17" t="s">
+      <c r="R30" s="17" t="s">
         <v>644</v>
       </c>
-      <c r="R30" s="2" t="s">
+      <c r="S30" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <v>4</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4837,49 +4911,52 @@
       <c r="E31" s="5">
         <v>1000</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="20" t="s">
         <v>507</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="I31" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="2"/>
+      <c r="L31" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="L31" s="19"/>
-      <c r="M31" t="s">
+      <c r="M31" s="19"/>
+      <c r="N31" t="s">
         <v>514</v>
       </c>
-      <c r="N31" s="26" t="s">
+      <c r="O31" s="26" t="s">
         <v>664</v>
       </c>
-      <c r="O31" s="22" t="s">
+      <c r="P31" s="22" t="s">
         <v>617</v>
       </c>
-      <c r="P31" s="17" t="s">
+      <c r="Q31" s="17" t="s">
         <v>643</v>
       </c>
-      <c r="Q31" s="17" t="s">
+      <c r="R31" s="17" t="s">
         <v>645</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="S31" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S31">
+      <c r="T31">
         <v>4</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4896,44 +4973,47 @@
       <c r="E32" s="2">
         <v>2000</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="20" t="s">
         <v>495</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="I32" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="2"/>
+      <c r="L32" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L32" s="19"/>
-      <c r="N32" s="26" t="s">
+      <c r="M32" s="19"/>
+      <c r="O32" s="26" t="s">
         <v>604</v>
       </c>
-      <c r="O32" s="22" t="s">
+      <c r="P32" s="22" t="s">
         <v>618</v>
       </c>
-      <c r="P32" s="5" t="s">
+      <c r="Q32" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="2" t="s">
+      <c r="R32" s="17"/>
+      <c r="S32" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S32">
+      <c r="T32">
         <v>5</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4950,44 +5030,47 @@
       <c r="E33" s="2">
         <v>0</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="20" t="s">
         <v>496</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="I33" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2" t="s">
+      <c r="K33" s="2"/>
+      <c r="L33" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L33" s="19"/>
-      <c r="N33" s="26" t="s">
+      <c r="M33" s="19"/>
+      <c r="O33" s="26" t="s">
         <v>604</v>
       </c>
-      <c r="O33" s="22" t="s">
+      <c r="P33" s="22" t="s">
         <v>619</v>
       </c>
-      <c r="P33" s="5" t="s">
+      <c r="Q33" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="2" t="s">
+      <c r="R33" s="17"/>
+      <c r="S33" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S33">
+      <c r="T33">
         <v>5</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <f t="shared" ref="A34:A51" si="1">ROW() - 1</f>
         <v>33</v>
@@ -5004,44 +5087,47 @@
       <c r="E34" s="2">
         <v>3000</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H34" s="28" t="s">
+      <c r="I34" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="18"/>
-      <c r="N34" s="24" t="s">
+      <c r="L34" s="2"/>
+      <c r="M34" s="18"/>
+      <c r="O34" s="24" t="s">
         <v>656</v>
       </c>
-      <c r="O34" s="22" t="s">
+      <c r="P34" s="22" t="s">
         <v>613</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>634</v>
       </c>
-      <c r="Q34" s="17">
+      <c r="R34" s="17">
         <v>2000</v>
       </c>
-      <c r="R34" s="2" t="s">
+      <c r="S34" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="S34">
+      <c r="T34">
         <v>5</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -5058,44 +5144,47 @@
       <c r="E35" s="2">
         <v>3000</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G35" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H35" s="28" t="s">
+      <c r="I35" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="J35" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="L35" s="18"/>
-      <c r="N35" s="24" t="s">
+      <c r="L35" s="2"/>
+      <c r="M35" s="18"/>
+      <c r="O35" s="24" t="s">
         <v>656</v>
       </c>
-      <c r="O35" s="22" t="s">
+      <c r="P35" s="22" t="s">
         <v>613</v>
       </c>
-      <c r="P35" t="s">
+      <c r="Q35" t="s">
         <v>634</v>
       </c>
-      <c r="Q35" s="17">
+      <c r="R35" s="17">
         <v>3000</v>
       </c>
-      <c r="R35" s="2" t="s">
+      <c r="S35" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="S35">
+      <c r="T35">
         <v>5</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -5110,44 +5199,47 @@
         <v>151</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G36" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="I36" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="J36" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="18"/>
-      <c r="N36" s="24" t="s">
+      <c r="L36" s="2"/>
+      <c r="M36" s="18"/>
+      <c r="O36" s="24" t="s">
         <v>656</v>
       </c>
-      <c r="O36" s="22" t="s">
+      <c r="P36" s="22" t="s">
         <v>613</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>634</v>
       </c>
-      <c r="Q36" s="17">
+      <c r="R36" s="17">
         <v>3000</v>
       </c>
-      <c r="R36" s="2" t="s">
+      <c r="S36" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="S36">
+      <c r="T36">
         <v>5</v>
       </c>
-      <c r="T36" t="s">
+      <c r="U36" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -5164,44 +5256,47 @@
       <c r="E37" s="2">
         <v>3000</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H37" s="28" t="s">
+      <c r="I37" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="J37" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="18"/>
-      <c r="N37" s="24" t="s">
+      <c r="L37" s="2"/>
+      <c r="M37" s="18"/>
+      <c r="O37" s="24" t="s">
         <v>656</v>
       </c>
-      <c r="O37" s="22" t="s">
+      <c r="P37" s="22" t="s">
         <v>613</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>646</v>
       </c>
-      <c r="Q37" s="17">
+      <c r="R37" s="17">
         <v>3000</v>
       </c>
-      <c r="R37" s="2" t="s">
+      <c r="S37" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="S37">
+      <c r="T37">
         <v>5</v>
       </c>
-      <c r="T37" t="s">
+      <c r="U37" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -5218,41 +5313,44 @@
       <c r="E38" s="2">
         <v>2000</v>
       </c>
-      <c r="F38" s="28" t="s">
+      <c r="F38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="28" t="s">
         <v>556</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="I38" s="20" t="s">
         <v>592</v>
       </c>
-      <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="N38" s="24" t="s">
+      <c r="L38" s="2"/>
+      <c r="O38" s="24" t="s">
         <v>606</v>
       </c>
-      <c r="O38" s="22" t="s">
+      <c r="P38" s="22" t="s">
         <v>617</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>635</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>647</v>
       </c>
-      <c r="R38" s="2" t="s">
+      <c r="S38" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="S38">
+      <c r="T38">
         <v>5</v>
       </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -5269,41 +5367,44 @@
       <c r="E39" s="2">
         <v>2000</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="F39" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G39" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="I39" s="20" t="s">
         <v>593</v>
       </c>
-      <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="N39" s="24" t="s">
+      <c r="L39" s="2"/>
+      <c r="O39" s="24" t="s">
         <v>607</v>
       </c>
-      <c r="O39" s="22" t="s">
+      <c r="P39" s="22" t="s">
         <v>620</v>
       </c>
-      <c r="P39" t="s">
+      <c r="Q39" t="s">
         <v>635</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="R39" t="s">
         <v>647</v>
       </c>
-      <c r="R39" s="2" t="s">
+      <c r="S39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="S39">
+      <c r="T39">
         <v>5</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -5318,41 +5419,42 @@
         <v>145</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="5"/>
+      <c r="G40" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H40" s="28" t="s">
+      <c r="I40" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="N40" s="24" t="s">
+      <c r="L40" s="2"/>
+      <c r="O40" s="24" t="s">
         <v>608</v>
       </c>
-      <c r="O40" s="22" t="s">
+      <c r="P40" s="22" t="s">
         <v>621</v>
       </c>
-      <c r="P40" s="5" t="s">
+      <c r="Q40" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="Q40" s="17">
+      <c r="R40" s="17">
         <v>400</v>
       </c>
-      <c r="R40" s="2" t="s">
+      <c r="S40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S40">
+      <c r="T40">
         <v>6</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -5367,41 +5469,42 @@
         <v>145</v>
       </c>
       <c r="E41" s="5"/>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="5"/>
+      <c r="G41" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H41" s="28" t="s">
+      <c r="I41" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="N41" s="24" t="s">
+      <c r="L41" s="2"/>
+      <c r="O41" s="24" t="s">
         <v>609</v>
       </c>
-      <c r="O41" s="22" t="s">
+      <c r="P41" s="22" t="s">
         <v>621</v>
       </c>
-      <c r="P41" s="5" t="s">
+      <c r="Q41" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="Q41" s="17">
+      <c r="R41" s="17">
         <v>500</v>
       </c>
-      <c r="R41" s="2" t="s">
+      <c r="S41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S41">
+      <c r="T41">
         <v>6</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -5416,41 +5519,42 @@
         <v>145</v>
       </c>
       <c r="E42" s="5"/>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="5"/>
+      <c r="G42" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H42" s="28" t="s">
+      <c r="I42" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="N42" s="24" t="s">
+      <c r="L42" s="2"/>
+      <c r="O42" s="24" t="s">
         <v>610</v>
       </c>
-      <c r="O42" s="22" t="s">
+      <c r="P42" s="22" t="s">
         <v>621</v>
       </c>
-      <c r="P42" s="5" t="s">
+      <c r="Q42" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="Q42" s="17">
+      <c r="R42" s="17">
         <v>600</v>
       </c>
-      <c r="R42" s="2" t="s">
+      <c r="S42" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S42">
+      <c r="T42">
         <v>6</v>
       </c>
-      <c r="T42" t="s">
+      <c r="U42" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -5467,43 +5571,46 @@
       <c r="E43" s="2">
         <v>2000</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G43" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H43" s="20" t="s">
+      <c r="I43" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="J43" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="N43" s="24" t="s">
+      <c r="L43" s="2"/>
+      <c r="O43" s="24" t="s">
         <v>659</v>
       </c>
-      <c r="O43" s="22" t="s">
+      <c r="P43" s="22" t="s">
         <v>622</v>
       </c>
-      <c r="P43" s="17" t="s">
+      <c r="Q43" s="17" t="s">
         <v>650</v>
       </c>
-      <c r="Q43" s="17" t="s">
+      <c r="R43" s="17" t="s">
         <v>651</v>
       </c>
-      <c r="R43" s="2" t="s">
+      <c r="S43" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="S43">
+      <c r="T43">
         <v>6</v>
       </c>
-      <c r="T43" t="s">
+      <c r="U43" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -5520,45 +5627,48 @@
       <c r="E44" s="2">
         <v>2000</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G44" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H44" s="28" t="s">
+      <c r="I44" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="J44" s="2"/>
-      <c r="K44" s="5" t="s">
+      <c r="K44" s="2"/>
+      <c r="L44" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="N44" s="24" t="s">
+      <c r="O44" s="24" t="s">
         <v>660</v>
       </c>
-      <c r="O44" s="22" t="s">
+      <c r="P44" s="22" t="s">
         <v>622</v>
       </c>
-      <c r="P44" s="17" t="s">
+      <c r="Q44" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="Q44" s="17" t="s">
+      <c r="R44" s="17" t="s">
         <v>653</v>
       </c>
-      <c r="R44" s="2" t="s">
+      <c r="S44" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <v>6</v>
       </c>
-      <c r="T44" t="s">
+      <c r="U44" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -5575,45 +5685,48 @@
       <c r="E45" s="2">
         <v>2000</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="F45" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G45" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H45" s="28" t="s">
+      <c r="I45" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="J45" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="J45" s="2"/>
-      <c r="K45" s="5" t="s">
+      <c r="K45" s="2"/>
+      <c r="L45" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="N45" s="24" t="s">
+      <c r="O45" s="24" t="s">
         <v>660</v>
       </c>
-      <c r="O45" s="22" t="s">
+      <c r="P45" s="22" t="s">
         <v>622</v>
       </c>
-      <c r="P45" s="17" t="s">
+      <c r="Q45" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="Q45" s="17" t="s">
+      <c r="R45" s="17" t="s">
         <v>654</v>
       </c>
-      <c r="R45" s="2" t="s">
+      <c r="S45" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="S45">
+      <c r="T45">
         <v>6</v>
       </c>
-      <c r="T45" t="s">
+      <c r="U45" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -5630,43 +5743,46 @@
       <c r="E46" s="2">
         <v>2000</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G46" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="H46" s="20" t="s">
+      <c r="I46" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="J46" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="N46" s="24" t="s">
+      <c r="L46" s="2"/>
+      <c r="O46" s="24" t="s">
         <v>659</v>
       </c>
-      <c r="O46" s="22" t="s">
+      <c r="P46" s="22" t="s">
         <v>622</v>
       </c>
-      <c r="P46" s="17" t="s">
+      <c r="Q46" s="17" t="s">
         <v>650</v>
       </c>
-      <c r="Q46" s="17" t="s">
+      <c r="R46" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="R46" s="2" t="s">
+      <c r="S46" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="S46">
+      <c r="T46">
         <v>6</v>
       </c>
-      <c r="T46" t="s">
+      <c r="U46" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -5681,17 +5797,18 @@
         <v>155</v>
       </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="2" t="s">
+      <c r="F47" s="2"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H47" s="20"/>
-      <c r="I47" s="2"/>
+      <c r="I47" s="20"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="R47" s="2"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="L47" s="2"/>
+      <c r="S47" s="2"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -5706,17 +5823,18 @@
         <v>155</v>
       </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="2" t="s">
+      <c r="F48" s="2"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H48" s="20"/>
-      <c r="I48" s="2"/>
+      <c r="I48" s="20"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="R48" s="2"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="L48" s="2"/>
+      <c r="S48" s="2"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -5731,23 +5849,24 @@
         <v>156</v>
       </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="20" t="s">
+      <c r="F49" s="2"/>
+      <c r="G49" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H49" s="20" t="s">
+      <c r="I49" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="R49" s="2" t="s">
+      <c r="L49" s="2"/>
+      <c r="S49" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -5762,15 +5881,16 @@
         <v>158</v>
       </c>
       <c r="E50" s="2"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="20"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="R50" s="2"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="L50" s="2"/>
+      <c r="S50" s="2"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -5785,17 +5905,18 @@
         <v>159</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="20"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="R51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="S51" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:V51">
-    <sortCondition ref="S2:S51"/>
+  <sortState ref="A2:W51">
+    <sortCondition ref="T2:T51"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}" topLeftCell="A11">

</xml_diff>